<commit_message>
[IMP] Moved to data/cifar - staring standard dogs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924FB54-FB34-0C42-8DAB-EC3CE96B2C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF4D125-3994-184C-B7CA-3DB5BCE93D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="760" windowWidth="14080" windowHeight="18360" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="1180" yWindow="760" windowWidth="28220" windowHeight="18360" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="232">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -361,15 +361,9 @@
     <t>3--13</t>
   </si>
   <si>
-    <t>35_2</t>
-  </si>
-  <si>
     <t>both (not early stop)</t>
   </si>
   <si>
-    <t>36_2</t>
-  </si>
-  <si>
     <t>34.98% vs 34.94%</t>
   </si>
   <si>
@@ -424,20 +418,321 @@
     <t>Brainit</t>
   </si>
   <si>
-    <t>Foveation</t>
-  </si>
-  <si>
     <t>batch 0</t>
   </si>
   <si>
-    <t>Foveation Longer</t>
+    <t>Seed Tests</t>
+  </si>
+  <si>
+    <t>ZoomVit</t>
+  </si>
+  <si>
+    <t>Scheduler patience moved from 3 to 8</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>Moved blur to init longer foveation</t>
+  </si>
+  <si>
+    <t>r1.1</t>
+  </si>
+  <si>
+    <t>r1.2</t>
+  </si>
+  <si>
+    <t>r1.3</t>
+  </si>
+  <si>
+    <t>r1.4</t>
+  </si>
+  <si>
+    <t>r1.5</t>
+  </si>
+  <si>
+    <t>r1.6</t>
+  </si>
+  <si>
+    <t>r1.7</t>
+  </si>
+  <si>
+    <t>r1.27</t>
+  </si>
+  <si>
+    <t>r1.21</t>
+  </si>
+  <si>
+    <t>r1.22</t>
+  </si>
+  <si>
+    <t>r1.23</t>
+  </si>
+  <si>
+    <t>r1.31</t>
+  </si>
+  <si>
+    <t>r1.32</t>
+  </si>
+  <si>
+    <t>r1.39</t>
+  </si>
+  <si>
+    <t>r1.40</t>
+  </si>
+  <si>
+    <t>r1.41</t>
+  </si>
+  <si>
+    <t>r1.42</t>
+  </si>
+  <si>
+    <t>r1.47</t>
+  </si>
+  <si>
+    <t>r1.48</t>
+  </si>
+  <si>
+    <t>r1.49</t>
+  </si>
+  <si>
+    <t>r1.50</t>
+  </si>
+  <si>
+    <t>r1.54</t>
+  </si>
+  <si>
+    <t>r1.55</t>
+  </si>
+  <si>
+    <t>r1.56</t>
+  </si>
+  <si>
+    <t>r1.8</t>
+  </si>
+  <si>
+    <t>r1.28</t>
+  </si>
+  <si>
+    <t>r1.9</t>
+  </si>
+  <si>
+    <t>r1.10</t>
+  </si>
+  <si>
+    <t>r1.11</t>
+  </si>
+  <si>
+    <t>r1.12</t>
+  </si>
+  <si>
+    <t>r1.13</t>
+  </si>
+  <si>
+    <t>r1.14</t>
+  </si>
+  <si>
+    <t>r1.15</t>
+  </si>
+  <si>
+    <t>r1.16</t>
+  </si>
+  <si>
+    <t>r1.17</t>
+  </si>
+  <si>
+    <t>r1.18</t>
+  </si>
+  <si>
+    <t>r1.19</t>
+  </si>
+  <si>
+    <t>r1.20</t>
+  </si>
+  <si>
+    <t>r1.29</t>
+  </si>
+  <si>
+    <t>r1.30</t>
+  </si>
+  <si>
+    <t>r1.35</t>
+  </si>
+  <si>
+    <t>r1.36</t>
+  </si>
+  <si>
+    <t>r1.57</t>
+  </si>
+  <si>
+    <t>r1.58</t>
+  </si>
+  <si>
+    <t>r1.24</t>
+  </si>
+  <si>
+    <t>r1.25</t>
+  </si>
+  <si>
+    <t>r1.26</t>
+  </si>
+  <si>
+    <t>r1.33</t>
+  </si>
+  <si>
+    <t>r1.34</t>
+  </si>
+  <si>
+    <t>r1.35_2</t>
+  </si>
+  <si>
+    <t>r1.36_2</t>
+  </si>
+  <si>
+    <t>r1.37</t>
+  </si>
+  <si>
+    <t>r1.38</t>
+  </si>
+  <si>
+    <t>r1.43</t>
+  </si>
+  <si>
+    <t>r1.44</t>
+  </si>
+  <si>
+    <t>r1.45</t>
+  </si>
+  <si>
+    <t>r1.46</t>
+  </si>
+  <si>
+    <t>r1.51</t>
+  </si>
+  <si>
+    <t>r1.52</t>
+  </si>
+  <si>
+    <t>r1.53</t>
+  </si>
+  <si>
+    <t>r1.59</t>
+  </si>
+  <si>
+    <t>r1.60</t>
+  </si>
+  <si>
+    <t>r1.61</t>
+  </si>
+  <si>
+    <t>r1.62</t>
+  </si>
+  <si>
+    <t>r0.1</t>
+  </si>
+  <si>
+    <t>r0.2</t>
+  </si>
+  <si>
+    <t>r0.3</t>
+  </si>
+  <si>
+    <t>r0.4</t>
+  </si>
+  <si>
+    <t>r2.1</t>
+  </si>
+  <si>
+    <t>r2.1v2</t>
+  </si>
+  <si>
+    <t>r2.1v3</t>
+  </si>
+  <si>
+    <t>r2.2</t>
+  </si>
+  <si>
+    <t>r2.3</t>
+  </si>
+  <si>
+    <t>r2.4</t>
+  </si>
+  <si>
+    <t>m1_normal Moved blur to init</t>
+  </si>
+  <si>
+    <t>61/71</t>
+  </si>
+  <si>
+    <t>r.2.5</t>
+  </si>
+  <si>
+    <t>FixedFoveation - weird seeding</t>
+  </si>
+  <si>
+    <t>FixedFoveation - proper seeding</t>
+  </si>
+  <si>
+    <t>FixedFoveation</t>
+  </si>
+  <si>
+    <t>70/80</t>
+  </si>
+  <si>
+    <t>88/98</t>
+  </si>
+  <si>
+    <t>Took really long to converge!</t>
+  </si>
+  <si>
+    <t>r.2.6</t>
+  </si>
+  <si>
+    <t>LearnableFoveation</t>
+  </si>
+  <si>
+    <t>r.2.7</t>
+  </si>
+  <si>
+    <t>find in r.2.6</t>
+  </si>
+  <si>
+    <t>r2.6</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>r.2.8</t>
+  </si>
+  <si>
+    <t>50% of training data, bz 256</t>
+  </si>
+  <si>
+    <t>10% of training data, bz 256</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switched to cosine scheduler with 50 T-max </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>FROM HERE ON!</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -572,8 +867,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -825,8 +1144,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -963,7 +1288,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1169,6 +1496,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1241,13 +1579,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1256,7 +1594,85 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1304,7 +1720,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1315,6 +1731,12 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1363,7 +1785,10 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1372,68 +1797,124 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="44" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="45" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="45" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1481,42 +1962,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1534,19 +1980,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1875,112 +2319,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
-  <dimension ref="B1:N72"/>
+  <dimension ref="B1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
-    <col min="10" max="10" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="45"/>
+    <col min="2" max="2" width="16.5" style="45" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="45"/>
+    <col min="5" max="5" width="27.83203125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="17" style="46" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="45"/>
+    <col min="9" max="9" width="17.5" style="45" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" style="45" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="M1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="25"/>
+      <c r="M1" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="47"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E2" t="s">
+      <c r="E2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="27"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M3" t="s">
+      <c r="M3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="29"/>
-    </row>
-    <row r="4" spans="2:14" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="N3" s="49"/>
+    </row>
+    <row r="4" spans="2:14" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="31"/>
-    </row>
-    <row r="5" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="N4" s="50"/>
+    </row>
+    <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="8">
         <v>0.75439999999999996</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="7">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="33"/>
-    </row>
-    <row r="6" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="N5" s="51"/>
+    </row>
+    <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="2">
         <v>0.83630000000000004</v>
       </c>
@@ -1993,138 +2447,144 @@
       <c r="I6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="47"/>
-    </row>
-    <row r="7" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="s">
+      <c r="N6" s="52"/>
+    </row>
+    <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="14">
         <v>0.77610000000000001</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="13">
         <v>19</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="35"/>
-    </row>
-    <row r="8" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="17" t="s">
+      <c r="N7" s="53"/>
+    </row>
+    <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="14">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="8">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="7">
         <v>19</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="37"/>
-    </row>
-    <row r="9" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="16">
-        <v>4</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11" t="s">
+      <c r="N8" s="54"/>
+    </row>
+    <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="14">
         <v>0.74109999999999998</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="13">
         <v>26</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="39"/>
-    </row>
-    <row r="10" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+      <c r="N9" s="55"/>
+    </row>
+    <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="14">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="8">
         <v>0.92279999999999995</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="7">
         <v>29</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="M10" t="s">
+      <c r="J10" s="9"/>
+      <c r="M10" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="N10" s="42"/>
-    </row>
-    <row r="11" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="18"/>
-      <c r="C11" s="15">
-        <v>6</v>
+      <c r="N10" s="56"/>
+    </row>
+    <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
@@ -2144,12 +2604,12 @@
       <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="18"/>
-      <c r="C12" s="15">
-        <v>7</v>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="20"/>
+      <c r="C12" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
@@ -2169,14 +2629,14 @@
       <c r="I12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="18"/>
-      <c r="C13" s="26">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="41" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2194,12 +2654,12 @@
       <c r="I13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="18"/>
-      <c r="C14" s="30">
-        <v>21</v>
+      <c r="B14" s="20"/>
+      <c r="C14" s="31" t="s">
+        <v>146</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>36</v>
@@ -2219,14 +2679,14 @@
       <c r="I14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="18"/>
-      <c r="C15" s="30">
-        <v>22</v>
+      <c r="B15" s="20"/>
+      <c r="C15" s="31" t="s">
+        <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
@@ -2246,12 +2706,12 @@
       <c r="I15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="18"/>
-      <c r="C16" s="30">
-        <v>23</v>
+      <c r="B16" s="20"/>
+      <c r="C16" s="31" t="s">
+        <v>148</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>36</v>
@@ -2271,12 +2731,12 @@
       <c r="I16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="30">
-        <v>31</v>
+      <c r="B17" s="20"/>
+      <c r="C17" s="31" t="s">
+        <v>149</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>36</v>
@@ -2296,12 +2756,12 @@
       <c r="I17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="18"/>
-      <c r="C18" s="30">
-        <v>32</v>
+      <c r="B18" s="20"/>
+      <c r="C18" s="31" t="s">
+        <v>150</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>36</v>
@@ -2321,12 +2781,12 @@
       <c r="I18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="9"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="18"/>
-      <c r="C19" s="34">
-        <v>39</v>
+      <c r="B19" s="20"/>
+      <c r="C19" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>47</v>
@@ -2346,12 +2806,12 @@
       <c r="I19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="18"/>
-      <c r="C20" s="34">
-        <v>40</v>
+      <c r="B20" s="20"/>
+      <c r="C20" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>47</v>
@@ -2371,12 +2831,12 @@
       <c r="I20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="18"/>
-      <c r="C21" s="34">
-        <v>41</v>
+      <c r="B21" s="20"/>
+      <c r="C21" s="33" t="s">
+        <v>153</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>47</v>
@@ -2396,12 +2856,12 @@
       <c r="I21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="18"/>
-      <c r="C22" s="34">
-        <v>42</v>
+      <c r="B22" s="20"/>
+      <c r="C22" s="33" t="s">
+        <v>154</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>47</v>
@@ -2421,12 +2881,12 @@
       <c r="I22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="18"/>
-      <c r="C23" s="36">
-        <v>47</v>
+      <c r="B23" s="20"/>
+      <c r="C23" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>47</v>
@@ -2446,12 +2906,12 @@
       <c r="I23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B24" s="18"/>
-      <c r="C24" s="36">
-        <v>48</v>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="20"/>
+      <c r="C24" s="34" t="s">
+        <v>156</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>47</v>
@@ -2459,7 +2919,7 @@
       <c r="E24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -2471,12 +2931,12 @@
       <c r="I24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B25" s="18"/>
-      <c r="C25" s="36">
-        <v>49</v>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="20"/>
+      <c r="C25" s="34" t="s">
+        <v>157</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>47</v>
@@ -2484,7 +2944,7 @@
       <c r="E25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -2496,12 +2956,12 @@
       <c r="I25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B26" s="18"/>
-      <c r="C26" s="36">
-        <v>50</v>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="20"/>
+      <c r="C26" s="34" t="s">
+        <v>158</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
@@ -2509,7 +2969,7 @@
       <c r="E26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -2521,12 +2981,12 @@
       <c r="I26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B27" s="18"/>
-      <c r="C27" s="38">
-        <v>54</v>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="20"/>
+      <c r="C27" s="35" t="s">
+        <v>159</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>47</v>
@@ -2534,7 +2994,7 @@
       <c r="E27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -2546,12 +3006,12 @@
       <c r="I27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B28" s="18"/>
-      <c r="C28" s="38">
-        <v>55</v>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="20"/>
+      <c r="C28" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>47</v>
@@ -2559,7 +3019,7 @@
       <c r="E28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2571,12 +3031,12 @@
       <c r="I28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B29" s="18"/>
-      <c r="C29" s="38">
-        <v>56</v>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="20"/>
+      <c r="C29" s="35" t="s">
+        <v>161</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
@@ -2584,7 +3044,7 @@
       <c r="E29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -2596,52 +3056,66 @@
       <c r="I29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="13"/>
-    </row>
-    <row r="31" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="17" t="s">
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="21"/>
+      <c r="C30" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="14">
+        <v>0.85589999999999999</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="24">
-        <v>8</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="8">
         <v>0.91569999999999996</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="7">
         <v>30</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="18"/>
-      <c r="C32" s="26">
-        <v>28</v>
+    <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="20"/>
+      <c r="C32" s="29" t="s">
+        <v>163</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>30</v>
@@ -2661,12 +3135,12 @@
       <c r="I32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B33" s="18"/>
-      <c r="C33" s="23">
-        <v>9</v>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="20"/>
+      <c r="C33" s="27" t="s">
+        <v>164</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>30</v>
@@ -2686,12 +3160,12 @@
       <c r="I33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B34" s="18"/>
-      <c r="C34" s="23">
-        <v>10</v>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="20"/>
+      <c r="C34" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>30</v>
@@ -2711,12 +3185,12 @@
       <c r="I34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J34" s="9"/>
-    </row>
-    <row r="35" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B35" s="18"/>
-      <c r="C35" s="23">
-        <v>11</v>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="20"/>
+      <c r="C35" s="27" t="s">
+        <v>166</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>30</v>
@@ -2736,12 +3210,12 @@
       <c r="I35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B36" s="18"/>
-      <c r="C36" s="23">
-        <v>12</v>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="20"/>
+      <c r="C36" s="27" t="s">
+        <v>167</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>30</v>
@@ -2761,12 +3235,12 @@
       <c r="I36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J36" s="9"/>
-    </row>
-    <row r="37" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B37" s="18"/>
-      <c r="C37" s="23">
-        <v>13</v>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="20"/>
+      <c r="C37" s="27" t="s">
+        <v>168</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>30</v>
@@ -2786,14 +3260,14 @@
       <c r="I37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="J37" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B38" s="18"/>
-      <c r="C38" s="23">
-        <v>14</v>
+    <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="20"/>
+      <c r="C38" s="27" t="s">
+        <v>169</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>30</v>
@@ -2813,14 +3287,14 @@
       <c r="I38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J38" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="18"/>
-      <c r="C39" s="26">
-        <v>15</v>
+    <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="20"/>
+      <c r="C39" s="29" t="s">
+        <v>170</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
@@ -2840,12 +3314,12 @@
       <c r="I39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B40" s="18"/>
-      <c r="C40" s="26">
-        <v>16</v>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="20"/>
+      <c r="C40" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
@@ -2865,14 +3339,14 @@
       <c r="I40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B41" s="18"/>
-      <c r="C41" s="26">
-        <v>17</v>
+    <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="20"/>
+      <c r="C41" s="29" t="s">
+        <v>172</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>30</v>
@@ -2892,12 +3366,12 @@
       <c r="I41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J41" s="9"/>
-    </row>
-    <row r="42" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B42" s="18"/>
-      <c r="C42" s="26">
-        <v>18</v>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="20"/>
+      <c r="C42" s="29" t="s">
+        <v>173</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
@@ -2917,12 +3391,12 @@
       <c r="I42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="9"/>
-    </row>
-    <row r="43" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B43" s="18"/>
-      <c r="C43" s="28">
-        <v>19</v>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="20"/>
+      <c r="C43" s="30" t="s">
+        <v>174</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>30</v>
@@ -2942,12 +3416,12 @@
       <c r="I43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B44" s="18"/>
-      <c r="C44" s="28">
-        <v>20</v>
+      <c r="J43" s="11"/>
+    </row>
+    <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="20"/>
+      <c r="C44" s="30" t="s">
+        <v>175</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>30</v>
@@ -2967,12 +3441,12 @@
       <c r="I44" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B45" s="18"/>
-      <c r="C45" s="28">
-        <v>29</v>
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="20"/>
+      <c r="C45" s="30" t="s">
+        <v>176</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>30</v>
@@ -2992,12 +3466,12 @@
       <c r="I45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J45" s="9"/>
-    </row>
-    <row r="46" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B46" s="18"/>
-      <c r="C46" s="28">
-        <v>30</v>
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="20"/>
+      <c r="C46" s="30" t="s">
+        <v>177</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>30</v>
@@ -3017,12 +3491,12 @@
       <c r="I46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J46" s="9"/>
+      <c r="J46" s="11"/>
     </row>
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="18"/>
-      <c r="C47" s="43">
-        <v>35</v>
+      <c r="B47" s="20"/>
+      <c r="C47" s="43" t="s">
+        <v>178</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>30</v>
@@ -3042,14 +3516,14 @@
       <c r="I47" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="J47" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B48" s="18"/>
-      <c r="C48" s="43">
-        <v>36</v>
+      <c r="B48" s="20"/>
+      <c r="C48" s="43" t="s">
+        <v>179</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>30</v>
@@ -3069,12 +3543,12 @@
       <c r="I48" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J48" s="9"/>
-    </row>
-    <row r="49" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B49" s="18"/>
-      <c r="C49" s="43">
-        <v>57</v>
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="20"/>
+      <c r="C49" s="37" t="s">
+        <v>180</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>30</v>
@@ -3092,12 +3566,12 @@
         <v>34</v>
       </c>
       <c r="I49" s="1"/>
-      <c r="J49" s="9"/>
+      <c r="J49" s="11"/>
     </row>
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="18"/>
-      <c r="C50" s="43">
-        <v>58</v>
+      <c r="B50" s="20"/>
+      <c r="C50" s="37" t="s">
+        <v>181</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>30</v>
@@ -3113,14 +3587,14 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="9" t="s">
+      <c r="J50" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="18"/>
-      <c r="C51" s="32">
-        <v>24</v>
+      <c r="B51" s="20"/>
+      <c r="C51" s="32" t="s">
+        <v>182</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>36</v>
@@ -3140,14 +3614,14 @@
       <c r="I51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J51" s="44" t="s">
+      <c r="J51" s="38" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="18"/>
-      <c r="C52" s="32">
-        <v>25</v>
+      <c r="B52" s="20"/>
+      <c r="C52" s="32" t="s">
+        <v>183</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>36</v>
@@ -3167,12 +3641,12 @@
       <c r="I52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="45"/>
+      <c r="J52" s="39"/>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="18"/>
-      <c r="C53" s="32">
-        <v>26</v>
+      <c r="B53" s="20"/>
+      <c r="C53" s="32" t="s">
+        <v>184</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>36</v>
@@ -3192,12 +3666,12 @@
       <c r="I53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="45"/>
+      <c r="J53" s="39"/>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="18"/>
-      <c r="C54" s="32">
-        <v>33</v>
+      <c r="B54" s="20"/>
+      <c r="C54" s="32" t="s">
+        <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>36</v>
@@ -3217,12 +3691,12 @@
       <c r="I54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J54" s="45"/>
+      <c r="J54" s="39"/>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="18"/>
-      <c r="C55" s="32">
-        <v>34</v>
+      <c r="B55" s="20"/>
+      <c r="C55" s="32" t="s">
+        <v>186</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>36</v>
@@ -3242,12 +3716,12 @@
       <c r="I55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J55" s="45"/>
-    </row>
-    <row r="56" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B56" s="18"/>
-      <c r="C56" s="34" t="s">
-        <v>113</v>
+      <c r="J55" s="39"/>
+    </row>
+    <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B56" s="20"/>
+      <c r="C56" s="33" t="s">
+        <v>187</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>47</v>
@@ -3265,14 +3739,14 @@
         <v>34</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J56" s="45"/>
-    </row>
-    <row r="57" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B57" s="18"/>
-      <c r="C57" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="J56" s="39"/>
+    </row>
+    <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B57" s="20"/>
+      <c r="C57" s="33" t="s">
+        <v>188</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>47</v>
@@ -3290,14 +3764,14 @@
         <v>34</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J57" s="45"/>
-    </row>
-    <row r="58" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B58" s="18"/>
-      <c r="C58" s="34">
-        <v>37</v>
+        <v>113</v>
+      </c>
+      <c r="J57" s="39"/>
+    </row>
+    <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B58" s="20"/>
+      <c r="C58" s="33" t="s">
+        <v>189</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>47</v>
@@ -3315,14 +3789,14 @@
         <v>34</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J58" s="45"/>
-    </row>
-    <row r="59" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B59" s="18"/>
-      <c r="C59" s="34">
-        <v>38</v>
+        <v>113</v>
+      </c>
+      <c r="J58" s="39"/>
+    </row>
+    <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B59" s="20"/>
+      <c r="C59" s="33" t="s">
+        <v>190</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>47</v>
@@ -3340,14 +3814,14 @@
         <v>34</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J59" s="45"/>
-    </row>
-    <row r="60" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B60" s="18"/>
-      <c r="C60" s="36">
-        <v>43</v>
+        <v>113</v>
+      </c>
+      <c r="J59" s="39"/>
+    </row>
+    <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" s="20"/>
+      <c r="C60" s="34" t="s">
+        <v>191</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>47</v>
@@ -3355,24 +3829,24 @@
       <c r="E60" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>116</v>
+      <c r="F60" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J60" s="45"/>
-    </row>
-    <row r="61" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B61" s="18"/>
-      <c r="C61" s="36">
-        <v>44</v>
+        <v>113</v>
+      </c>
+      <c r="J60" s="39"/>
+    </row>
+    <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B61" s="20"/>
+      <c r="C61" s="34" t="s">
+        <v>192</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>47</v>
@@ -3380,24 +3854,24 @@
       <c r="E61" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>118</v>
+      <c r="F61" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J61" s="45"/>
-    </row>
-    <row r="62" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B62" s="18"/>
-      <c r="C62" s="36">
-        <v>45</v>
+        <v>113</v>
+      </c>
+      <c r="J61" s="39"/>
+    </row>
+    <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B62" s="20"/>
+      <c r="C62" s="34" t="s">
+        <v>193</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>47</v>
@@ -3405,24 +3879,24 @@
       <c r="E62" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>120</v>
+      <c r="F62" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J62" s="45"/>
-    </row>
-    <row r="63" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B63" s="18"/>
-      <c r="C63" s="36">
-        <v>46</v>
+        <v>113</v>
+      </c>
+      <c r="J62" s="39"/>
+    </row>
+    <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B63" s="20"/>
+      <c r="C63" s="34" t="s">
+        <v>194</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>47</v>
@@ -3430,24 +3904,24 @@
       <c r="E63" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>121</v>
+      <c r="F63" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J63" s="45"/>
-    </row>
-    <row r="64" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B64" s="18"/>
-      <c r="C64" s="38">
-        <v>51</v>
+        <v>113</v>
+      </c>
+      <c r="J63" s="39"/>
+    </row>
+    <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B64" s="20"/>
+      <c r="C64" s="35" t="s">
+        <v>195</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>47</v>
@@ -3455,24 +3929,24 @@
       <c r="E64" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>122</v>
+      <c r="F64" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J64" s="45"/>
-    </row>
-    <row r="65" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B65" s="18"/>
-      <c r="C65" s="38">
-        <v>52</v>
+        <v>113</v>
+      </c>
+      <c r="J64" s="39"/>
+    </row>
+    <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B65" s="20"/>
+      <c r="C65" s="35" t="s">
+        <v>196</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>47</v>
@@ -3480,24 +3954,24 @@
       <c r="E65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>124</v>
+      <c r="F65" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J65" s="45"/>
-    </row>
-    <row r="66" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B66" s="18"/>
-      <c r="C66" s="38">
-        <v>53</v>
+        <v>113</v>
+      </c>
+      <c r="J65" s="39"/>
+    </row>
+    <row r="66" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="20"/>
+      <c r="C66" s="35" t="s">
+        <v>197</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>47</v>
@@ -3505,36 +3979,36 @@
       <c r="E66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>126</v>
+      <c r="F66" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J66" s="45"/>
-    </row>
-    <row r="67" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B67" s="18"/>
-      <c r="C67" s="40">
-        <v>59</v>
+        <v>113</v>
+      </c>
+      <c r="J66" s="39"/>
+    </row>
+    <row r="67" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="20"/>
+      <c r="C67" s="36" t="s">
+        <v>198</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F67" s="2">
         <v>0.92459999999999998</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>34</v>
@@ -3542,18 +4016,18 @@
       <c r="I67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="45"/>
-    </row>
-    <row r="68" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B68" s="18"/>
-      <c r="C68" s="40">
-        <v>60</v>
+      <c r="J67" s="39"/>
+    </row>
+    <row r="68" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="20"/>
+      <c r="C68" s="36" t="s">
+        <v>199</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F68" s="2">
         <v>0.91800000000000004</v>
@@ -3567,18 +4041,18 @@
       <c r="I68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J68" s="45"/>
-    </row>
-    <row r="69" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B69" s="18"/>
-      <c r="C69" s="40">
-        <v>61</v>
+      <c r="J68" s="39"/>
+    </row>
+    <row r="69" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="20"/>
+      <c r="C69" s="36" t="s">
+        <v>200</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F69" s="2">
         <v>0.92310000000000003</v>
@@ -3590,96 +4064,567 @@
         <v>34</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J69" s="45"/>
-    </row>
-    <row r="70" spans="2:10" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="19"/>
-      <c r="C70" s="41">
-        <v>62</v>
-      </c>
-      <c r="D70" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J69" s="39"/>
+    </row>
+    <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="21"/>
+      <c r="C70" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F70" s="12">
+      <c r="E70" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F70" s="23">
         <v>0.90859999999999996</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G70" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H70" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I70" s="11" t="s">
+      <c r="H70" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J70" s="46"/>
-    </row>
-    <row r="71" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B71" s="3" t="s">
+      <c r="J70" s="39"/>
+    </row>
+    <row r="71" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="3">
-        <v>1</v>
-      </c>
-      <c r="D71" s="3" t="s">
+      <c r="C71" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F71" s="8">
+        <v>0.92759999999999998</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="9"/>
+    </row>
+    <row r="72" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="60"/>
+      <c r="C72" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0.92759999999999998</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="11"/>
+    </row>
+    <row r="73" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="60"/>
+      <c r="C73" s="64" t="s">
+        <v>204</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F73" s="2"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="11"/>
+    </row>
+    <row r="74" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="61"/>
+      <c r="C74" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F74" s="14"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="15"/>
+    </row>
+    <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B75" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F71" s="48">
+      <c r="E75" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F75" s="40">
         <v>0.84760000000000002</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G75" s="5">
         <v>50</v>
       </c>
-      <c r="H71" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J71" s="3"/>
-    </row>
-    <row r="72" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="C72" s="50">
-        <v>2</v>
-      </c>
-      <c r="D72" s="49" t="s">
+      <c r="H75" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B76" s="20"/>
+      <c r="C76" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E72" s="49" t="s">
+      <c r="E76" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F76" s="2">
+        <v>0.80649999999999999</v>
+      </c>
+      <c r="G76" s="1">
+        <v>50</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B77" s="20"/>
+      <c r="C77" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0.84240000000000004</v>
+      </c>
+      <c r="G77" s="1">
+        <v>50</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J77" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G72">
-        <v>100</v>
-      </c>
-      <c r="H72" s="49" t="s">
-        <v>34</v>
-      </c>
+    </row>
+    <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B78" s="20"/>
+      <c r="C78" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B79" s="20"/>
+      <c r="C79" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0.85909999999999997</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B80" s="20"/>
+      <c r="C80" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F80" s="2">
+        <v>0.84889999999999999</v>
+      </c>
+      <c r="G80" s="1">
+        <v>50</v>
+      </c>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B81" s="20"/>
+      <c r="C81" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F81" s="23">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="G81" s="1">
+        <v>50</v>
+      </c>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J81" s="4"/>
+    </row>
+    <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B82" s="20"/>
+      <c r="C82" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F82" s="2">
+        <v>0.87190000000000001</v>
+      </c>
+      <c r="G82" s="1">
+        <v>50</v>
+      </c>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B83" s="20"/>
+      <c r="C83" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F83" s="2">
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="G83" s="1">
+        <v>50</v>
+      </c>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B84" s="20"/>
+      <c r="C84" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F84" s="2">
+        <v>0.6804</v>
+      </c>
+      <c r="G84" s="1">
+        <v>50</v>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B85" s="20"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B86" s="20"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B87" s="20"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B88" s="20"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B89" s="20"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B90" s="20"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B91" s="20"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B92" s="20"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B93" s="20"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B94" s="20"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B95" s="20"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B96" s="20"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B97" s="20"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B98" s="20"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B99" s="20"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B100" s="20"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B101" s="20"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="21"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B30"/>
     <mergeCell ref="B31:B70"/>
     <mergeCell ref="J51:J70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B102"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C5:C6"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D5:D1048576">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",D5)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",D5)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[IMP] ResNet Standard Dogs sending p1
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF4D125-3994-184C-B7CA-3DB5BCE93D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE91BD9-970D-F94C-ABBF-8736AA186D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="760" windowWidth="28220" windowHeight="18360" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="1180" yWindow="760" windowWidth="28220" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
-    <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
+    <sheet name="StanfordDogs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="234">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -727,12 +728,18 @@
       <t>FROM HERE ON!</t>
     </r>
   </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>Resnet simple transforms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -891,8 +898,21 @@
       <color theme="8"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="46">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1150,8 +1170,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6C9EC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5E6A2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1675,6 +1713,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1720,7 +1817,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1734,12 +1831,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1749,15 +1840,9 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1776,15 +1861,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1831,12 +1907,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="44" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1890,31 +1960,127 @@
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="46" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="46" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="46" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="46" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="47" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2321,120 +2487,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="45"/>
-    <col min="2" max="2" width="16.5" style="45" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="45"/>
-    <col min="5" max="5" width="27.83203125" style="45" customWidth="1"/>
-    <col min="6" max="6" width="17" style="46" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="45"/>
-    <col min="9" max="9" width="17.5" style="45" customWidth="1"/>
-    <col min="10" max="10" width="29.33203125" style="45" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="45"/>
+    <col min="1" max="1" width="10.83203125" style="36"/>
+    <col min="2" max="2" width="16.5" style="36" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="36"/>
+    <col min="5" max="5" width="27.83203125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="17" style="37" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="36"/>
+    <col min="9" max="9" width="17.5" style="36" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" style="36" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="47"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="48"/>
+      <c r="N2" s="39"/>
     </row>
     <row r="3" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="49"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="2:14" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="50"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>0.75439999999999996</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>7</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="51"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="2">
         <v>0.83630000000000004</v>
       </c>
@@ -2447,143 +2613,143 @@
       <c r="I6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="52"/>
+      <c r="N6" s="43"/>
     </row>
     <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="10">
         <v>0.77610000000000001</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="9">
         <v>19</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="45" t="s">
+      <c r="M7" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="53"/>
+      <c r="N7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>19</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="45" t="s">
+      <c r="M8" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="54"/>
+      <c r="N8" s="45"/>
     </row>
     <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="57"/>
+      <c r="C9" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="10">
         <v>0.74109999999999998</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="9">
         <v>26</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="55"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>0.92279999999999995</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>29</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="M10" s="45" t="s">
+      <c r="J10" s="7"/>
+      <c r="M10" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="N10" s="56"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="9" t="s">
         <v>143</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2604,11 +2770,11 @@
       <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="11"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="58"/>
+      <c r="C12" s="12" t="s">
         <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2629,14 +2795,14 @@
       <c r="I12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="20"/>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="58"/>
+      <c r="C13" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="32" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2654,11 +2820,11 @@
       <c r="I13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="11"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="24" t="s">
         <v>146</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2679,13 +2845,13 @@
       <c r="I14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="58"/>
+      <c r="C15" s="24" t="s">
         <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2706,11 +2872,11 @@
       <c r="I15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="20"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="58"/>
+      <c r="C16" s="24" t="s">
         <v>148</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2731,11 +2897,11 @@
       <c r="I16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="11"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="24" t="s">
         <v>149</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2756,11 +2922,11 @@
       <c r="I17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="58"/>
+      <c r="C18" s="24" t="s">
         <v>150</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2781,11 +2947,11 @@
       <c r="I18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="11"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="20"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="58"/>
+      <c r="C19" s="26" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2806,11 +2972,11 @@
       <c r="I19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="20"/>
-      <c r="C20" s="33" t="s">
+      <c r="B20" s="58"/>
+      <c r="C20" s="26" t="s">
         <v>152</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2831,11 +2997,11 @@
       <c r="I20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="20"/>
-      <c r="C21" s="33" t="s">
+      <c r="B21" s="58"/>
+      <c r="C21" s="26" t="s">
         <v>153</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -2856,11 +3022,11 @@
       <c r="I21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="11"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="20"/>
-      <c r="C22" s="33" t="s">
+      <c r="B22" s="58"/>
+      <c r="C22" s="26" t="s">
         <v>154</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2881,11 +3047,11 @@
       <c r="I22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="11"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="20"/>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="27" t="s">
         <v>155</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2906,11 +3072,11 @@
       <c r="I23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="20"/>
-      <c r="C24" s="34" t="s">
+      <c r="B24" s="58"/>
+      <c r="C24" s="27" t="s">
         <v>156</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -2931,11 +3097,11 @@
       <c r="I24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="11"/>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="20"/>
-      <c r="C25" s="34" t="s">
+      <c r="B25" s="58"/>
+      <c r="C25" s="27" t="s">
         <v>157</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -2956,11 +3122,11 @@
       <c r="I25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="20"/>
-      <c r="C26" s="34" t="s">
+      <c r="B26" s="58"/>
+      <c r="C26" s="27" t="s">
         <v>158</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -2981,11 +3147,11 @@
       <c r="I26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="11"/>
+      <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="20"/>
-      <c r="C27" s="35" t="s">
+      <c r="B27" s="58"/>
+      <c r="C27" s="28" t="s">
         <v>159</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3006,11 +3172,11 @@
       <c r="I27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="11"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="20"/>
-      <c r="C28" s="35" t="s">
+      <c r="B28" s="58"/>
+      <c r="C28" s="28" t="s">
         <v>160</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -3031,11 +3197,11 @@
       <c r="I28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="20"/>
-      <c r="C29" s="35" t="s">
+      <c r="B29" s="58"/>
+      <c r="C29" s="28" t="s">
         <v>161</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -3056,65 +3222,65 @@
       <c r="I29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="11"/>
+      <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="21"/>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="57"/>
+      <c r="C30" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="10">
         <v>0.85589999999999999</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I30" s="13" t="s">
+      <c r="H30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="15"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <v>0.91569999999999996</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="5">
         <v>30</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="20"/>
-      <c r="C32" s="29" t="s">
+      <c r="B32" s="58"/>
+      <c r="C32" s="22" t="s">
         <v>163</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -3135,11 +3301,11 @@
       <c r="I32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="J32" s="8"/>
     </row>
     <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="20"/>
-      <c r="C33" s="27" t="s">
+      <c r="B33" s="58"/>
+      <c r="C33" s="20" t="s">
         <v>164</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3160,11 +3326,11 @@
       <c r="I33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="20"/>
-      <c r="C34" s="27" t="s">
+      <c r="B34" s="58"/>
+      <c r="C34" s="20" t="s">
         <v>165</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -3185,11 +3351,11 @@
       <c r="I34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J34" s="11"/>
+      <c r="J34" s="8"/>
     </row>
     <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="20"/>
-      <c r="C35" s="27" t="s">
+      <c r="B35" s="58"/>
+      <c r="C35" s="20" t="s">
         <v>166</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -3210,11 +3376,11 @@
       <c r="I35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="8"/>
     </row>
     <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="20"/>
-      <c r="C36" s="27" t="s">
+      <c r="B36" s="58"/>
+      <c r="C36" s="20" t="s">
         <v>167</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -3235,11 +3401,11 @@
       <c r="I36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J36" s="11"/>
+      <c r="J36" s="8"/>
     </row>
     <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="20"/>
-      <c r="C37" s="27" t="s">
+      <c r="B37" s="58"/>
+      <c r="C37" s="20" t="s">
         <v>168</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -3260,13 +3426,13 @@
       <c r="I37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J37" s="11" t="s">
+      <c r="J37" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="20"/>
-      <c r="C38" s="27" t="s">
+      <c r="B38" s="58"/>
+      <c r="C38" s="20" t="s">
         <v>169</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -3287,13 +3453,13 @@
       <c r="I38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="J38" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="20"/>
-      <c r="C39" s="29" t="s">
+      <c r="B39" s="58"/>
+      <c r="C39" s="22" t="s">
         <v>170</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -3314,11 +3480,11 @@
       <c r="I39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="11"/>
+      <c r="J39" s="8"/>
     </row>
     <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="20"/>
-      <c r="C40" s="29" t="s">
+      <c r="B40" s="58"/>
+      <c r="C40" s="22" t="s">
         <v>171</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -3339,13 +3505,13 @@
       <c r="I40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="11" t="s">
+      <c r="J40" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="20"/>
-      <c r="C41" s="29" t="s">
+      <c r="B41" s="58"/>
+      <c r="C41" s="22" t="s">
         <v>172</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -3366,11 +3532,11 @@
       <c r="I41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J41" s="11"/>
+      <c r="J41" s="8"/>
     </row>
     <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="20"/>
-      <c r="C42" s="29" t="s">
+      <c r="B42" s="58"/>
+      <c r="C42" s="22" t="s">
         <v>173</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -3391,11 +3557,11 @@
       <c r="I42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="11"/>
+      <c r="J42" s="8"/>
     </row>
     <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="20"/>
-      <c r="C43" s="30" t="s">
+      <c r="B43" s="58"/>
+      <c r="C43" s="23" t="s">
         <v>174</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -3416,11 +3582,11 @@
       <c r="I43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J43" s="11"/>
+      <c r="J43" s="8"/>
     </row>
     <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="20"/>
-      <c r="C44" s="30" t="s">
+      <c r="B44" s="58"/>
+      <c r="C44" s="23" t="s">
         <v>175</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -3441,11 +3607,11 @@
       <c r="I44" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="11"/>
+      <c r="J44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="20"/>
-      <c r="C45" s="30" t="s">
+      <c r="B45" s="58"/>
+      <c r="C45" s="23" t="s">
         <v>176</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -3466,11 +3632,11 @@
       <c r="I45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J45" s="11"/>
+      <c r="J45" s="8"/>
     </row>
     <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="20"/>
-      <c r="C46" s="30" t="s">
+      <c r="B46" s="58"/>
+      <c r="C46" s="23" t="s">
         <v>177</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -3491,11 +3657,11 @@
       <c r="I46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J46" s="11"/>
+      <c r="J46" s="8"/>
     </row>
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="20"/>
-      <c r="C47" s="43" t="s">
+      <c r="B47" s="58"/>
+      <c r="C47" s="34" t="s">
         <v>178</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -3516,13 +3682,13 @@
       <c r="I47" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J47" s="11" t="s">
+      <c r="J47" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B48" s="20"/>
-      <c r="C48" s="43" t="s">
+      <c r="B48" s="58"/>
+      <c r="C48" s="34" t="s">
         <v>179</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -3543,11 +3709,11 @@
       <c r="I48" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J48" s="11"/>
+      <c r="J48" s="8"/>
     </row>
     <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="20"/>
-      <c r="C49" s="37" t="s">
+      <c r="B49" s="58"/>
+      <c r="C49" s="30" t="s">
         <v>180</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -3566,11 +3732,11 @@
         <v>34</v>
       </c>
       <c r="I49" s="1"/>
-      <c r="J49" s="11"/>
+      <c r="J49" s="8"/>
     </row>
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="20"/>
-      <c r="C50" s="37" t="s">
+      <c r="B50" s="58"/>
+      <c r="C50" s="30" t="s">
         <v>181</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -3587,13 +3753,13 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="11" t="s">
+      <c r="J50" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="20"/>
-      <c r="C51" s="32" t="s">
+      <c r="B51" s="58"/>
+      <c r="C51" s="25" t="s">
         <v>182</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -3614,13 +3780,13 @@
       <c r="I51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J51" s="38" t="s">
+      <c r="J51" s="59" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="20"/>
-      <c r="C52" s="32" t="s">
+      <c r="B52" s="58"/>
+      <c r="C52" s="25" t="s">
         <v>183</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -3641,11 +3807,11 @@
       <c r="I52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="39"/>
+      <c r="J52" s="60"/>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="20"/>
-      <c r="C53" s="32" t="s">
+      <c r="B53" s="58"/>
+      <c r="C53" s="25" t="s">
         <v>184</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -3666,11 +3832,11 @@
       <c r="I53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="39"/>
+      <c r="J53" s="60"/>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="20"/>
-      <c r="C54" s="32" t="s">
+      <c r="B54" s="58"/>
+      <c r="C54" s="25" t="s">
         <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -3691,11 +3857,11 @@
       <c r="I54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J54" s="39"/>
+      <c r="J54" s="60"/>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="20"/>
-      <c r="C55" s="32" t="s">
+      <c r="B55" s="58"/>
+      <c r="C55" s="25" t="s">
         <v>186</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -3716,11 +3882,11 @@
       <c r="I55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J55" s="39"/>
+      <c r="J55" s="60"/>
     </row>
     <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="20"/>
-      <c r="C56" s="33" t="s">
+      <c r="B56" s="58"/>
+      <c r="C56" s="26" t="s">
         <v>187</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -3741,11 +3907,11 @@
       <c r="I56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J56" s="39"/>
+      <c r="J56" s="60"/>
     </row>
     <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="20"/>
-      <c r="C57" s="33" t="s">
+      <c r="B57" s="58"/>
+      <c r="C57" s="26" t="s">
         <v>188</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -3766,11 +3932,11 @@
       <c r="I57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J57" s="39"/>
+      <c r="J57" s="60"/>
     </row>
     <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B58" s="20"/>
-      <c r="C58" s="33" t="s">
+      <c r="B58" s="58"/>
+      <c r="C58" s="26" t="s">
         <v>189</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -3791,11 +3957,11 @@
       <c r="I58" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J58" s="39"/>
+      <c r="J58" s="60"/>
     </row>
     <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="20"/>
-      <c r="C59" s="33" t="s">
+      <c r="B59" s="58"/>
+      <c r="C59" s="26" t="s">
         <v>190</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -3816,11 +3982,11 @@
       <c r="I59" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J59" s="39"/>
+      <c r="J59" s="60"/>
     </row>
     <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="20"/>
-      <c r="C60" s="34" t="s">
+      <c r="B60" s="58"/>
+      <c r="C60" s="27" t="s">
         <v>191</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -3841,11 +4007,11 @@
       <c r="I60" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J60" s="39"/>
+      <c r="J60" s="60"/>
     </row>
     <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B61" s="20"/>
-      <c r="C61" s="34" t="s">
+      <c r="B61" s="58"/>
+      <c r="C61" s="27" t="s">
         <v>192</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -3866,11 +4032,11 @@
       <c r="I61" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J61" s="39"/>
+      <c r="J61" s="60"/>
     </row>
     <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B62" s="20"/>
-      <c r="C62" s="34" t="s">
+      <c r="B62" s="58"/>
+      <c r="C62" s="27" t="s">
         <v>193</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -3891,11 +4057,11 @@
       <c r="I62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J62" s="39"/>
+      <c r="J62" s="60"/>
     </row>
     <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B63" s="20"/>
-      <c r="C63" s="34" t="s">
+      <c r="B63" s="58"/>
+      <c r="C63" s="27" t="s">
         <v>194</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3916,11 +4082,11 @@
       <c r="I63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J63" s="39"/>
+      <c r="J63" s="60"/>
     </row>
     <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="20"/>
-      <c r="C64" s="35" t="s">
+      <c r="B64" s="58"/>
+      <c r="C64" s="28" t="s">
         <v>195</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -3941,11 +4107,11 @@
       <c r="I64" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J64" s="39"/>
+      <c r="J64" s="60"/>
     </row>
     <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B65" s="20"/>
-      <c r="C65" s="35" t="s">
+      <c r="B65" s="58"/>
+      <c r="C65" s="28" t="s">
         <v>196</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3966,11 +4132,11 @@
       <c r="I65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J65" s="39"/>
+      <c r="J65" s="60"/>
     </row>
     <row r="66" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="20"/>
-      <c r="C66" s="35" t="s">
+      <c r="B66" s="58"/>
+      <c r="C66" s="28" t="s">
         <v>197</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -3991,11 +4157,11 @@
       <c r="I66" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J66" s="39"/>
+      <c r="J66" s="60"/>
     </row>
     <row r="67" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="20"/>
-      <c r="C67" s="36" t="s">
+      <c r="B67" s="58"/>
+      <c r="C67" s="29" t="s">
         <v>198</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -4016,11 +4182,11 @@
       <c r="I67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="39"/>
-    </row>
-    <row r="68" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="20"/>
-      <c r="C68" s="36" t="s">
+      <c r="J67" s="60"/>
+    </row>
+    <row r="68" spans="2:10" ht="35" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="58"/>
+      <c r="C68" s="29" t="s">
         <v>199</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -4041,11 +4207,11 @@
       <c r="I68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J68" s="39"/>
-    </row>
-    <row r="69" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="20"/>
-      <c r="C69" s="36" t="s">
+      <c r="J68" s="60"/>
+    </row>
+    <row r="69" spans="2:10" ht="35" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="58"/>
+      <c r="C69" s="29" t="s">
         <v>200</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -4066,11 +4232,11 @@
       <c r="I69" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J69" s="39"/>
+      <c r="J69" s="60"/>
     </row>
     <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="21"/>
-      <c r="C70" s="62" t="s">
+      <c r="B70" s="57"/>
+      <c r="C70" s="49" t="s">
         <v>201</v>
       </c>
       <c r="D70" s="4" t="s">
@@ -4079,7 +4245,7 @@
       <c r="E70" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F70" s="23">
+      <c r="F70" s="16">
         <v>0.90859999999999996</v>
       </c>
       <c r="G70" s="4" t="s">
@@ -4091,32 +4257,32 @@
       <c r="I70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J70" s="39"/>
-    </row>
-    <row r="71" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="59" t="s">
+      <c r="J70" s="60"/>
+    </row>
+    <row r="71" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="63" t="s">
+      <c r="C71" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7" t="s">
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F71" s="6">
         <v>0.92759999999999998</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="G71" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="9"/>
-    </row>
-    <row r="72" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="60"/>
-      <c r="C72" s="64" t="s">
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="62"/>
+      <c r="C72" s="51" t="s">
         <v>203</v>
       </c>
       <c r="D72" s="1"/>
@@ -4131,11 +4297,11 @@
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="11"/>
-    </row>
-    <row r="73" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="60"/>
-      <c r="C73" s="64" t="s">
+      <c r="J72" s="8"/>
+    </row>
+    <row r="73" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="62"/>
+      <c r="C73" s="51" t="s">
         <v>204</v>
       </c>
       <c r="D73" s="1"/>
@@ -4146,53 +4312,53 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="11"/>
+      <c r="J73" s="8"/>
     </row>
     <row r="74" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="61"/>
-      <c r="C74" s="65" t="s">
+      <c r="B74" s="63"/>
+      <c r="C74" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13" t="s">
+      <c r="D74" s="9"/>
+      <c r="E74" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F74" s="14"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="15"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="11"/>
     </row>
     <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="C75" s="58" t="s">
+      <c r="C75" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F75" s="40">
+      <c r="F75" s="31">
         <v>0.84760000000000002</v>
       </c>
-      <c r="G75" s="5">
+      <c r="G75" s="3">
         <v>50</v>
       </c>
-      <c r="H75" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I75" s="5" t="s">
+      <c r="H75" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J75" s="5"/>
+      <c r="J75" s="3"/>
     </row>
     <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B76" s="20"/>
-      <c r="C76" s="17" t="s">
+      <c r="B76" s="58"/>
+      <c r="C76" s="13" t="s">
         <v>207</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -4216,8 +4382,8 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B77" s="20"/>
-      <c r="C77" s="17" t="s">
+      <c r="B77" s="58"/>
+      <c r="C77" s="13" t="s">
         <v>208</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -4243,8 +4409,8 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B78" s="20"/>
-      <c r="C78" s="17" t="s">
+      <c r="B78" s="58"/>
+      <c r="C78" s="13" t="s">
         <v>209</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -4268,8 +4434,8 @@
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B79" s="20"/>
-      <c r="C79" s="17" t="s">
+      <c r="B79" s="58"/>
+      <c r="C79" s="13" t="s">
         <v>210</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -4295,8 +4461,8 @@
       </c>
     </row>
     <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B80" s="20"/>
-      <c r="C80" s="17" t="s">
+      <c r="B80" s="58"/>
+      <c r="C80" s="13" t="s">
         <v>214</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -4318,8 +4484,8 @@
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B81" s="20"/>
-      <c r="C81" s="22" t="s">
+      <c r="B81" s="58"/>
+      <c r="C81" s="15" t="s">
         <v>221</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -4328,7 +4494,7 @@
       <c r="E81" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F81" s="23">
+      <c r="F81" s="16">
         <v>0.91720000000000002</v>
       </c>
       <c r="G81" s="1">
@@ -4341,8 +4507,8 @@
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B82" s="20"/>
-      <c r="C82" s="17" t="s">
+      <c r="B82" s="58"/>
+      <c r="C82" s="13" t="s">
         <v>223</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -4364,8 +4530,8 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B83" s="20"/>
-      <c r="C83" s="17" t="s">
+      <c r="B83" s="58"/>
+      <c r="C83" s="13" t="s">
         <v>224</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -4385,8 +4551,8 @@
       <c r="J83" s="1"/>
     </row>
     <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B84" s="20"/>
-      <c r="C84" s="17" t="s">
+      <c r="B84" s="58"/>
+      <c r="C84" s="13" t="s">
         <v>227</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -4406,8 +4572,8 @@
       <c r="J84" s="1"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="20"/>
-      <c r="C85" s="17"/>
+      <c r="B85" s="58"/>
+      <c r="C85" s="13"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="2"/>
@@ -4417,8 +4583,8 @@
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="20"/>
-      <c r="C86" s="17"/>
+      <c r="B86" s="58"/>
+      <c r="C86" s="13"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="2"/>
@@ -4428,8 +4594,8 @@
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B87" s="20"/>
-      <c r="C87" s="17"/>
+      <c r="B87" s="58"/>
+      <c r="C87" s="13"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="2"/>
@@ -4439,8 +4605,8 @@
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B88" s="20"/>
-      <c r="C88" s="17"/>
+      <c r="B88" s="58"/>
+      <c r="C88" s="13"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="2"/>
@@ -4450,8 +4616,8 @@
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="20"/>
-      <c r="C89" s="17"/>
+      <c r="B89" s="58"/>
+      <c r="C89" s="13"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="2"/>
@@ -4461,8 +4627,8 @@
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="20"/>
-      <c r="C90" s="17"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="13"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="2"/>
@@ -4472,8 +4638,8 @@
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B91" s="20"/>
-      <c r="C91" s="17"/>
+      <c r="B91" s="58"/>
+      <c r="C91" s="13"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="2"/>
@@ -4483,8 +4649,8 @@
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B92" s="20"/>
-      <c r="C92" s="17"/>
+      <c r="B92" s="58"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="2"/>
@@ -4494,8 +4660,8 @@
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" s="20"/>
-      <c r="C93" s="17"/>
+      <c r="B93" s="58"/>
+      <c r="C93" s="13"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="2"/>
@@ -4505,8 +4671,8 @@
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="20"/>
-      <c r="C94" s="17"/>
+      <c r="B94" s="58"/>
+      <c r="C94" s="13"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="2"/>
@@ -4516,8 +4682,8 @@
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="20"/>
-      <c r="C95" s="17"/>
+      <c r="B95" s="58"/>
+      <c r="C95" s="13"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="2"/>
@@ -4527,8 +4693,8 @@
       <c r="J95" s="1"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="20"/>
-      <c r="C96" s="17"/>
+      <c r="B96" s="58"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="2"/>
@@ -4538,8 +4704,8 @@
       <c r="J96" s="1"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B97" s="20"/>
-      <c r="C97" s="17"/>
+      <c r="B97" s="58"/>
+      <c r="C97" s="13"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="2"/>
@@ -4549,8 +4715,8 @@
       <c r="J97" s="1"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" s="20"/>
-      <c r="C98" s="17"/>
+      <c r="B98" s="58"/>
+      <c r="C98" s="13"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="2"/>
@@ -4560,8 +4726,8 @@
       <c r="J98" s="1"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="20"/>
-      <c r="C99" s="17"/>
+      <c r="B99" s="58"/>
+      <c r="C99" s="13"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="2"/>
@@ -4571,8 +4737,8 @@
       <c r="J99" s="1"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B100" s="20"/>
-      <c r="C100" s="17"/>
+      <c r="B100" s="58"/>
+      <c r="C100" s="13"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="2"/>
@@ -4582,8 +4748,8 @@
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B101" s="20"/>
-      <c r="C101" s="17"/>
+      <c r="B101" s="58"/>
+      <c r="C101" s="13"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="2"/>
@@ -4593,8 +4759,8 @@
       <c r="J101" s="1"/>
     </row>
     <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="21"/>
-      <c r="C102" s="17"/>
+      <c r="B102" s="57"/>
+      <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="2"/>
@@ -4605,15 +4771,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B102"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B30"/>
     <mergeCell ref="B31:B70"/>
     <mergeCell ref="J51:J70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B102"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D5:D1048576">
@@ -4629,4 +4795,299 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66"/>
+      <c r="B3" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+    </row>
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="66"/>
+      <c r="B4" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="87" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="73"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="66"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="66"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="66"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="66"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="66"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="66"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="66"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="66"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="66"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="66"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="66"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="66"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="66"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="66"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="66"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="66"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="66"/>
+    </row>
+    <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[IMP] Sending seeds and batch_1
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE91BD9-970D-F94C-ABBF-8736AA186D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA326ABB-3098-7C46-B660-D420306D9F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="760" windowWidth="28220" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="241">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -732,7 +732,28 @@
     <t>p1</t>
   </si>
   <si>
-    <t>Resnet simple transforms</t>
+    <t>Training time approx 1hour</t>
+  </si>
+  <si>
+    <t>21/31</t>
+  </si>
+  <si>
+    <t>Resnet simple transforms (scratch). ReduceLROnPlateau</t>
+  </si>
+  <si>
+    <t>Overfit so quickly and crazily</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>Resnet pretrained ReduceLROnPlateau</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>Resnet pretrained ReduceLROnPlateau vanilla transforms + color_jitter</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1772,6 +1793,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1817,7 +1847,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1975,45 +2005,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2041,47 +2032,89 @@
     <xf numFmtId="0" fontId="22" fillId="47" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="47" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="48" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="48" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="47" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2487,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N102"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2562,16 +2595,16 @@
       <c r="N4" s="41"/>
     </row>
     <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="79" t="s">
         <v>138</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="79" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6">
@@ -2595,12 +2628,12 @@
       <c r="N5" s="42"/>
     </row>
     <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="54"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="65"/>
+      <c r="E6" s="80"/>
       <c r="F6" s="2">
         <v>0.83630000000000004</v>
       </c>
@@ -2622,7 +2655,7 @@
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="9" t="s">
         <v>139</v>
       </c>
@@ -2653,7 +2686,7 @@
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="76" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -2686,7 +2719,7 @@
       <c r="N8" s="45"/>
     </row>
     <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="57"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="9" t="s">
         <v>141</v>
       </c>
@@ -2717,7 +2750,7 @@
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="76" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -2748,7 +2781,7 @@
       <c r="N10" s="47"/>
     </row>
     <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="9" t="s">
         <v>143</v>
       </c>
@@ -2773,7 +2806,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="58"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="12" t="s">
         <v>144</v>
       </c>
@@ -2798,7 +2831,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="58"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="33" t="s">
         <v>145</v>
       </c>
@@ -2823,7 +2856,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="58"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="24" t="s">
         <v>146</v>
       </c>
@@ -2850,7 +2883,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="24" t="s">
         <v>147</v>
       </c>
@@ -2875,7 +2908,7 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="58"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="24" t="s">
         <v>148</v>
       </c>
@@ -2900,7 +2933,7 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="58"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="24" t="s">
         <v>149</v>
       </c>
@@ -2925,7 +2958,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="58"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="24" t="s">
         <v>150</v>
       </c>
@@ -2950,7 +2983,7 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="58"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="26" t="s">
         <v>151</v>
       </c>
@@ -2975,7 +3008,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="58"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="26" t="s">
         <v>152</v>
       </c>
@@ -3000,7 +3033,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="58"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="26" t="s">
         <v>153</v>
       </c>
@@ -3025,7 +3058,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="58"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="26" t="s">
         <v>154</v>
       </c>
@@ -3050,7 +3083,7 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="58"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="27" t="s">
         <v>155</v>
       </c>
@@ -3075,7 +3108,7 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="58"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="27" t="s">
         <v>156</v>
       </c>
@@ -3100,7 +3133,7 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="58"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="27" t="s">
         <v>157</v>
       </c>
@@ -3125,7 +3158,7 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="58"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="27" t="s">
         <v>158</v>
       </c>
@@ -3150,7 +3183,7 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="58"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="28" t="s">
         <v>159</v>
       </c>
@@ -3175,7 +3208,7 @@
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="58"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="28" t="s">
         <v>160</v>
       </c>
@@ -3200,7 +3233,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="58"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="28" t="s">
         <v>161</v>
       </c>
@@ -3225,7 +3258,7 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="57"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="14" t="s">
         <v>211</v>
       </c>
@@ -3250,7 +3283,7 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="76" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="21" t="s">
@@ -3279,7 +3312,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="58"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="22" t="s">
         <v>163</v>
       </c>
@@ -3304,7 +3337,7 @@
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="58"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="20" t="s">
         <v>164</v>
       </c>
@@ -3329,7 +3362,7 @@
       <c r="J33" s="8"/>
     </row>
     <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="58"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="20" t="s">
         <v>165</v>
       </c>
@@ -3354,7 +3387,7 @@
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="58"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="20" t="s">
         <v>166</v>
       </c>
@@ -3379,7 +3412,7 @@
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="58"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="20" t="s">
         <v>167</v>
       </c>
@@ -3404,7 +3437,7 @@
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="58"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="20" t="s">
         <v>168</v>
       </c>
@@ -3431,7 +3464,7 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="58"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="20" t="s">
         <v>169</v>
       </c>
@@ -3458,7 +3491,7 @@
       </c>
     </row>
     <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="58"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="22" t="s">
         <v>170</v>
       </c>
@@ -3483,7 +3516,7 @@
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="58"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="22" t="s">
         <v>171</v>
       </c>
@@ -3510,7 +3543,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="58"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="22" t="s">
         <v>172</v>
       </c>
@@ -3535,7 +3568,7 @@
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="58"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="22" t="s">
         <v>173</v>
       </c>
@@ -3560,7 +3593,7 @@
       <c r="J42" s="8"/>
     </row>
     <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="58"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="23" t="s">
         <v>174</v>
       </c>
@@ -3585,7 +3618,7 @@
       <c r="J43" s="8"/>
     </row>
     <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="58"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="23" t="s">
         <v>175</v>
       </c>
@@ -3610,7 +3643,7 @@
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="58"/>
+      <c r="B45" s="77"/>
       <c r="C45" s="23" t="s">
         <v>176</v>
       </c>
@@ -3635,7 +3668,7 @@
       <c r="J45" s="8"/>
     </row>
     <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="58"/>
+      <c r="B46" s="77"/>
       <c r="C46" s="23" t="s">
         <v>177</v>
       </c>
@@ -3660,7 +3693,7 @@
       <c r="J46" s="8"/>
     </row>
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="58"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="34" t="s">
         <v>178</v>
       </c>
@@ -3687,7 +3720,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B48" s="58"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="34" t="s">
         <v>179</v>
       </c>
@@ -3712,7 +3745,7 @@
       <c r="J48" s="8"/>
     </row>
     <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="58"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="30" t="s">
         <v>180</v>
       </c>
@@ -3735,7 +3768,7 @@
       <c r="J49" s="8"/>
     </row>
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="58"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="30" t="s">
         <v>181</v>
       </c>
@@ -3758,7 +3791,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="58"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="25" t="s">
         <v>182</v>
       </c>
@@ -3780,12 +3813,12 @@
       <c r="I51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J51" s="59" t="s">
+      <c r="J51" s="84" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="58"/>
+      <c r="B52" s="77"/>
       <c r="C52" s="25" t="s">
         <v>183</v>
       </c>
@@ -3807,10 +3840,10 @@
       <c r="I52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="60"/>
+      <c r="J52" s="85"/>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="58"/>
+      <c r="B53" s="77"/>
       <c r="C53" s="25" t="s">
         <v>184</v>
       </c>
@@ -3832,10 +3865,10 @@
       <c r="I53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="60"/>
+      <c r="J53" s="85"/>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="58"/>
+      <c r="B54" s="77"/>
       <c r="C54" s="25" t="s">
         <v>185</v>
       </c>
@@ -3857,10 +3890,10 @@
       <c r="I54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J54" s="60"/>
+      <c r="J54" s="85"/>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="58"/>
+      <c r="B55" s="77"/>
       <c r="C55" s="25" t="s">
         <v>186</v>
       </c>
@@ -3882,10 +3915,10 @@
       <c r="I55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J55" s="60"/>
+      <c r="J55" s="85"/>
     </row>
     <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="58"/>
+      <c r="B56" s="77"/>
       <c r="C56" s="26" t="s">
         <v>187</v>
       </c>
@@ -3907,10 +3940,10 @@
       <c r="I56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J56" s="60"/>
+      <c r="J56" s="85"/>
     </row>
     <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="58"/>
+      <c r="B57" s="77"/>
       <c r="C57" s="26" t="s">
         <v>188</v>
       </c>
@@ -3932,10 +3965,10 @@
       <c r="I57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J57" s="60"/>
+      <c r="J57" s="85"/>
     </row>
     <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B58" s="58"/>
+      <c r="B58" s="77"/>
       <c r="C58" s="26" t="s">
         <v>189</v>
       </c>
@@ -3957,10 +3990,10 @@
       <c r="I58" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J58" s="60"/>
+      <c r="J58" s="85"/>
     </row>
     <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="58"/>
+      <c r="B59" s="77"/>
       <c r="C59" s="26" t="s">
         <v>190</v>
       </c>
@@ -3982,10 +4015,10 @@
       <c r="I59" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J59" s="60"/>
+      <c r="J59" s="85"/>
     </row>
     <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="58"/>
+      <c r="B60" s="77"/>
       <c r="C60" s="27" t="s">
         <v>191</v>
       </c>
@@ -4007,10 +4040,10 @@
       <c r="I60" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J60" s="60"/>
+      <c r="J60" s="85"/>
     </row>
     <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B61" s="58"/>
+      <c r="B61" s="77"/>
       <c r="C61" s="27" t="s">
         <v>192</v>
       </c>
@@ -4032,10 +4065,10 @@
       <c r="I61" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J61" s="60"/>
+      <c r="J61" s="85"/>
     </row>
     <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B62" s="58"/>
+      <c r="B62" s="77"/>
       <c r="C62" s="27" t="s">
         <v>193</v>
       </c>
@@ -4057,10 +4090,10 @@
       <c r="I62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J62" s="60"/>
+      <c r="J62" s="85"/>
     </row>
     <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B63" s="58"/>
+      <c r="B63" s="77"/>
       <c r="C63" s="27" t="s">
         <v>194</v>
       </c>
@@ -4082,10 +4115,10 @@
       <c r="I63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J63" s="60"/>
+      <c r="J63" s="85"/>
     </row>
     <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="58"/>
+      <c r="B64" s="77"/>
       <c r="C64" s="28" t="s">
         <v>195</v>
       </c>
@@ -4107,10 +4140,10 @@
       <c r="I64" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J64" s="60"/>
+      <c r="J64" s="85"/>
     </row>
     <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B65" s="58"/>
+      <c r="B65" s="77"/>
       <c r="C65" s="28" t="s">
         <v>196</v>
       </c>
@@ -4132,10 +4165,10 @@
       <c r="I65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J65" s="60"/>
-    </row>
-    <row r="66" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="58"/>
+      <c r="J65" s="85"/>
+    </row>
+    <row r="66" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B66" s="77"/>
       <c r="C66" s="28" t="s">
         <v>197</v>
       </c>
@@ -4157,10 +4190,10 @@
       <c r="I66" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J66" s="60"/>
-    </row>
-    <row r="67" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="58"/>
+      <c r="J66" s="85"/>
+    </row>
+    <row r="67" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="77"/>
       <c r="C67" s="29" t="s">
         <v>198</v>
       </c>
@@ -4182,10 +4215,10 @@
       <c r="I67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="60"/>
-    </row>
-    <row r="68" spans="2:10" ht="35" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="58"/>
+      <c r="J67" s="85"/>
+    </row>
+    <row r="68" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="77"/>
       <c r="C68" s="29" t="s">
         <v>199</v>
       </c>
@@ -4207,10 +4240,10 @@
       <c r="I68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J68" s="60"/>
-    </row>
-    <row r="69" spans="2:10" ht="35" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="58"/>
+      <c r="J68" s="85"/>
+    </row>
+    <row r="69" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="77"/>
       <c r="C69" s="29" t="s">
         <v>200</v>
       </c>
@@ -4232,10 +4265,10 @@
       <c r="I69" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J69" s="60"/>
+      <c r="J69" s="85"/>
     </row>
     <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="57"/>
+      <c r="B70" s="78"/>
       <c r="C70" s="49" t="s">
         <v>201</v>
       </c>
@@ -4257,10 +4290,10 @@
       <c r="I70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J70" s="60"/>
-    </row>
-    <row r="71" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="61" t="s">
+      <c r="J70" s="85"/>
+    </row>
+    <row r="71" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="73" t="s">
         <v>133</v>
       </c>
       <c r="C71" s="50" t="s">
@@ -4280,8 +4313,8 @@
       <c r="I71" s="5"/>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="62"/>
+    <row r="72" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="74"/>
       <c r="C72" s="51" t="s">
         <v>203</v>
       </c>
@@ -4299,8 +4332,8 @@
       <c r="I72" s="1"/>
       <c r="J72" s="8"/>
     </row>
-    <row r="73" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="62"/>
+    <row r="73" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="74"/>
       <c r="C73" s="51" t="s">
         <v>204</v>
       </c>
@@ -4315,7 +4348,7 @@
       <c r="J73" s="8"/>
     </row>
     <row r="74" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="63"/>
+      <c r="B74" s="75"/>
       <c r="C74" s="52" t="s">
         <v>205</v>
       </c>
@@ -4330,7 +4363,7 @@
       <c r="J74" s="11"/>
     </row>
     <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="76" t="s">
         <v>131</v>
       </c>
       <c r="C75" s="48" t="s">
@@ -4357,7 +4390,7 @@
       <c r="J75" s="3"/>
     </row>
     <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B76" s="58"/>
+      <c r="B76" s="77"/>
       <c r="C76" s="13" t="s">
         <v>207</v>
       </c>
@@ -4382,7 +4415,7 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B77" s="58"/>
+      <c r="B77" s="77"/>
       <c r="C77" s="13" t="s">
         <v>208</v>
       </c>
@@ -4409,7 +4442,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B78" s="58"/>
+      <c r="B78" s="77"/>
       <c r="C78" s="13" t="s">
         <v>209</v>
       </c>
@@ -4434,7 +4467,7 @@
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B79" s="58"/>
+      <c r="B79" s="77"/>
       <c r="C79" s="13" t="s">
         <v>210</v>
       </c>
@@ -4461,7 +4494,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B80" s="58"/>
+      <c r="B80" s="77"/>
       <c r="C80" s="13" t="s">
         <v>214</v>
       </c>
@@ -4484,7 +4517,7 @@
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B81" s="58"/>
+      <c r="B81" s="77"/>
       <c r="C81" s="15" t="s">
         <v>221</v>
       </c>
@@ -4507,7 +4540,7 @@
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B82" s="58"/>
+      <c r="B82" s="77"/>
       <c r="C82" s="13" t="s">
         <v>223</v>
       </c>
@@ -4530,7 +4563,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B83" s="58"/>
+      <c r="B83" s="77"/>
       <c r="C83" s="13" t="s">
         <v>224</v>
       </c>
@@ -4551,7 +4584,7 @@
       <c r="J83" s="1"/>
     </row>
     <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B84" s="58"/>
+      <c r="B84" s="77"/>
       <c r="C84" s="13" t="s">
         <v>227</v>
       </c>
@@ -4572,7 +4605,7 @@
       <c r="J84" s="1"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="58"/>
+      <c r="B85" s="77"/>
       <c r="C85" s="13"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -4583,7 +4616,7 @@
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="58"/>
+      <c r="B86" s="77"/>
       <c r="C86" s="13"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4594,7 +4627,7 @@
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B87" s="58"/>
+      <c r="B87" s="77"/>
       <c r="C87" s="13"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4605,7 +4638,7 @@
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B88" s="58"/>
+      <c r="B88" s="77"/>
       <c r="C88" s="13"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4616,7 +4649,7 @@
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="58"/>
+      <c r="B89" s="77"/>
       <c r="C89" s="13"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4627,7 +4660,7 @@
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="58"/>
+      <c r="B90" s="77"/>
       <c r="C90" s="13"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -4638,7 +4671,7 @@
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B91" s="58"/>
+      <c r="B91" s="77"/>
       <c r="C91" s="13"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4649,7 +4682,7 @@
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B92" s="58"/>
+      <c r="B92" s="77"/>
       <c r="C92" s="13"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4660,7 +4693,7 @@
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" s="58"/>
+      <c r="B93" s="77"/>
       <c r="C93" s="13"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4671,7 +4704,7 @@
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="58"/>
+      <c r="B94" s="77"/>
       <c r="C94" s="13"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4682,7 +4715,7 @@
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="58"/>
+      <c r="B95" s="77"/>
       <c r="C95" s="13"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -4693,7 +4726,7 @@
       <c r="J95" s="1"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="58"/>
+      <c r="B96" s="77"/>
       <c r="C96" s="13"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4704,7 +4737,7 @@
       <c r="J96" s="1"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B97" s="58"/>
+      <c r="B97" s="77"/>
       <c r="C97" s="13"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4715,7 +4748,7 @@
       <c r="J97" s="1"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" s="58"/>
+      <c r="B98" s="77"/>
       <c r="C98" s="13"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4726,7 +4759,7 @@
       <c r="J98" s="1"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="58"/>
+      <c r="B99" s="77"/>
       <c r="C99" s="13"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4737,7 +4770,7 @@
       <c r="J99" s="1"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B100" s="58"/>
+      <c r="B100" s="77"/>
       <c r="C100" s="13"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4748,7 +4781,7 @@
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B101" s="58"/>
+      <c r="B101" s="77"/>
       <c r="C101" s="13"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4759,7 +4792,7 @@
       <c r="J101" s="1"/>
     </row>
     <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="57"/>
+      <c r="B102" s="78"/>
       <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4771,6 +4804,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="J51:J70"/>
     <mergeCell ref="B71:B74"/>
     <mergeCell ref="B75:B102"/>
     <mergeCell ref="E5:E6"/>
@@ -4779,7 +4813,6 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B30"/>
     <mergeCell ref="B31:B70"/>
-    <mergeCell ref="J51:J70"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D5:D1048576">
@@ -4802,291 +4835,313 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.5" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="89" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="68" t="s">
+      <c r="A3" s="53"/>
+      <c r="B3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-    </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="66"/>
-      <c r="B4" s="76" t="s">
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+    </row>
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
+      <c r="B4" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="71" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="72" t="s">
-        <v>233</v>
-      </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
+      <c r="E4" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="60">
+        <v>0.36480000000000001</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+    </row>
+    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="53"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="64"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+    </row>
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="53"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="71" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" s="64"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="66"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="87"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="66"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="66"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="66"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="66"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="66"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="66"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="66"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="66"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="66"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="66"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B4:B21"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[IMP] Sending batch 2 p5-9
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA326ABB-3098-7C46-B660-D420306D9F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF917E2-74F3-DF4A-ADC3-A6C66342EF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="760" windowWidth="28220" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="15240" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
     <sheet name="StanfordDogs" sheetId="2" r:id="rId2"/>
+    <sheet name="Config Tables" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="287">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -741,19 +742,192 @@
     <t>Resnet simple transforms (scratch). ReduceLROnPlateau</t>
   </si>
   <si>
-    <t>Overfit so quickly and crazily</t>
-  </si>
-  <si>
     <t>p2</t>
   </si>
   <si>
-    <t>Resnet pretrained ReduceLROnPlateau</t>
-  </si>
-  <si>
     <t>p3</t>
   </si>
   <si>
-    <t>Resnet pretrained ReduceLROnPlateau vanilla transforms + color_jitter</t>
+    <t>Seed tests</t>
+  </si>
+  <si>
+    <t>p3 but from scratch</t>
+  </si>
+  <si>
+    <t>ps1</t>
+  </si>
+  <si>
+    <t>ps2</t>
+  </si>
+  <si>
+    <t>ps3</t>
+  </si>
+  <si>
+    <t>ps4</t>
+  </si>
+  <si>
+    <t>p3 but from scratch. Epoch 1 3.0740 32.06</t>
+  </si>
+  <si>
+    <t>p3. epoch 1 4.8127 1.70</t>
+  </si>
+  <si>
+    <t>p3 epoch 4.8127 1.70</t>
+  </si>
+  <si>
+    <t>15/25</t>
+  </si>
+  <si>
+    <t>17/27</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>ZoomVit (scratch) + color_jitter (0.1s)</t>
+  </si>
+  <si>
+    <t>BrainiT</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>Resnet pretrained ReduceLROnPlateau V1</t>
+  </si>
+  <si>
+    <t>Resnet pretrained ReduceLROnPlateau vanilla transforms + color_jitter (0.2s) V1</t>
+  </si>
+  <si>
+    <t>Overfit so quickly and crazily.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Still overfits! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Wrong</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - need to use imagenet norm and redo transforms</t>
+    </r>
+  </si>
+  <si>
+    <t>Still in learning phase. Train longer</t>
+  </si>
+  <si>
+    <t>ResNet</t>
+  </si>
+  <si>
+    <t>Pretrained</t>
+  </si>
+  <si>
+    <t>Scratch</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Resize(256)
+CenterCrop(224)
+Tensor
+Normalise(Imagenet)</t>
+  </si>
+  <si>
+    <t>Resize((224, 224))
+Tensor
+Normalise(StanfordDogs)</t>
+  </si>
+  <si>
+    <t>ResNet/ZoomViT</t>
+  </si>
+  <si>
+    <t>RRC(224, scale=(0.8, 1))
+RHorizontalFlip()
+ColorJitter(0.2, 0.2, 0.2)
+Tensor
+Normalise(StanfordDogs)</t>
+  </si>
+  <si>
+    <t>RRC(224, scale=(0.7, 1))
+RHorizontalFlip()
+ColorJitter(0.2, 0.2, 0.2)
+Tensor
+Normalise(Imagenet)</t>
+  </si>
+  <si>
+    <t>Transforms</t>
+  </si>
+  <si>
+    <t>Optimisers and schedulers</t>
+  </si>
+  <si>
+    <t>CosineLRScheduler(t_initial=45, warmup_t=5, warmup_lr_init=1e-5, lr_min=1e-6)
+AdamW(lr=0.001, weight_decay=1e-4)</t>
+  </si>
+  <si>
+    <t>CosineLRScheduler(t_initial=45, warmup_t=5, warmup_lr_init=1e-5, lr_min=1e-6)
+AdamW(lr=0.001, weight_decay=1e-2)</t>
+  </si>
+  <si>
+    <t>Resnet pretrained, correct (config tables)</t>
+  </si>
+  <si>
+    <t>ZoomVit scratch, correct (config tables)</t>
+  </si>
+  <si>
+    <t>Resnet scratch, correct (config tables)</t>
+  </si>
+  <si>
+    <t>Resnet pretrained, correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>p7</t>
+  </si>
+  <si>
+    <t>ZoomVit scratch, correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>p8</t>
+  </si>
+  <si>
+    <t>ZoomViT (pretrained), correct (config tables)</t>
+  </si>
+  <si>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>ZoomViT (pretrained), correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>Brainit (scratch) +  correct (config tables</t>
+  </si>
+  <si>
+    <t>Brainit scratch, correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>Brainit (pretrained), correct (config tables)</t>
+  </si>
+  <si>
+    <t>Brainit (pretrained), correct (config tables) but no color jitter</t>
   </si>
 </sst>
 </file>
@@ -933,7 +1107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1209,8 +1383,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -1773,10 +1959,23 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1784,20 +1983,122 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1847,7 +2148,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2005,6 +2306,9 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2044,27 +2348,12 @@
     <xf numFmtId="0" fontId="22" fillId="48" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="48" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2113,8 +2402,129 @@
     <xf numFmtId="0" fontId="22" fillId="47" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="49" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="49" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="50" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="50" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2520,8 +2930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N102"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2595,16 +3005,16 @@
       <c r="N4" s="41"/>
     </row>
     <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="75" t="s">
         <v>138</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="75" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6">
@@ -2628,12 +3038,12 @@
       <c r="N5" s="42"/>
     </row>
     <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="82"/>
-      <c r="C6" s="80"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="80"/>
+      <c r="E6" s="76"/>
       <c r="F6" s="2">
         <v>0.83630000000000004</v>
       </c>
@@ -2655,7 +3065,7 @@
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="83"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="9" t="s">
         <v>139</v>
       </c>
@@ -2686,7 +3096,7 @@
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="72" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -2719,7 +3129,7 @@
       <c r="N8" s="45"/>
     </row>
     <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="78"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="9" t="s">
         <v>141</v>
       </c>
@@ -2750,7 +3160,7 @@
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="72" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -2781,7 +3191,7 @@
       <c r="N10" s="47"/>
     </row>
     <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="77"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="9" t="s">
         <v>143</v>
       </c>
@@ -2806,7 +3216,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="77"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="12" t="s">
         <v>144</v>
       </c>
@@ -2831,7 +3241,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="77"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="33" t="s">
         <v>145</v>
       </c>
@@ -2856,7 +3266,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="77"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="24" t="s">
         <v>146</v>
       </c>
@@ -2883,7 +3293,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="77"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="24" t="s">
         <v>147</v>
       </c>
@@ -2908,7 +3318,7 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="77"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="24" t="s">
         <v>148</v>
       </c>
@@ -2933,7 +3343,7 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="77"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="24" t="s">
         <v>149</v>
       </c>
@@ -2958,7 +3368,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="77"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="24" t="s">
         <v>150</v>
       </c>
@@ -2983,7 +3393,7 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="77"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="26" t="s">
         <v>151</v>
       </c>
@@ -3008,7 +3418,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="77"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="26" t="s">
         <v>152</v>
       </c>
@@ -3033,7 +3443,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="77"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="26" t="s">
         <v>153</v>
       </c>
@@ -3058,7 +3468,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="77"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="26" t="s">
         <v>154</v>
       </c>
@@ -3083,7 +3493,7 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="77"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="27" t="s">
         <v>155</v>
       </c>
@@ -3108,7 +3518,7 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="77"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="27" t="s">
         <v>156</v>
       </c>
@@ -3133,7 +3543,7 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="77"/>
+      <c r="B25" s="73"/>
       <c r="C25" s="27" t="s">
         <v>157</v>
       </c>
@@ -3158,7 +3568,7 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="77"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="27" t="s">
         <v>158</v>
       </c>
@@ -3183,7 +3593,7 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="77"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="28" t="s">
         <v>159</v>
       </c>
@@ -3208,7 +3618,7 @@
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="77"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="28" t="s">
         <v>160</v>
       </c>
@@ -3233,7 +3643,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="77"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="28" t="s">
         <v>161</v>
       </c>
@@ -3258,7 +3668,7 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="78"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="14" t="s">
         <v>211</v>
       </c>
@@ -3283,7 +3693,7 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="72" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="21" t="s">
@@ -3312,7 +3722,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="77"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="22" t="s">
         <v>163</v>
       </c>
@@ -3337,7 +3747,7 @@
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="77"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="20" t="s">
         <v>164</v>
       </c>
@@ -3362,7 +3772,7 @@
       <c r="J33" s="8"/>
     </row>
     <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="77"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="20" t="s">
         <v>165</v>
       </c>
@@ -3387,7 +3797,7 @@
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="77"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="20" t="s">
         <v>166</v>
       </c>
@@ -3412,7 +3822,7 @@
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="77"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="20" t="s">
         <v>167</v>
       </c>
@@ -3437,7 +3847,7 @@
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="77"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="20" t="s">
         <v>168</v>
       </c>
@@ -3464,7 +3874,7 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="77"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="20" t="s">
         <v>169</v>
       </c>
@@ -3491,7 +3901,7 @@
       </c>
     </row>
     <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="77"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="22" t="s">
         <v>170</v>
       </c>
@@ -3516,7 +3926,7 @@
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="77"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="22" t="s">
         <v>171</v>
       </c>
@@ -3543,7 +3953,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="77"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="22" t="s">
         <v>172</v>
       </c>
@@ -3568,7 +3978,7 @@
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="77"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="22" t="s">
         <v>173</v>
       </c>
@@ -3593,7 +4003,7 @@
       <c r="J42" s="8"/>
     </row>
     <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="77"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="23" t="s">
         <v>174</v>
       </c>
@@ -3618,7 +4028,7 @@
       <c r="J43" s="8"/>
     </row>
     <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="77"/>
+      <c r="B44" s="73"/>
       <c r="C44" s="23" t="s">
         <v>175</v>
       </c>
@@ -3643,7 +4053,7 @@
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="77"/>
+      <c r="B45" s="73"/>
       <c r="C45" s="23" t="s">
         <v>176</v>
       </c>
@@ -3668,7 +4078,7 @@
       <c r="J45" s="8"/>
     </row>
     <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="77"/>
+      <c r="B46" s="73"/>
       <c r="C46" s="23" t="s">
         <v>177</v>
       </c>
@@ -3693,7 +4103,7 @@
       <c r="J46" s="8"/>
     </row>
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="77"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="34" t="s">
         <v>178</v>
       </c>
@@ -3720,7 +4130,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B48" s="77"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="34" t="s">
         <v>179</v>
       </c>
@@ -3745,7 +4155,7 @@
       <c r="J48" s="8"/>
     </row>
     <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="77"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="30" t="s">
         <v>180</v>
       </c>
@@ -3768,7 +4178,7 @@
       <c r="J49" s="8"/>
     </row>
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="77"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="30" t="s">
         <v>181</v>
       </c>
@@ -3791,7 +4201,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="77"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="25" t="s">
         <v>182</v>
       </c>
@@ -3813,12 +4223,12 @@
       <c r="I51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J51" s="84" t="s">
+      <c r="J51" s="80" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="77"/>
+      <c r="B52" s="73"/>
       <c r="C52" s="25" t="s">
         <v>183</v>
       </c>
@@ -3840,10 +4250,10 @@
       <c r="I52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="85"/>
+      <c r="J52" s="81"/>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="77"/>
+      <c r="B53" s="73"/>
       <c r="C53" s="25" t="s">
         <v>184</v>
       </c>
@@ -3865,10 +4275,10 @@
       <c r="I53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="85"/>
+      <c r="J53" s="81"/>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="77"/>
+      <c r="B54" s="73"/>
       <c r="C54" s="25" t="s">
         <v>185</v>
       </c>
@@ -3890,10 +4300,10 @@
       <c r="I54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J54" s="85"/>
+      <c r="J54" s="81"/>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="77"/>
+      <c r="B55" s="73"/>
       <c r="C55" s="25" t="s">
         <v>186</v>
       </c>
@@ -3915,10 +4325,10 @@
       <c r="I55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J55" s="85"/>
+      <c r="J55" s="81"/>
     </row>
     <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="77"/>
+      <c r="B56" s="73"/>
       <c r="C56" s="26" t="s">
         <v>187</v>
       </c>
@@ -3940,10 +4350,10 @@
       <c r="I56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J56" s="85"/>
+      <c r="J56" s="81"/>
     </row>
     <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="77"/>
+      <c r="B57" s="73"/>
       <c r="C57" s="26" t="s">
         <v>188</v>
       </c>
@@ -3965,10 +4375,10 @@
       <c r="I57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J57" s="85"/>
+      <c r="J57" s="81"/>
     </row>
     <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B58" s="77"/>
+      <c r="B58" s="73"/>
       <c r="C58" s="26" t="s">
         <v>189</v>
       </c>
@@ -3990,10 +4400,10 @@
       <c r="I58" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J58" s="85"/>
+      <c r="J58" s="81"/>
     </row>
     <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="77"/>
+      <c r="B59" s="73"/>
       <c r="C59" s="26" t="s">
         <v>190</v>
       </c>
@@ -4015,10 +4425,10 @@
       <c r="I59" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J59" s="85"/>
+      <c r="J59" s="81"/>
     </row>
     <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="77"/>
+      <c r="B60" s="73"/>
       <c r="C60" s="27" t="s">
         <v>191</v>
       </c>
@@ -4040,10 +4450,10 @@
       <c r="I60" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J60" s="85"/>
+      <c r="J60" s="81"/>
     </row>
     <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B61" s="77"/>
+      <c r="B61" s="73"/>
       <c r="C61" s="27" t="s">
         <v>192</v>
       </c>
@@ -4065,10 +4475,10 @@
       <c r="I61" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J61" s="85"/>
+      <c r="J61" s="81"/>
     </row>
     <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B62" s="77"/>
+      <c r="B62" s="73"/>
       <c r="C62" s="27" t="s">
         <v>193</v>
       </c>
@@ -4090,10 +4500,10 @@
       <c r="I62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J62" s="85"/>
+      <c r="J62" s="81"/>
     </row>
     <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B63" s="77"/>
+      <c r="B63" s="73"/>
       <c r="C63" s="27" t="s">
         <v>194</v>
       </c>
@@ -4115,10 +4525,10 @@
       <c r="I63" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J63" s="85"/>
+      <c r="J63" s="81"/>
     </row>
     <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="77"/>
+      <c r="B64" s="73"/>
       <c r="C64" s="28" t="s">
         <v>195</v>
       </c>
@@ -4140,10 +4550,10 @@
       <c r="I64" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J64" s="85"/>
+      <c r="J64" s="81"/>
     </row>
     <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B65" s="77"/>
+      <c r="B65" s="73"/>
       <c r="C65" s="28" t="s">
         <v>196</v>
       </c>
@@ -4165,10 +4575,10 @@
       <c r="I65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J65" s="85"/>
+      <c r="J65" s="81"/>
     </row>
     <row r="66" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B66" s="77"/>
+      <c r="B66" s="73"/>
       <c r="C66" s="28" t="s">
         <v>197</v>
       </c>
@@ -4190,10 +4600,10 @@
       <c r="I66" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J66" s="85"/>
+      <c r="J66" s="81"/>
     </row>
     <row r="67" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="77"/>
+      <c r="B67" s="73"/>
       <c r="C67" s="29" t="s">
         <v>198</v>
       </c>
@@ -4215,10 +4625,10 @@
       <c r="I67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="85"/>
+      <c r="J67" s="81"/>
     </row>
     <row r="68" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="77"/>
+      <c r="B68" s="73"/>
       <c r="C68" s="29" t="s">
         <v>199</v>
       </c>
@@ -4240,10 +4650,10 @@
       <c r="I68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J68" s="85"/>
+      <c r="J68" s="81"/>
     </row>
     <row r="69" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="77"/>
+      <c r="B69" s="73"/>
       <c r="C69" s="29" t="s">
         <v>200</v>
       </c>
@@ -4265,10 +4675,10 @@
       <c r="I69" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J69" s="85"/>
+      <c r="J69" s="81"/>
     </row>
     <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="78"/>
+      <c r="B70" s="74"/>
       <c r="C70" s="49" t="s">
         <v>201</v>
       </c>
@@ -4290,10 +4700,10 @@
       <c r="I70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J70" s="85"/>
+      <c r="J70" s="81"/>
     </row>
     <row r="71" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="73" t="s">
+      <c r="B71" s="69" t="s">
         <v>133</v>
       </c>
       <c r="C71" s="50" t="s">
@@ -4314,7 +4724,7 @@
       <c r="J71" s="7"/>
     </row>
     <row r="72" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="74"/>
+      <c r="B72" s="70"/>
       <c r="C72" s="51" t="s">
         <v>203</v>
       </c>
@@ -4333,7 +4743,7 @@
       <c r="J72" s="8"/>
     </row>
     <row r="73" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="74"/>
+      <c r="B73" s="70"/>
       <c r="C73" s="51" t="s">
         <v>204</v>
       </c>
@@ -4348,7 +4758,7 @@
       <c r="J73" s="8"/>
     </row>
     <row r="74" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="75"/>
+      <c r="B74" s="71"/>
       <c r="C74" s="52" t="s">
         <v>205</v>
       </c>
@@ -4363,7 +4773,7 @@
       <c r="J74" s="11"/>
     </row>
     <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="76" t="s">
+      <c r="B75" s="72" t="s">
         <v>131</v>
       </c>
       <c r="C75" s="48" t="s">
@@ -4390,7 +4800,7 @@
       <c r="J75" s="3"/>
     </row>
     <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B76" s="77"/>
+      <c r="B76" s="73"/>
       <c r="C76" s="13" t="s">
         <v>207</v>
       </c>
@@ -4415,7 +4825,7 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B77" s="77"/>
+      <c r="B77" s="73"/>
       <c r="C77" s="13" t="s">
         <v>208</v>
       </c>
@@ -4442,7 +4852,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B78" s="77"/>
+      <c r="B78" s="73"/>
       <c r="C78" s="13" t="s">
         <v>209</v>
       </c>
@@ -4467,7 +4877,7 @@
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B79" s="77"/>
+      <c r="B79" s="73"/>
       <c r="C79" s="13" t="s">
         <v>210</v>
       </c>
@@ -4494,7 +4904,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B80" s="77"/>
+      <c r="B80" s="73"/>
       <c r="C80" s="13" t="s">
         <v>214</v>
       </c>
@@ -4517,7 +4927,7 @@
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B81" s="77"/>
+      <c r="B81" s="73"/>
       <c r="C81" s="15" t="s">
         <v>221</v>
       </c>
@@ -4540,7 +4950,7 @@
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B82" s="77"/>
+      <c r="B82" s="73"/>
       <c r="C82" s="13" t="s">
         <v>223</v>
       </c>
@@ -4563,7 +4973,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B83" s="77"/>
+      <c r="B83" s="73"/>
       <c r="C83" s="13" t="s">
         <v>224</v>
       </c>
@@ -4584,7 +4994,7 @@
       <c r="J83" s="1"/>
     </row>
     <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B84" s="77"/>
+      <c r="B84" s="73"/>
       <c r="C84" s="13" t="s">
         <v>227</v>
       </c>
@@ -4605,7 +5015,7 @@
       <c r="J84" s="1"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="77"/>
+      <c r="B85" s="73"/>
       <c r="C85" s="13"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -4616,7 +5026,7 @@
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="77"/>
+      <c r="B86" s="73"/>
       <c r="C86" s="13"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4627,7 +5037,7 @@
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B87" s="77"/>
+      <c r="B87" s="73"/>
       <c r="C87" s="13"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4638,7 +5048,7 @@
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B88" s="77"/>
+      <c r="B88" s="73"/>
       <c r="C88" s="13"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4649,7 +5059,7 @@
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="77"/>
+      <c r="B89" s="73"/>
       <c r="C89" s="13"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4660,7 +5070,7 @@
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="77"/>
+      <c r="B90" s="73"/>
       <c r="C90" s="13"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -4671,7 +5081,7 @@
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B91" s="77"/>
+      <c r="B91" s="73"/>
       <c r="C91" s="13"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4682,7 +5092,7 @@
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B92" s="77"/>
+      <c r="B92" s="73"/>
       <c r="C92" s="13"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4693,7 +5103,7 @@
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" s="77"/>
+      <c r="B93" s="73"/>
       <c r="C93" s="13"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4704,7 +5114,7 @@
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="77"/>
+      <c r="B94" s="73"/>
       <c r="C94" s="13"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4715,7 +5125,7 @@
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="77"/>
+      <c r="B95" s="73"/>
       <c r="C95" s="13"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -4726,7 +5136,7 @@
       <c r="J95" s="1"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="77"/>
+      <c r="B96" s="73"/>
       <c r="C96" s="13"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4737,7 +5147,7 @@
       <c r="J96" s="1"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B97" s="77"/>
+      <c r="B97" s="73"/>
       <c r="C97" s="13"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4748,7 +5158,7 @@
       <c r="J97" s="1"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" s="77"/>
+      <c r="B98" s="73"/>
       <c r="C98" s="13"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4759,7 +5169,7 @@
       <c r="J98" s="1"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="77"/>
+      <c r="B99" s="73"/>
       <c r="C99" s="13"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4770,7 +5180,7 @@
       <c r="J99" s="1"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B100" s="77"/>
+      <c r="B100" s="73"/>
       <c r="C100" s="13"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4781,7 +5191,7 @@
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B101" s="77"/>
+      <c r="B101" s="73"/>
       <c r="C101" s="13"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4792,7 +5202,7 @@
       <c r="J101" s="1"/>
     </row>
     <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="78"/>
+      <c r="B102" s="74"/>
       <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4832,316 +5242,720 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="111"/>
+    <col min="8" max="8" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-    </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="89" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+    </row>
+    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54"/>
+      <c r="B2" s="107" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="55" t="s">
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="38"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-    </row>
-    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
-      <c r="B4" s="86" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="39"/>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="54"/>
+      <c r="B4" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="112" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="114" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="60">
+      <c r="F4" s="115">
         <v>0.36480000000000001</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="114" t="s">
         <v>234</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="116" t="s">
+        <v>256</v>
+      </c>
+      <c r="I4" s="54"/>
+      <c r="J4" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="40"/>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="54"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>275</v>
+      </c>
+      <c r="F5" s="61"/>
+      <c r="G5" s="60">
+        <v>30</v>
+      </c>
+      <c r="H5" s="62"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="41"/>
+    </row>
+    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="112" t="s">
         <v>236</v>
       </c>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-    </row>
-    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="53"/>
-      <c r="B5" s="87"/>
-      <c r="C5" s="71" t="s">
+      <c r="D6" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="114" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="115">
+        <v>0.65839999999999999</v>
+      </c>
+      <c r="G6" s="114" t="s">
+        <v>247</v>
+      </c>
+      <c r="H6" s="116" t="s">
+        <v>257</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+    </row>
+    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="112" t="s">
         <v>237</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D7" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E7" s="114" t="s">
+        <v>255</v>
+      </c>
+      <c r="F7" s="115">
+        <v>0.65269999999999995</v>
+      </c>
+      <c r="G7" s="114" t="s">
+        <v>248</v>
+      </c>
+      <c r="H7" s="116" t="s">
+        <v>257</v>
+      </c>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+    </row>
+    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="120" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" s="121" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="122" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="123"/>
+      <c r="G8" s="122">
+        <v>30</v>
+      </c>
+      <c r="H8" s="124"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+    </row>
+    <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" s="65"/>
+      <c r="G9" s="63">
+        <v>30</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="54"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="54"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="54"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="54"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="54"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="54"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="54"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="54"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="54"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="54"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="54"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="54"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+    </row>
+    <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="54"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+    </row>
+    <row r="23" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="85" t="s">
         <v>238</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-    </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="71" t="s">
+      <c r="C23" s="50" t="s">
+        <v>240</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F23" s="6">
+        <v>47.49</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="86"/>
+      <c r="C24" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="F24" s="2">
+        <v>47.49</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="86"/>
+      <c r="C25" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F25" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="87"/>
+      <c r="C26" s="110" t="s">
+        <v>243</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" s="16">
+        <v>6.7</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="53"/>
+    </row>
+    <row r="27" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="62" t="s">
-        <v>240</v>
-      </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="53"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="53"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="53"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
-      <c r="B20" s="87"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-    </row>
-    <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
+      <c r="E27" s="118" t="s">
+        <v>250</v>
+      </c>
+      <c r="F27" s="119">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="G27" s="118">
+        <v>50</v>
+      </c>
+      <c r="H27" s="118" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="83"/>
+      <c r="C28" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D28" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="125" t="s">
+        <v>274</v>
+      </c>
+      <c r="F28" s="126"/>
+      <c r="G28" s="125"/>
+      <c r="H28" s="125"/>
+    </row>
+    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B29" s="83"/>
+      <c r="C29" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="D29" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="125" t="s">
+        <v>280</v>
+      </c>
+      <c r="F29" s="126"/>
+      <c r="G29" s="125"/>
+      <c r="H29" s="125"/>
+    </row>
+    <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B30" s="83"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B31" s="83"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="84"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="82" t="s">
+        <v>251</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="D33" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="125" t="s">
+        <v>283</v>
+      </c>
+      <c r="F33" s="126"/>
+      <c r="G33" s="125"/>
+      <c r="H33" s="125"/>
+    </row>
+    <row r="34" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B34" s="83"/>
+      <c r="C34" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" s="125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="125" t="s">
+        <v>285</v>
+      </c>
+      <c r="F34" s="126"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="125"/>
+    </row>
+    <row r="35" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B35" s="83"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B36" s="83"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="83"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="83"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="83"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="84"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="B4:B22"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B63F8CF-F012-4149-9CDA-3AB5262AB13A}">
+  <dimension ref="B3:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="111" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="102" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="95"/>
+    </row>
+    <row r="5" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="103"/>
+      <c r="C5" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="99" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="100" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="96" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="97" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="D10" s="99" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="B11" s="104" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="97" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="97" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="101" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="106" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="106" t="s">
+        <v>272</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[IMP] Sending batch 6
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF917E2-74F3-DF4A-ADC3-A6C66342EF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5A4A98-8E06-124A-970F-7828922050E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="15260" yWindow="760" windowWidth="14140" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="334">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -141,9 +141,6 @@
     <t>20/30</t>
   </si>
   <si>
-    <t>With model 27</t>
-  </si>
-  <si>
     <t>25% of training data, bz 128</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
     <t>38/48</t>
   </si>
   <si>
-    <t>With model 35</t>
-  </si>
-  <si>
     <t>35/45</t>
   </si>
   <si>
@@ -697,9 +691,6 @@
   </si>
   <si>
     <t>find in r.2.6</t>
-  </si>
-  <si>
-    <t>r2.6</t>
   </si>
   <si>
     <t>N/A</t>
@@ -915,6 +906,9 @@
     <t>p9</t>
   </si>
   <si>
+    <t>p10</t>
+  </si>
+  <si>
     <t>ZoomViT (pretrained), correct (config tables) but no color jitter</t>
   </si>
   <si>
@@ -928,6 +922,153 @@
   </si>
   <si>
     <t>Brainit (pretrained), correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>43/50</t>
+  </si>
+  <si>
+    <t>42/50</t>
+  </si>
+  <si>
+    <t>40/50</t>
+  </si>
+  <si>
+    <t>Overfitting</t>
+  </si>
+  <si>
+    <t>With model 27. VAL NOT KEPT CONST</t>
+  </si>
+  <si>
+    <t>VAL NOT KEPT CONST</t>
+  </si>
+  <si>
+    <t>With model 35. VAL NOT KEPT CONST</t>
+  </si>
+  <si>
+    <t>r2.6. VAL NOT KEPT CONST</t>
+  </si>
+  <si>
+    <t>Val not downsampled</t>
+  </si>
+  <si>
+    <t>p11</t>
+  </si>
+  <si>
+    <t>p12</t>
+  </si>
+  <si>
+    <t>p13</t>
+  </si>
+  <si>
+    <t>p14</t>
+  </si>
+  <si>
+    <t>p15</t>
+  </si>
+  <si>
+    <t>p16</t>
+  </si>
+  <si>
+    <t>p17</t>
+  </si>
+  <si>
+    <t>p18</t>
+  </si>
+  <si>
+    <t>10% per class - p5</t>
+  </si>
+  <si>
+    <t>25% per class - p5</t>
+  </si>
+  <si>
+    <t>50% per class - p5</t>
+  </si>
+  <si>
+    <t>10% per class - p7</t>
+  </si>
+  <si>
+    <t>25% per class - p7</t>
+  </si>
+  <si>
+    <t>50% per class - p7</t>
+  </si>
+  <si>
+    <t>10% per class - p9</t>
+  </si>
+  <si>
+    <t>25% per class - p9</t>
+  </si>
+  <si>
+    <t>50% per class - p9</t>
+  </si>
+  <si>
+    <t>p19</t>
+  </si>
+  <si>
+    <t>p20</t>
+  </si>
+  <si>
+    <t>p21</t>
+  </si>
+  <si>
+    <t>p22</t>
+  </si>
+  <si>
+    <t>p23</t>
+  </si>
+  <si>
+    <t>p24</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p26</t>
+  </si>
+  <si>
+    <t>p27</t>
+  </si>
+  <si>
+    <t>p28</t>
+  </si>
+  <si>
+    <t>p29</t>
+  </si>
+  <si>
+    <t>p30</t>
+  </si>
+  <si>
+    <t>p31</t>
+  </si>
+  <si>
+    <t>4--30</t>
+  </si>
+  <si>
+    <t>45.17%%</t>
+  </si>
+  <si>
+    <t>26/30</t>
+  </si>
+  <si>
+    <t>37/50</t>
+  </si>
+  <si>
+    <t>35/50</t>
+  </si>
+  <si>
+    <t>4--50</t>
+  </si>
+  <si>
+    <t>14/30</t>
+  </si>
+  <si>
+    <t>17/30</t>
+  </si>
+  <si>
+    <t>28/30</t>
+  </si>
+  <si>
+    <t>44/50</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="51">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1395,8 +1536,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="56">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -1813,17 +1972,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -2148,7 +2296,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2291,19 +2439,19 @@
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2318,112 +2466,221 @@
     <xf numFmtId="0" fontId="22" fillId="46" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="46" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="46" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="46" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="46" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="46" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="47" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="48" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="48" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="48" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="49" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="49" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="50" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="50" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="50" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="51" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="51" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="51" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="51" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="47" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="47" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="48" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="47" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="47" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="48" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="48" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2432,98 +2689,58 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="23" fillId="49" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="49" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="49" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="49" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="50" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="50" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="50" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="50" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="52" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="52" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="52" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="52" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="53" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="53" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="53" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="53" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="53" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="22" fillId="51" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2930,8 +3147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N102"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N4"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2943,7 +3160,7 @@
     <col min="6" max="6" width="17" style="37" customWidth="1"/>
     <col min="7" max="8" width="10.83203125" style="36"/>
     <col min="9" max="9" width="17.5" style="36" customWidth="1"/>
-    <col min="10" max="10" width="29.33203125" style="36" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" style="36" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="36"/>
   </cols>
   <sheetData>
@@ -2952,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N1" s="38"/>
     </row>
@@ -3005,16 +3222,16 @@
       <c r="N4" s="41"/>
     </row>
     <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="75" t="s">
-        <v>138</v>
+      <c r="C5" s="118" t="s">
+        <v>136</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="118" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6">
@@ -3038,12 +3255,12 @@
       <c r="N5" s="42"/>
     </row>
     <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="78"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="119"/>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="76"/>
+      <c r="E6" s="119"/>
       <c r="F6" s="2">
         <v>0.83630000000000004</v>
       </c>
@@ -3065,9 +3282,9 @@
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>30</v>
@@ -3096,11 +3313,11 @@
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="115" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>30</v>
@@ -3129,9 +3346,9 @@
       <c r="N8" s="45"/>
     </row>
     <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="74"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>30</v>
@@ -3160,11 +3377,11 @@
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="115" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>30</v>
@@ -3191,9 +3408,9 @@
       <c r="N10" s="47"/>
     </row>
     <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="73"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
@@ -3216,9 +3433,9 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="73"/>
+      <c r="B12" s="116"/>
       <c r="C12" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
@@ -3241,9 +3458,9 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="73"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>30</v>
@@ -3266,9 +3483,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="73"/>
+      <c r="B14" s="116"/>
       <c r="C14" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>36</v>
@@ -3289,25 +3506,25 @@
         <v>35</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>39</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="73"/>
+      <c r="B15" s="116"/>
       <c r="C15" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2">
         <v>0.84379999999999999</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>34</v>
@@ -3315,24 +3532,26 @@
       <c r="I15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="8"/>
+      <c r="J15" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="73"/>
+      <c r="B16" s="116"/>
       <c r="C16" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2">
         <v>0.88500000000000001</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>34</v>
@@ -3340,24 +3559,26 @@
       <c r="I16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="8"/>
+      <c r="J16" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="73"/>
+      <c r="B17" s="116"/>
       <c r="C17" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="2">
         <v>0.26769999999999999</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>34</v>
@@ -3365,24 +3586,26 @@
       <c r="I17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="J17" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="73"/>
+      <c r="B18" s="116"/>
       <c r="C18" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="2">
         <v>0.47689999999999999</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>34</v>
@@ -3390,24 +3613,26 @@
       <c r="I18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J18" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="73"/>
+      <c r="B19" s="116"/>
       <c r="C19" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F19" s="2">
         <v>0.4521</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>34</v>
@@ -3418,21 +3643,21 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="73"/>
+      <c r="B20" s="116"/>
       <c r="C20" s="26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2">
         <v>0.42209999999999998</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>34</v>
@@ -3443,21 +3668,21 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="73"/>
+      <c r="B21" s="116"/>
       <c r="C21" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" s="2">
         <v>0.39529999999999998</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>34</v>
@@ -3468,21 +3693,21 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="73"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="2">
         <v>0.34429999999999999</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3493,21 +3718,21 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="73"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F23" s="2">
         <v>0.32550000000000001</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3518,21 +3743,21 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="73"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>34</v>
@@ -3543,21 +3768,21 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="73"/>
+      <c r="B25" s="116"/>
       <c r="C25" s="27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>34</v>
@@ -3568,21 +3793,21 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="73"/>
+      <c r="B26" s="116"/>
       <c r="C26" s="27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>34</v>
@@ -3593,21 +3818,21 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="73"/>
+      <c r="B27" s="116"/>
       <c r="C27" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>34</v>
@@ -3618,21 +3843,21 @@
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="73"/>
+      <c r="B28" s="116"/>
       <c r="C28" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>34</v>
@@ -3643,21 +3868,21 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="73"/>
+      <c r="B29" s="116"/>
       <c r="C29" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3668,21 +3893,21 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="74"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F30" s="10">
         <v>0.85589999999999999</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>34</v>
@@ -3693,17 +3918,17 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="72" t="s">
-        <v>69</v>
+      <c r="B31" s="115" t="s">
+        <v>68</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F31" s="6">
         <v>0.91569999999999996</v>
@@ -3718,25 +3943,25 @@
         <v>17</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="73"/>
+      <c r="B32" s="116"/>
       <c r="C32" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="2">
         <v>0.89139999999999997</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>34</v>
@@ -3747,15 +3972,15 @@
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="73"/>
+      <c r="B33" s="116"/>
       <c r="C33" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F33" s="2">
         <v>0.89610000000000001</v>
@@ -3767,20 +3992,20 @@
         <v>16</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J33" s="8"/>
     </row>
     <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="73"/>
+      <c r="B34" s="116"/>
       <c r="C34" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34" s="2">
         <v>0.91479999999999995</v>
@@ -3792,20 +4017,20 @@
         <v>16</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="73"/>
+      <c r="B35" s="116"/>
       <c r="C35" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F35" s="2">
         <v>0.91259999999999997</v>
@@ -3817,20 +4042,20 @@
         <v>16</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="73"/>
+      <c r="B36" s="116"/>
       <c r="C36" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F36" s="2">
         <v>0.90820000000000001</v>
@@ -3842,20 +4067,20 @@
         <v>16</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="73"/>
+      <c r="B37" s="116"/>
       <c r="C37" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F37" s="2">
         <v>0.89249999999999996</v>
@@ -3867,22 +4092,22 @@
         <v>16</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="73"/>
+      <c r="B38" s="116"/>
       <c r="C38" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F38" s="2">
         <v>0.9042</v>
@@ -3894,28 +4119,28 @@
         <v>16</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="73"/>
+      <c r="B39" s="116"/>
       <c r="C39" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" s="2">
         <v>0.91830000000000001</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>34</v>
@@ -3926,21 +4151,21 @@
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="73"/>
+      <c r="B40" s="116"/>
       <c r="C40" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F40" s="2">
         <v>0.9204</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>34</v>
@@ -3949,25 +4174,25 @@
         <v>35</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="73"/>
+      <c r="B41" s="116"/>
       <c r="C41" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F41" s="2">
         <v>0.91979999999999995</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>34</v>
@@ -3978,21 +4203,21 @@
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="73"/>
+      <c r="B42" s="116"/>
       <c r="C42" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F42" s="2">
         <v>0.91820000000000002</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>34</v>
@@ -4003,21 +4228,21 @@
       <c r="J42" s="8"/>
     </row>
     <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="73"/>
+      <c r="B43" s="116"/>
       <c r="C43" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F43" s="2">
         <v>0.90639999999999998</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>34</v>
@@ -4028,21 +4253,21 @@
       <c r="J43" s="8"/>
     </row>
     <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="73"/>
+      <c r="B44" s="116"/>
       <c r="C44" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F44" s="2">
         <v>0.91010000000000002</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>34</v>
@@ -4053,21 +4278,21 @@
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="73"/>
+      <c r="B45" s="116"/>
       <c r="C45" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F45" s="2">
         <v>0.92069999999999996</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>34</v>
@@ -4078,21 +4303,21 @@
       <c r="J45" s="8"/>
     </row>
     <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="73"/>
+      <c r="B46" s="116"/>
       <c r="C46" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F46" s="2">
         <v>0.88849999999999996</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>34</v>
@@ -4103,21 +4328,21 @@
       <c r="J46" s="8"/>
     </row>
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="73"/>
+      <c r="B47" s="116"/>
       <c r="C47" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F47" s="2">
         <v>0.92730000000000001</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>34</v>
@@ -4126,25 +4351,25 @@
         <v>35</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B48" s="73"/>
+      <c r="B48" s="116"/>
       <c r="C48" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F48" s="2">
         <v>0.92849999999999999</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>34</v>
@@ -4155,21 +4380,21 @@
       <c r="J48" s="8"/>
     </row>
     <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="73"/>
+      <c r="B49" s="116"/>
       <c r="C49" s="30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F49" s="2">
         <v>0.91579999999999995</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>34</v>
@@ -4178,32 +4403,32 @@
       <c r="J49" s="8"/>
     </row>
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="73"/>
+      <c r="B50" s="116"/>
       <c r="C50" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F50" s="2">
         <v>0.91810000000000003</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="73"/>
+      <c r="B51" s="116"/>
       <c r="C51" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>36</v>
@@ -4215,7 +4440,7 @@
         <v>0.69769999999999999</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>34</v>
@@ -4223,26 +4448,26 @@
       <c r="I51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J51" s="80" t="s">
-        <v>109</v>
+      <c r="J51" s="74" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="73"/>
+      <c r="B52" s="116"/>
       <c r="C52" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F52" s="2">
         <v>0.84519999999999995</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>34</v>
@@ -4250,24 +4475,26 @@
       <c r="I52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="81"/>
+      <c r="J52" s="74" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="73"/>
+      <c r="B53" s="116"/>
       <c r="C53" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F53" s="2">
         <v>0.88180000000000003</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>34</v>
@@ -4275,24 +4502,26 @@
       <c r="I53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="81"/>
+      <c r="J53" s="74" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="73"/>
+      <c r="B54" s="116"/>
       <c r="C54" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F54" s="2">
         <v>0.19670000000000001</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>34</v>
@@ -4300,24 +4529,26 @@
       <c r="I54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J54" s="81"/>
+      <c r="J54" s="74" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="73"/>
+      <c r="B55" s="116"/>
       <c r="C55" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F55" s="2">
         <v>0.31030000000000002</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>34</v>
@@ -4325,299 +4556,303 @@
       <c r="I55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J55" s="81"/>
+      <c r="J55" s="74" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="73"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F56" s="2">
         <v>0.50349999999999995</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J56" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J56" s="111" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="73"/>
+      <c r="B57" s="116"/>
       <c r="C57" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F57" s="2">
         <v>0.45710000000000001</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J57" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J57" s="111"/>
     </row>
     <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B58" s="73"/>
+      <c r="B58" s="116"/>
       <c r="C58" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F58" s="2">
         <v>0.41149999999999998</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J58" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J58" s="111"/>
     </row>
     <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="73"/>
+      <c r="B59" s="116"/>
       <c r="C59" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F59" s="2">
         <v>0.34549999999999997</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J59" s="111"/>
+    </row>
+    <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" s="116"/>
+      <c r="C60" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="J59" s="81"/>
-    </row>
-    <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="73"/>
-      <c r="C60" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J60" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J60" s="111"/>
     </row>
     <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B61" s="73"/>
+      <c r="B61" s="116"/>
       <c r="C61" s="27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J61" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J61" s="111"/>
     </row>
     <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B62" s="73"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="27" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J62" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J62" s="111"/>
     </row>
     <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B63" s="73"/>
+      <c r="B63" s="116"/>
       <c r="C63" s="27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J63" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J63" s="111"/>
     </row>
     <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="73"/>
+      <c r="B64" s="116"/>
       <c r="C64" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J64" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J64" s="111"/>
     </row>
     <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B65" s="73"/>
+      <c r="B65" s="116"/>
       <c r="C65" s="28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J65" s="81"/>
-    </row>
-    <row r="66" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B66" s="73"/>
+        <v>111</v>
+      </c>
+      <c r="J65" s="111"/>
+    </row>
+    <row r="66" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="116"/>
       <c r="C66" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J66" s="81"/>
-    </row>
-    <row r="67" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="73"/>
+        <v>111</v>
+      </c>
+      <c r="J66" s="111"/>
+    </row>
+    <row r="67" spans="2:10" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="116"/>
       <c r="C67" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F67" s="2">
         <v>0.92459999999999998</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>34</v>
@@ -4625,24 +4860,24 @@
       <c r="I67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="81"/>
-    </row>
-    <row r="68" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="73"/>
+      <c r="J67" s="111"/>
+    </row>
+    <row r="68" spans="2:10" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="116"/>
       <c r="C68" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F68" s="2">
         <v>0.91800000000000004</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>34</v>
@@ -4650,49 +4885,49 @@
       <c r="I68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J68" s="81"/>
-    </row>
-    <row r="69" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="73"/>
+      <c r="J68" s="111"/>
+    </row>
+    <row r="69" spans="2:10" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="116"/>
       <c r="C69" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F69" s="2">
         <v>0.92310000000000003</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J69" s="81"/>
+        <v>111</v>
+      </c>
+      <c r="J69" s="111"/>
     </row>
     <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="74"/>
+      <c r="B70" s="117"/>
       <c r="C70" s="49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F70" s="16">
         <v>0.90859999999999996</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>34</v>
@@ -4700,90 +4935,90 @@
       <c r="I70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J70" s="81"/>
-    </row>
-    <row r="71" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="69" t="s">
-        <v>133</v>
+      <c r="J70" s="111"/>
+    </row>
+    <row r="71" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="112" t="s">
+        <v>131</v>
       </c>
       <c r="C71" s="50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F71" s="6">
         <v>0.92759999999999998</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="J71" s="7"/>
-    </row>
-    <row r="72" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="70"/>
+      <c r="J71" s="111"/>
+    </row>
+    <row r="72" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="113"/>
       <c r="C72" s="51" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F72" s="2">
         <v>0.92759999999999998</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="8"/>
-    </row>
-    <row r="73" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="70"/>
+      <c r="J72" s="111"/>
+    </row>
+    <row r="73" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="113"/>
       <c r="C73" s="51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="8"/>
-    </row>
-    <row r="74" spans="2:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="71"/>
+      <c r="J73" s="111"/>
+    </row>
+    <row r="74" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="114"/>
       <c r="C74" s="52" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F74" s="10"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
-      <c r="J74" s="11"/>
+      <c r="J74" s="111"/>
     </row>
     <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="72" t="s">
-        <v>131</v>
+      <c r="B75" s="115" t="s">
+        <v>129</v>
       </c>
       <c r="C75" s="48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F75" s="31">
         <v>0.84760000000000002</v>
@@ -4795,20 +5030,20 @@
         <v>34</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J75" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="J75" s="111"/>
     </row>
     <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B76" s="73"/>
+      <c r="B76" s="116"/>
       <c r="C76" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F76" s="2">
         <v>0.80649999999999999</v>
@@ -4820,20 +5055,20 @@
         <v>34</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B77" s="73"/>
+      <c r="B77" s="116"/>
       <c r="C77" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F77" s="2">
         <v>0.84240000000000004</v>
@@ -4845,28 +5080,28 @@
         <v>34</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B78" s="73"/>
+      <c r="B78" s="116"/>
       <c r="C78" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F78" s="2">
         <v>0.84250000000000003</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>34</v>
@@ -4877,21 +5112,21 @@
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B79" s="73"/>
+      <c r="B79" s="116"/>
       <c r="C79" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F79" s="2">
         <v>0.85909999999999997</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>34</v>
@@ -4900,19 +5135,19 @@
         <v>35</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B80" s="73"/>
+      <c r="B80" s="116"/>
       <c r="C80" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F80" s="2">
         <v>0.84889999999999999</v>
@@ -4922,20 +5157,20 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B81" s="73"/>
+      <c r="B81" s="116"/>
       <c r="C81" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F81" s="16">
         <v>0.91720000000000002</v>
@@ -4945,20 +5180,20 @@
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B82" s="73"/>
+      <c r="B82" s="116"/>
       <c r="C82" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F82" s="2">
         <v>0.87190000000000001</v>
@@ -4969,19 +5204,19 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
-        <v>225</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B83" s="73"/>
+      <c r="B83" s="116"/>
       <c r="C83" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F83" s="2">
         <v>0.52159999999999995</v>
@@ -4991,18 +5226,20 @@
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
+      <c r="J83" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B84" s="73"/>
+      <c r="B84" s="116"/>
       <c r="C84" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="E84" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F84" s="2">
         <v>0.6804</v>
@@ -5012,10 +5249,12 @@
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
+      <c r="J84" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="73"/>
+      <c r="B85" s="116"/>
       <c r="C85" s="13"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -5026,7 +5265,7 @@
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="73"/>
+      <c r="B86" s="116"/>
       <c r="C86" s="13"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -5037,7 +5276,7 @@
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B87" s="73"/>
+      <c r="B87" s="116"/>
       <c r="C87" s="13"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -5048,7 +5287,7 @@
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B88" s="73"/>
+      <c r="B88" s="116"/>
       <c r="C88" s="13"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -5059,7 +5298,7 @@
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="73"/>
+      <c r="B89" s="116"/>
       <c r="C89" s="13"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -5070,7 +5309,7 @@
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="73"/>
+      <c r="B90" s="116"/>
       <c r="C90" s="13"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -5081,7 +5320,7 @@
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B91" s="73"/>
+      <c r="B91" s="116"/>
       <c r="C91" s="13"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -5092,7 +5331,7 @@
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B92" s="73"/>
+      <c r="B92" s="116"/>
       <c r="C92" s="13"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -5103,7 +5342,7 @@
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" s="73"/>
+      <c r="B93" s="116"/>
       <c r="C93" s="13"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -5114,7 +5353,7 @@
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="73"/>
+      <c r="B94" s="116"/>
       <c r="C94" s="13"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -5125,7 +5364,7 @@
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="73"/>
+      <c r="B95" s="116"/>
       <c r="C95" s="13"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -5136,7 +5375,7 @@
       <c r="J95" s="1"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="73"/>
+      <c r="B96" s="116"/>
       <c r="C96" s="13"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -5147,7 +5386,7 @@
       <c r="J96" s="1"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B97" s="73"/>
+      <c r="B97" s="116"/>
       <c r="C97" s="13"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -5158,7 +5397,7 @@
       <c r="J97" s="1"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" s="73"/>
+      <c r="B98" s="116"/>
       <c r="C98" s="13"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -5169,7 +5408,7 @@
       <c r="J98" s="1"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="73"/>
+      <c r="B99" s="116"/>
       <c r="C99" s="13"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -5180,7 +5419,7 @@
       <c r="J99" s="1"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B100" s="73"/>
+      <c r="B100" s="116"/>
       <c r="C100" s="13"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -5191,7 +5430,7 @@
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B101" s="73"/>
+      <c r="B101" s="116"/>
       <c r="C101" s="13"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -5202,7 +5441,7 @@
       <c r="J101" s="1"/>
     </row>
     <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="74"/>
+      <c r="B102" s="117"/>
       <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -5214,7 +5453,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="J51:J70"/>
+    <mergeCell ref="J56:J75"/>
     <mergeCell ref="B71:B74"/>
     <mergeCell ref="B75:B102"/>
     <mergeCell ref="E5:E6"/>
@@ -5242,16 +5481,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="111"/>
+    <col min="6" max="6" width="10.83203125" style="88"/>
     <col min="8" max="8" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5269,18 +5508,18 @@
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54"/>
-      <c r="B2" s="107" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
+      <c r="B2" s="126" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="126"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
       <c r="I2" s="54"/>
       <c r="J2" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K2" s="38"/>
     </row>
@@ -5315,26 +5554,26 @@
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="54"/>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="89" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="91" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="113" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="114" t="s">
-        <v>235</v>
-      </c>
-      <c r="F4" s="115">
+      <c r="F4" s="92">
         <v>0.36480000000000001</v>
       </c>
-      <c r="G4" s="114" t="s">
-        <v>234</v>
-      </c>
-      <c r="H4" s="116" t="s">
-        <v>256</v>
+      <c r="G4" s="91" t="s">
+        <v>231</v>
+      </c>
+      <c r="H4" s="93" t="s">
+        <v>253</v>
       </c>
       <c r="I4" s="54"/>
       <c r="J4" s="36" t="s">
@@ -5344,17 +5583,21 @@
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="54"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="68"/>
+      <c r="B5" s="124"/>
+      <c r="C5" s="68" t="s">
+        <v>320</v>
+      </c>
       <c r="D5" s="67" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>275</v>
-      </c>
-      <c r="F5" s="61"/>
-      <c r="G5" s="60">
-        <v>30</v>
+        <v>272</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>326</v>
       </c>
       <c r="H5" s="62"/>
       <c r="I5" s="54"/>
@@ -5365,165 +5608,239 @@
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="54"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="112" t="s">
-        <v>236</v>
-      </c>
-      <c r="D6" s="117" t="s">
+      <c r="B6" s="124"/>
+      <c r="C6" s="89" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="114" t="s">
+      <c r="E6" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6" s="92">
+        <v>0.65839999999999999</v>
+      </c>
+      <c r="G6" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="H6" s="93" t="s">
         <v>254</v>
-      </c>
-      <c r="F6" s="115">
-        <v>0.65839999999999999</v>
-      </c>
-      <c r="G6" s="114" t="s">
-        <v>247</v>
-      </c>
-      <c r="H6" s="116" t="s">
-        <v>257</v>
       </c>
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="54"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="112" t="s">
-        <v>237</v>
-      </c>
-      <c r="D7" s="117" t="s">
+      <c r="B7" s="124"/>
+      <c r="C7" s="89" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="114" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="115">
+      <c r="E7" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="F7" s="92">
         <v>0.65269999999999995</v>
       </c>
-      <c r="G7" s="114" t="s">
-        <v>248</v>
-      </c>
-      <c r="H7" s="116" t="s">
-        <v>257</v>
+      <c r="G7" s="91" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="93" t="s">
+        <v>254</v>
       </c>
       <c r="I7" s="54"/>
       <c r="J7" s="54"/>
     </row>
     <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="120" t="s">
-        <v>252</v>
-      </c>
-      <c r="D8" s="121" t="s">
+      <c r="B8" s="124"/>
+      <c r="C8" s="97" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="122" t="s">
-        <v>273</v>
-      </c>
-      <c r="F8" s="123"/>
-      <c r="G8" s="122">
-        <v>30</v>
-      </c>
-      <c r="H8" s="124"/>
+      <c r="E8" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="F8" s="100">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="G8" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="101" t="s">
+        <v>288</v>
+      </c>
       <c r="I8" s="54"/>
       <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="64" t="s">
+      <c r="B9" s="124"/>
+      <c r="C9" s="141" t="s">
+        <v>321</v>
+      </c>
+      <c r="D9" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="63" t="s">
-        <v>276</v>
-      </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="63">
-        <v>30</v>
-      </c>
-      <c r="H9" s="66"/>
+      <c r="E9" s="143" t="s">
+        <v>273</v>
+      </c>
+      <c r="F9" s="144">
+        <v>0.74019999999999997</v>
+      </c>
+      <c r="G9" s="143" t="s">
+        <v>332</v>
+      </c>
+      <c r="H9" s="145"/>
       <c r="I9" s="54"/>
       <c r="J9" s="54"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="66"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="104" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="106" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" s="107">
+        <v>0.46329999999999999</v>
+      </c>
+      <c r="G10" s="148" t="s">
+        <v>324</v>
+      </c>
+      <c r="H10" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="66"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="104" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="106" t="s">
+        <v>303</v>
+      </c>
+      <c r="F11" s="107">
+        <v>0.62519999999999998</v>
+      </c>
+      <c r="G11" s="106" t="s">
+        <v>330</v>
+      </c>
+      <c r="H11" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="54"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="66"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="104" t="s">
+        <v>295</v>
+      </c>
+      <c r="D12" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="106" t="s">
+        <v>304</v>
+      </c>
+      <c r="F12" s="107">
+        <v>0.69059999999999999</v>
+      </c>
+      <c r="G12" s="106" t="s">
+        <v>331</v>
+      </c>
+      <c r="H12" s="108" t="s">
+        <v>293</v>
+      </c>
       <c r="I12" s="54"/>
       <c r="J12" s="54"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="66"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="134" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="137">
+        <v>0.13159999999999999</v>
+      </c>
+      <c r="G13" s="138" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="139"/>
       <c r="I13" s="54"/>
       <c r="J13" s="54"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="66"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="134" t="s">
+        <v>312</v>
+      </c>
+      <c r="D14" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="136" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="137">
+        <v>5.57E-2</v>
+      </c>
+      <c r="G14" s="138" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="139"/>
       <c r="I14" s="54"/>
       <c r="J14" s="54"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="66"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="134" t="s">
+        <v>313</v>
+      </c>
+      <c r="D15" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="137">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="G15" s="138" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="139"/>
       <c r="I15" s="54"/>
       <c r="J15" s="54"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
-      <c r="B16" s="83"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="68"/>
       <c r="D16" s="64"/>
       <c r="E16" s="63"/>
@@ -5535,7 +5852,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
-      <c r="B17" s="83"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="68"/>
       <c r="D17" s="64"/>
       <c r="E17" s="63"/>
@@ -5547,7 +5864,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
-      <c r="B18" s="83"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="68"/>
       <c r="D18" s="64"/>
       <c r="E18" s="63"/>
@@ -5559,7 +5876,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
-      <c r="B19" s="83"/>
+      <c r="B19" s="124"/>
       <c r="C19" s="68"/>
       <c r="D19" s="64"/>
       <c r="E19" s="63"/>
@@ -5571,7 +5888,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
-      <c r="B20" s="83"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="68"/>
       <c r="D20" s="64"/>
       <c r="E20" s="63"/>
@@ -5583,7 +5900,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
-      <c r="B21" s="83"/>
+      <c r="B21" s="124"/>
       <c r="C21" s="68"/>
       <c r="D21" s="64"/>
       <c r="E21" s="63"/>
@@ -5595,26 +5912,26 @@
     </row>
     <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="54"/>
-      <c r="B22" s="84"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="92"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="54"/>
       <c r="J22" s="54"/>
     </row>
     <row r="23" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="85" t="s">
-        <v>238</v>
+      <c r="B23" s="127" t="s">
+        <v>235</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F23" s="6">
         <v>47.49</v>
@@ -5623,13 +5940,13 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="86"/>
+      <c r="B24" s="128"/>
       <c r="C24" s="51" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F24" s="2">
         <v>47.49</v>
@@ -5638,13 +5955,13 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="86"/>
+      <c r="B25" s="128"/>
       <c r="C25" s="51" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F25" s="2">
         <v>6.7</v>
@@ -5653,13 +5970,13 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="87"/>
-      <c r="C26" s="110" t="s">
-        <v>243</v>
+      <c r="B26" s="129"/>
+      <c r="C26" s="87" t="s">
+        <v>240</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F26" s="16">
         <v>6.7</v>
@@ -5668,164 +5985,224 @@
       <c r="H26" s="53"/>
     </row>
     <row r="27" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="82" t="s">
-        <v>134</v>
+      <c r="B27" s="123" t="s">
+        <v>132</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="D27" s="118" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="118" t="s">
+      <c r="E27" s="95" t="s">
+        <v>247</v>
+      </c>
+      <c r="F27" s="96">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="G27" s="95">
+        <v>50</v>
+      </c>
+      <c r="H27" s="95" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="124"/>
+      <c r="C28" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="F27" s="119">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="G27" s="118">
-        <v>50</v>
-      </c>
-      <c r="H27" s="118" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="83"/>
-      <c r="C28" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="D28" s="125" t="s">
+      <c r="D28" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="125" t="s">
+      <c r="E28" s="102" t="s">
+        <v>271</v>
+      </c>
+      <c r="F28" s="103">
+        <v>0.52239999999999998</v>
+      </c>
+      <c r="G28" s="102" t="s">
+        <v>285</v>
+      </c>
+      <c r="H28" s="102" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B29" s="124"/>
+      <c r="C29" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="F28" s="126"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-    </row>
-    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B29" s="83"/>
-      <c r="C29" s="22" t="s">
+      <c r="D29" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="102" t="s">
         <v>277</v>
       </c>
-      <c r="D29" s="125" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="125" t="s">
-        <v>280</v>
-      </c>
-      <c r="F29" s="126"/>
-      <c r="G29" s="125"/>
-      <c r="H29" s="125"/>
+      <c r="F29" s="103">
+        <v>0.69030000000000002</v>
+      </c>
+      <c r="G29" s="102" t="s">
+        <v>286</v>
+      </c>
+      <c r="H29" s="102" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B30" s="83"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="13"/>
       <c r="D30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B31" s="83"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="1" t="s">
+      <c r="B31" s="124"/>
+      <c r="C31" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D31" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="84"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="E31" s="146" t="s">
+        <v>280</v>
+      </c>
+      <c r="F31" s="147">
+        <v>0.67720000000000002</v>
+      </c>
+      <c r="G31" s="146" t="s">
+        <v>328</v>
+      </c>
+      <c r="H31" s="146" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="124"/>
+      <c r="C32" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="106" t="s">
+        <v>305</v>
+      </c>
+      <c r="F32" s="109">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="G32" s="110" t="s">
+        <v>327</v>
+      </c>
+      <c r="H32" s="108" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="33" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B33" s="82" t="s">
-        <v>251</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="D33" s="125" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="125" t="s">
-        <v>283</v>
-      </c>
-      <c r="F33" s="126"/>
-      <c r="G33" s="125"/>
-      <c r="H33" s="125"/>
-    </row>
-    <row r="34" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B34" s="83"/>
-      <c r="C34" s="22" t="s">
-        <v>281</v>
-      </c>
-      <c r="D34" s="125" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="125" t="s">
-        <v>285</v>
-      </c>
-      <c r="F34" s="126"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="125"/>
-    </row>
-    <row r="35" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B35" s="83"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B36" s="83"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="B33" s="124"/>
+      <c r="C33" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="D33" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="106" t="s">
+        <v>306</v>
+      </c>
+      <c r="F33" s="109">
+        <v>0.1991</v>
+      </c>
+      <c r="G33" s="110" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="108" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="124"/>
+      <c r="C34" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="D34" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="106" t="s">
+        <v>307</v>
+      </c>
+      <c r="F34" s="109">
+        <v>0.56259999999999999</v>
+      </c>
+      <c r="G34" s="110" t="s">
+        <v>98</v>
+      </c>
+      <c r="H34" s="108" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="124"/>
+      <c r="C35" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="D35" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="140">
+        <v>0.1024</v>
+      </c>
+      <c r="G35" s="136" t="s">
         <v>286</v>
       </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="83"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="83"/>
+      <c r="H35" s="136"/>
+    </row>
+    <row r="36" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="124"/>
+      <c r="C36" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D36" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="136" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="140">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G36" s="136" t="s">
+        <v>286</v>
+      </c>
+      <c r="H36" s="136"/>
+    </row>
+    <row r="37" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="124"/>
+      <c r="C37" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="D37" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="140">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="G37" s="136"/>
+      <c r="H37" s="136"/>
+    </row>
+    <row r="38" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="125"/>
       <c r="C38" s="13"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -5833,32 +6210,220 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="83"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="84"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+    <row r="39" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B39" s="123" t="s">
+        <v>248</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="D39" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="102" t="s">
+        <v>281</v>
+      </c>
+      <c r="F39" s="103">
+        <v>0.4929</v>
+      </c>
+      <c r="G39" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="102" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B40" s="124"/>
+      <c r="C40" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="D40" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="102" t="s">
+        <v>283</v>
+      </c>
+      <c r="F40" s="103">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="G40" s="102" t="s">
+        <v>287</v>
+      </c>
+      <c r="H40" s="102" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B41" s="124"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B42" s="124"/>
+      <c r="C42" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="D42" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="146" t="s">
+        <v>284</v>
+      </c>
+      <c r="F42" s="147">
+        <v>0.67969999999999997</v>
+      </c>
+      <c r="G42" s="146" t="s">
+        <v>333</v>
+      </c>
+      <c r="H42" s="146"/>
+    </row>
+    <row r="43" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B43" s="124"/>
+      <c r="C43" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="D43" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="106" t="s">
+        <v>308</v>
+      </c>
+      <c r="F43" s="109">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G43" s="149" t="s">
+        <v>329</v>
+      </c>
+      <c r="H43" s="108" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="124"/>
+      <c r="C44" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="D44" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="106" t="s">
+        <v>309</v>
+      </c>
+      <c r="F44" s="109">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="G44" s="110">
+        <v>50</v>
+      </c>
+      <c r="H44" s="108" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B45" s="124"/>
+      <c r="C45" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="D45" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="106" t="s">
+        <v>310</v>
+      </c>
+      <c r="F45" s="109">
+        <v>0.54239999999999999</v>
+      </c>
+      <c r="G45" s="110" t="s">
+        <v>327</v>
+      </c>
+      <c r="H45" s="108" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B46" s="124"/>
+      <c r="C46" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="140">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="G46" s="136" t="s">
+        <v>287</v>
+      </c>
+      <c r="H46" s="136"/>
+    </row>
+    <row r="47" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B47" s="124"/>
+      <c r="C47" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="136" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="140">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="G47" s="136" t="s">
+        <v>287</v>
+      </c>
+      <c r="H47" s="136"/>
+    </row>
+    <row r="48" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="124"/>
+      <c r="C48" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="D48" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="140">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="G48" s="136" t="s">
+        <v>287</v>
+      </c>
+      <c r="H48" s="136"/>
+    </row>
+    <row r="49" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="125"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="B39:B49"/>
     <mergeCell ref="B4:B22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="B27:B38"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5879,77 +6444,77 @@
   <sheetData>
     <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="102" t="s">
-        <v>269</v>
-      </c>
-      <c r="C4" s="93" t="s">
+      <c r="B4" s="132" t="s">
         <v>266</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="C4" s="130" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="131"/>
     </row>
     <row r="5" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="103"/>
-      <c r="C5" s="98" t="s">
+      <c r="B5" s="133"/>
+      <c r="C5" s="78" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="80" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="75" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>261</v>
-      </c>
-      <c r="D5" s="99" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="100" t="s">
-        <v>262</v>
-      </c>
-      <c r="C6" s="96" t="s">
-        <v>267</v>
-      </c>
-      <c r="D6" s="97" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="94" t="s">
-        <v>263</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>265</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="105" t="s">
-        <v>270</v>
-      </c>
-      <c r="C10" s="98" t="s">
-        <v>261</v>
-      </c>
-      <c r="D10" s="99" t="s">
-        <v>260</v>
+      <c r="B10" s="83" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="B11" s="104" t="s">
-        <v>259</v>
-      </c>
-      <c r="C11" s="97" t="s">
-        <v>271</v>
-      </c>
-      <c r="D11" s="97" t="s">
-        <v>271</v>
+      <c r="B11" s="82" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="77" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="77" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="101" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="106" t="s">
-        <v>272</v>
-      </c>
-      <c r="D12" s="106" t="s">
-        <v>272</v>
+      <c r="B12" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>269</v>
+      </c>
+      <c r="D12" s="84" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] Sending batch 7
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5A4A98-8E06-124A-970F-7828922050E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBD5978-1581-9B44-B44B-7583A4DB4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15260" yWindow="760" windowWidth="14140" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="15240" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="342">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -1069,6 +1069,30 @@
   </si>
   <si>
     <t>44/50</t>
+  </si>
+  <si>
+    <t>p32</t>
+  </si>
+  <si>
+    <t>p33</t>
+  </si>
+  <si>
+    <t>p34</t>
+  </si>
+  <si>
+    <t>p35</t>
+  </si>
+  <si>
+    <t>p7 with variance loss 0.05</t>
+  </si>
+  <si>
+    <t>p6 with variance loss 0.05</t>
+  </si>
+  <si>
+    <t>p7 with entropy loss 0.01</t>
+  </si>
+  <si>
+    <t>p6 with entropy loss 0.01</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="54">
+  <fills count="55">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1554,6 +1578,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="55">
     <border>
@@ -2296,7 +2326,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2475,15 +2505,6 @@
     <xf numFmtId="0" fontId="22" fillId="46" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="47" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="47" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="48" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2494,9 +2515,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="48" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="48" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2741,6 +2759,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="54" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="53" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3222,16 +3254,16 @@
       <c r="N4" s="41"/>
     </row>
     <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="114" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="118" t="s">
+      <c r="E5" s="114" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6">
@@ -3255,12 +3287,12 @@
       <c r="N5" s="42"/>
     </row>
     <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="121"/>
-      <c r="C6" s="119"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="119"/>
+      <c r="E6" s="115"/>
       <c r="F6" s="2">
         <v>0.83630000000000004</v>
       </c>
@@ -3282,7 +3314,7 @@
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="122"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="9" t="s">
         <v>137</v>
       </c>
@@ -3313,7 +3345,7 @@
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="111" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -3346,7 +3378,7 @@
       <c r="N8" s="45"/>
     </row>
     <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="117"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="9" t="s">
         <v>139</v>
       </c>
@@ -3377,7 +3409,7 @@
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="115" t="s">
+      <c r="B10" s="111" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -3408,7 +3440,7 @@
       <c r="N10" s="47"/>
     </row>
     <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="116"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="9" t="s">
         <v>141</v>
       </c>
@@ -3433,7 +3465,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="116"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="12" t="s">
         <v>142</v>
       </c>
@@ -3458,7 +3490,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="116"/>
+      <c r="B13" s="112"/>
       <c r="C13" s="33" t="s">
         <v>143</v>
       </c>
@@ -3483,7 +3515,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="116"/>
+      <c r="B14" s="112"/>
       <c r="C14" s="24" t="s">
         <v>144</v>
       </c>
@@ -3510,7 +3542,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="116"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="24" t="s">
         <v>145</v>
       </c>
@@ -3537,7 +3569,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="116"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="24" t="s">
         <v>146</v>
       </c>
@@ -3564,7 +3596,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="116"/>
+      <c r="B17" s="112"/>
       <c r="C17" s="24" t="s">
         <v>147</v>
       </c>
@@ -3591,7 +3623,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="116"/>
+      <c r="B18" s="112"/>
       <c r="C18" s="24" t="s">
         <v>148</v>
       </c>
@@ -3618,7 +3650,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="116"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="26" t="s">
         <v>149</v>
       </c>
@@ -3643,7 +3675,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="116"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="26" t="s">
         <v>150</v>
       </c>
@@ -3668,7 +3700,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="116"/>
+      <c r="B21" s="112"/>
       <c r="C21" s="26" t="s">
         <v>151</v>
       </c>
@@ -3693,7 +3725,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="116"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="26" t="s">
         <v>152</v>
       </c>
@@ -3718,7 +3750,7 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="116"/>
+      <c r="B23" s="112"/>
       <c r="C23" s="27" t="s">
         <v>153</v>
       </c>
@@ -3743,7 +3775,7 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="116"/>
+      <c r="B24" s="112"/>
       <c r="C24" s="27" t="s">
         <v>154</v>
       </c>
@@ -3768,7 +3800,7 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="116"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="27" t="s">
         <v>155</v>
       </c>
@@ -3793,7 +3825,7 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="116"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="27" t="s">
         <v>156</v>
       </c>
@@ -3818,7 +3850,7 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="116"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="28" t="s">
         <v>157</v>
       </c>
@@ -3843,7 +3875,7 @@
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="116"/>
+      <c r="B28" s="112"/>
       <c r="C28" s="28" t="s">
         <v>158</v>
       </c>
@@ -3868,7 +3900,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="116"/>
+      <c r="B29" s="112"/>
       <c r="C29" s="28" t="s">
         <v>159</v>
       </c>
@@ -3893,7 +3925,7 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="117"/>
+      <c r="B30" s="113"/>
       <c r="C30" s="14" t="s">
         <v>209</v>
       </c>
@@ -3918,7 +3950,7 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="115" t="s">
+      <c r="B31" s="111" t="s">
         <v>68</v>
       </c>
       <c r="C31" s="21" t="s">
@@ -3947,7 +3979,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="116"/>
+      <c r="B32" s="112"/>
       <c r="C32" s="22" t="s">
         <v>161</v>
       </c>
@@ -3972,7 +4004,7 @@
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="116"/>
+      <c r="B33" s="112"/>
       <c r="C33" s="20" t="s">
         <v>162</v>
       </c>
@@ -3997,7 +4029,7 @@
       <c r="J33" s="8"/>
     </row>
     <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="116"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="20" t="s">
         <v>163</v>
       </c>
@@ -4022,7 +4054,7 @@
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="116"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="20" t="s">
         <v>164</v>
       </c>
@@ -4047,7 +4079,7 @@
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="116"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="20" t="s">
         <v>165</v>
       </c>
@@ -4072,7 +4104,7 @@
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="116"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="20" t="s">
         <v>166</v>
       </c>
@@ -4099,7 +4131,7 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="116"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="20" t="s">
         <v>167</v>
       </c>
@@ -4126,7 +4158,7 @@
       </c>
     </row>
     <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="116"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="22" t="s">
         <v>168</v>
       </c>
@@ -4151,7 +4183,7 @@
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="116"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="22" t="s">
         <v>169</v>
       </c>
@@ -4178,7 +4210,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="116"/>
+      <c r="B41" s="112"/>
       <c r="C41" s="22" t="s">
         <v>170</v>
       </c>
@@ -4203,7 +4235,7 @@
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="116"/>
+      <c r="B42" s="112"/>
       <c r="C42" s="22" t="s">
         <v>171</v>
       </c>
@@ -4228,7 +4260,7 @@
       <c r="J42" s="8"/>
     </row>
     <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="116"/>
+      <c r="B43" s="112"/>
       <c r="C43" s="23" t="s">
         <v>172</v>
       </c>
@@ -4253,7 +4285,7 @@
       <c r="J43" s="8"/>
     </row>
     <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="116"/>
+      <c r="B44" s="112"/>
       <c r="C44" s="23" t="s">
         <v>173</v>
       </c>
@@ -4278,7 +4310,7 @@
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="116"/>
+      <c r="B45" s="112"/>
       <c r="C45" s="23" t="s">
         <v>174</v>
       </c>
@@ -4303,7 +4335,7 @@
       <c r="J45" s="8"/>
     </row>
     <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="116"/>
+      <c r="B46" s="112"/>
       <c r="C46" s="23" t="s">
         <v>175</v>
       </c>
@@ -4328,7 +4360,7 @@
       <c r="J46" s="8"/>
     </row>
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="116"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="34" t="s">
         <v>176</v>
       </c>
@@ -4355,7 +4387,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B48" s="116"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="34" t="s">
         <v>177</v>
       </c>
@@ -4380,7 +4412,7 @@
       <c r="J48" s="8"/>
     </row>
     <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="116"/>
+      <c r="B49" s="112"/>
       <c r="C49" s="30" t="s">
         <v>178</v>
       </c>
@@ -4403,7 +4435,7 @@
       <c r="J49" s="8"/>
     </row>
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="116"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="30" t="s">
         <v>179</v>
       </c>
@@ -4426,7 +4458,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="116"/>
+      <c r="B51" s="112"/>
       <c r="C51" s="25" t="s">
         <v>180</v>
       </c>
@@ -4448,12 +4480,12 @@
       <c r="I51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J51" s="74" t="s">
+      <c r="J51" s="70" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="116"/>
+      <c r="B52" s="112"/>
       <c r="C52" s="25" t="s">
         <v>181</v>
       </c>
@@ -4475,12 +4507,12 @@
       <c r="I52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="74" t="s">
+      <c r="J52" s="70" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="116"/>
+      <c r="B53" s="112"/>
       <c r="C53" s="25" t="s">
         <v>182</v>
       </c>
@@ -4502,12 +4534,12 @@
       <c r="I53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="74" t="s">
+      <c r="J53" s="70" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="116"/>
+      <c r="B54" s="112"/>
       <c r="C54" s="25" t="s">
         <v>183</v>
       </c>
@@ -4529,12 +4561,12 @@
       <c r="I54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J54" s="74" t="s">
+      <c r="J54" s="70" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="116"/>
+      <c r="B55" s="112"/>
       <c r="C55" s="25" t="s">
         <v>184</v>
       </c>
@@ -4556,12 +4588,12 @@
       <c r="I55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J55" s="74" t="s">
+      <c r="J55" s="70" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="116"/>
+      <c r="B56" s="112"/>
       <c r="C56" s="26" t="s">
         <v>185</v>
       </c>
@@ -4583,12 +4615,12 @@
       <c r="I56" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J56" s="111" t="s">
+      <c r="J56" s="107" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="116"/>
+      <c r="B57" s="112"/>
       <c r="C57" s="26" t="s">
         <v>186</v>
       </c>
@@ -4610,10 +4642,10 @@
       <c r="I57" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J57" s="111"/>
+      <c r="J57" s="107"/>
     </row>
     <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B58" s="116"/>
+      <c r="B58" s="112"/>
       <c r="C58" s="26" t="s">
         <v>187</v>
       </c>
@@ -4635,10 +4667,10 @@
       <c r="I58" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J58" s="111"/>
+      <c r="J58" s="107"/>
     </row>
     <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="116"/>
+      <c r="B59" s="112"/>
       <c r="C59" s="26" t="s">
         <v>188</v>
       </c>
@@ -4660,10 +4692,10 @@
       <c r="I59" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J59" s="111"/>
+      <c r="J59" s="107"/>
     </row>
     <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="116"/>
+      <c r="B60" s="112"/>
       <c r="C60" s="27" t="s">
         <v>189</v>
       </c>
@@ -4685,10 +4717,10 @@
       <c r="I60" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J60" s="111"/>
+      <c r="J60" s="107"/>
     </row>
     <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B61" s="116"/>
+      <c r="B61" s="112"/>
       <c r="C61" s="27" t="s">
         <v>190</v>
       </c>
@@ -4710,10 +4742,10 @@
       <c r="I61" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J61" s="111"/>
+      <c r="J61" s="107"/>
     </row>
     <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B62" s="116"/>
+      <c r="B62" s="112"/>
       <c r="C62" s="27" t="s">
         <v>191</v>
       </c>
@@ -4735,10 +4767,10 @@
       <c r="I62" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J62" s="111"/>
+      <c r="J62" s="107"/>
     </row>
     <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B63" s="116"/>
+      <c r="B63" s="112"/>
       <c r="C63" s="27" t="s">
         <v>192</v>
       </c>
@@ -4760,10 +4792,10 @@
       <c r="I63" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J63" s="111"/>
+      <c r="J63" s="107"/>
     </row>
     <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="116"/>
+      <c r="B64" s="112"/>
       <c r="C64" s="28" t="s">
         <v>193</v>
       </c>
@@ -4785,10 +4817,10 @@
       <c r="I64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J64" s="111"/>
+      <c r="J64" s="107"/>
     </row>
     <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B65" s="116"/>
+      <c r="B65" s="112"/>
       <c r="C65" s="28" t="s">
         <v>194</v>
       </c>
@@ -4810,10 +4842,10 @@
       <c r="I65" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J65" s="111"/>
+      <c r="J65" s="107"/>
     </row>
     <row r="66" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="116"/>
+      <c r="B66" s="112"/>
       <c r="C66" s="28" t="s">
         <v>195</v>
       </c>
@@ -4835,10 +4867,10 @@
       <c r="I66" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J66" s="111"/>
+      <c r="J66" s="107"/>
     </row>
     <row r="67" spans="2:10" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="116"/>
+      <c r="B67" s="112"/>
       <c r="C67" s="29" t="s">
         <v>196</v>
       </c>
@@ -4860,10 +4892,10 @@
       <c r="I67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="111"/>
+      <c r="J67" s="107"/>
     </row>
     <row r="68" spans="2:10" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="116"/>
+      <c r="B68" s="112"/>
       <c r="C68" s="29" t="s">
         <v>197</v>
       </c>
@@ -4885,10 +4917,10 @@
       <c r="I68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J68" s="111"/>
+      <c r="J68" s="107"/>
     </row>
     <row r="69" spans="2:10" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="116"/>
+      <c r="B69" s="112"/>
       <c r="C69" s="29" t="s">
         <v>198</v>
       </c>
@@ -4910,10 +4942,10 @@
       <c r="I69" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J69" s="111"/>
+      <c r="J69" s="107"/>
     </row>
     <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="117"/>
+      <c r="B70" s="113"/>
       <c r="C70" s="49" t="s">
         <v>199</v>
       </c>
@@ -4935,10 +4967,10 @@
       <c r="I70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J70" s="111"/>
+      <c r="J70" s="107"/>
     </row>
     <row r="71" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="112" t="s">
+      <c r="B71" s="108" t="s">
         <v>131</v>
       </c>
       <c r="C71" s="50" t="s">
@@ -4956,10 +4988,10 @@
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="J71" s="111"/>
+      <c r="J71" s="107"/>
     </row>
     <row r="72" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="113"/>
+      <c r="B72" s="109"/>
       <c r="C72" s="51" t="s">
         <v>201</v>
       </c>
@@ -4975,10 +5007,10 @@
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="111"/>
+      <c r="J72" s="107"/>
     </row>
     <row r="73" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="113"/>
+      <c r="B73" s="109"/>
       <c r="C73" s="51" t="s">
         <v>202</v>
       </c>
@@ -4990,10 +5022,10 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="111"/>
+      <c r="J73" s="107"/>
     </row>
     <row r="74" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="114"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="52" t="s">
         <v>203</v>
       </c>
@@ -5005,10 +5037,10 @@
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
-      <c r="J74" s="111"/>
+      <c r="J74" s="107"/>
     </row>
     <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="115" t="s">
+      <c r="B75" s="111" t="s">
         <v>129</v>
       </c>
       <c r="C75" s="48" t="s">
@@ -5032,10 +5064,10 @@
       <c r="I75" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J75" s="111"/>
+      <c r="J75" s="107"/>
     </row>
     <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B76" s="116"/>
+      <c r="B76" s="112"/>
       <c r="C76" s="13" t="s">
         <v>205</v>
       </c>
@@ -5060,7 +5092,7 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B77" s="116"/>
+      <c r="B77" s="112"/>
       <c r="C77" s="13" t="s">
         <v>206</v>
       </c>
@@ -5087,7 +5119,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B78" s="116"/>
+      <c r="B78" s="112"/>
       <c r="C78" s="13" t="s">
         <v>207</v>
       </c>
@@ -5112,7 +5144,7 @@
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B79" s="116"/>
+      <c r="B79" s="112"/>
       <c r="C79" s="13" t="s">
         <v>208</v>
       </c>
@@ -5139,7 +5171,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B80" s="116"/>
+      <c r="B80" s="112"/>
       <c r="C80" s="13" t="s">
         <v>212</v>
       </c>
@@ -5162,7 +5194,7 @@
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B81" s="116"/>
+      <c r="B81" s="112"/>
       <c r="C81" s="15" t="s">
         <v>219</v>
       </c>
@@ -5185,7 +5217,7 @@
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B82" s="116"/>
+      <c r="B82" s="112"/>
       <c r="C82" s="13" t="s">
         <v>221</v>
       </c>
@@ -5208,7 +5240,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B83" s="116"/>
+      <c r="B83" s="112"/>
       <c r="C83" s="13" t="s">
         <v>222</v>
       </c>
@@ -5231,7 +5263,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B84" s="116"/>
+      <c r="B84" s="112"/>
       <c r="C84" s="13" t="s">
         <v>224</v>
       </c>
@@ -5254,7 +5286,7 @@
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="116"/>
+      <c r="B85" s="112"/>
       <c r="C85" s="13"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -5265,7 +5297,7 @@
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="116"/>
+      <c r="B86" s="112"/>
       <c r="C86" s="13"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -5276,7 +5308,7 @@
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B87" s="116"/>
+      <c r="B87" s="112"/>
       <c r="C87" s="13"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -5287,7 +5319,7 @@
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B88" s="116"/>
+      <c r="B88" s="112"/>
       <c r="C88" s="13"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -5298,7 +5330,7 @@
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="116"/>
+      <c r="B89" s="112"/>
       <c r="C89" s="13"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -5309,7 +5341,7 @@
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="116"/>
+      <c r="B90" s="112"/>
       <c r="C90" s="13"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -5320,7 +5352,7 @@
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B91" s="116"/>
+      <c r="B91" s="112"/>
       <c r="C91" s="13"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -5331,7 +5363,7 @@
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B92" s="116"/>
+      <c r="B92" s="112"/>
       <c r="C92" s="13"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -5342,7 +5374,7 @@
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" s="116"/>
+      <c r="B93" s="112"/>
       <c r="C93" s="13"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -5353,7 +5385,7 @@
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="116"/>
+      <c r="B94" s="112"/>
       <c r="C94" s="13"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -5364,7 +5396,7 @@
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="116"/>
+      <c r="B95" s="112"/>
       <c r="C95" s="13"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -5375,7 +5407,7 @@
       <c r="J95" s="1"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="116"/>
+      <c r="B96" s="112"/>
       <c r="C96" s="13"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -5386,7 +5418,7 @@
       <c r="J96" s="1"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B97" s="116"/>
+      <c r="B97" s="112"/>
       <c r="C97" s="13"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -5397,7 +5429,7 @@
       <c r="J97" s="1"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" s="116"/>
+      <c r="B98" s="112"/>
       <c r="C98" s="13"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -5408,7 +5440,7 @@
       <c r="J98" s="1"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="116"/>
+      <c r="B99" s="112"/>
       <c r="C99" s="13"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -5419,7 +5451,7 @@
       <c r="J99" s="1"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B100" s="116"/>
+      <c r="B100" s="112"/>
       <c r="C100" s="13"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -5430,7 +5462,7 @@
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B101" s="116"/>
+      <c r="B101" s="112"/>
       <c r="C101" s="13"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -5441,7 +5473,7 @@
       <c r="J101" s="1"/>
     </row>
     <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="117"/>
+      <c r="B102" s="113"/>
       <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -5481,16 +5513,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="88"/>
+    <col min="6" max="6" width="10.83203125" style="84"/>
     <col min="8" max="8" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5508,18 +5540,18 @@
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="122" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
       <c r="I2" s="54"/>
       <c r="J2" s="36" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="K2" s="38"/>
     </row>
@@ -5548,131 +5580,137 @@
       </c>
       <c r="I3" s="54"/>
       <c r="J3" s="36" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="54"/>
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="87" t="s">
         <v>232</v>
       </c>
-      <c r="F4" s="92">
+      <c r="F4" s="88">
         <v>0.36480000000000001</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="87" t="s">
         <v>231</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="89" t="s">
         <v>253</v>
       </c>
       <c r="I4" s="54"/>
       <c r="J4" s="36" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="K4" s="40"/>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="54"/>
-      <c r="B5" s="124"/>
-      <c r="C5" s="68" t="s">
+      <c r="B5" s="120"/>
+      <c r="C5" s="137" t="s">
         <v>320</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="151" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="139" t="s">
         <v>272</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="140" t="s">
         <v>325</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="139" t="s">
         <v>326</v>
       </c>
-      <c r="H5" s="62"/>
+      <c r="H5" s="141"/>
       <c r="I5" s="54"/>
-      <c r="J5" s="36" t="s">
-        <v>13</v>
+      <c r="J5" s="54" t="s">
+        <v>19</v>
       </c>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="54"/>
-      <c r="B6" s="124"/>
-      <c r="C6" s="89" t="s">
+      <c r="B6" s="120"/>
+      <c r="C6" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="D6" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="87" t="s">
         <v>251</v>
       </c>
-      <c r="F6" s="92">
+      <c r="F6" s="88">
         <v>0.65839999999999999</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="G6" s="87" t="s">
         <v>244</v>
       </c>
-      <c r="H6" s="93" t="s">
+      <c r="H6" s="89" t="s">
         <v>254</v>
       </c>
       <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
+      <c r="J6" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="149"/>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="54"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="89" t="s">
+      <c r="B7" s="120"/>
+      <c r="C7" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="87" t="s">
         <v>252</v>
       </c>
-      <c r="F7" s="92">
+      <c r="F7" s="88">
         <v>0.65269999999999995</v>
       </c>
-      <c r="G7" s="91" t="s">
+      <c r="G7" s="87" t="s">
         <v>245</v>
       </c>
-      <c r="H7" s="93" t="s">
+      <c r="H7" s="89" t="s">
         <v>254</v>
       </c>
       <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
+      <c r="J7" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="150"/>
     </row>
     <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
-      <c r="B8" s="124"/>
-      <c r="C8" s="97" t="s">
+      <c r="B8" s="120"/>
+      <c r="C8" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="95" t="s">
         <v>270</v>
       </c>
-      <c r="F8" s="100">
+      <c r="F8" s="96">
         <v>0.73540000000000005</v>
       </c>
-      <c r="G8" s="99" t="s">
+      <c r="G8" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="101" t="s">
+      <c r="H8" s="97" t="s">
         <v>288</v>
       </c>
       <c r="I8" s="54"/>
@@ -5680,45 +5718,45 @@
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
-      <c r="B9" s="124"/>
-      <c r="C9" s="141" t="s">
+      <c r="B9" s="120"/>
+      <c r="C9" s="137" t="s">
         <v>321</v>
       </c>
-      <c r="D9" s="142" t="s">
+      <c r="D9" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="143" t="s">
+      <c r="E9" s="139" t="s">
         <v>273</v>
       </c>
-      <c r="F9" s="144">
+      <c r="F9" s="140">
         <v>0.74019999999999997</v>
       </c>
-      <c r="G9" s="143" t="s">
+      <c r="G9" s="139" t="s">
         <v>332</v>
       </c>
-      <c r="H9" s="145"/>
+      <c r="H9" s="141"/>
       <c r="I9" s="54"/>
       <c r="J9" s="54"/>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="104" t="s">
+      <c r="B10" s="120"/>
+      <c r="C10" s="100" t="s">
         <v>279</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D10" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="102" t="s">
         <v>302</v>
       </c>
-      <c r="F10" s="107">
+      <c r="F10" s="103">
         <v>0.46329999999999999</v>
       </c>
-      <c r="G10" s="148" t="s">
+      <c r="G10" s="144" t="s">
         <v>324</v>
       </c>
-      <c r="H10" s="108" t="s">
+      <c r="H10" s="104" t="s">
         <v>293</v>
       </c>
       <c r="I10" s="54"/>
@@ -5726,23 +5764,23 @@
     </row>
     <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
-      <c r="B11" s="124"/>
-      <c r="C11" s="104" t="s">
+      <c r="B11" s="120"/>
+      <c r="C11" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="106" t="s">
+      <c r="E11" s="102" t="s">
         <v>303</v>
       </c>
-      <c r="F11" s="107">
+      <c r="F11" s="103">
         <v>0.62519999999999998</v>
       </c>
-      <c r="G11" s="106" t="s">
+      <c r="G11" s="102" t="s">
         <v>330</v>
       </c>
-      <c r="H11" s="108" t="s">
+      <c r="H11" s="104" t="s">
         <v>293</v>
       </c>
       <c r="I11" s="54"/>
@@ -5750,23 +5788,23 @@
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="54"/>
-      <c r="B12" s="124"/>
-      <c r="C12" s="104" t="s">
+      <c r="B12" s="120"/>
+      <c r="C12" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="106" t="s">
+      <c r="E12" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="F12" s="107">
+      <c r="F12" s="103">
         <v>0.69059999999999999</v>
       </c>
-      <c r="G12" s="106" t="s">
+      <c r="G12" s="102" t="s">
         <v>331</v>
       </c>
-      <c r="H12" s="108" t="s">
+      <c r="H12" s="104" t="s">
         <v>293</v>
       </c>
       <c r="I12" s="54"/>
@@ -5774,156 +5812,156 @@
     </row>
     <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="134" t="s">
+      <c r="B13" s="120"/>
+      <c r="C13" s="130" t="s">
         <v>311</v>
       </c>
-      <c r="D13" s="135" t="s">
+      <c r="D13" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="136" t="s">
+      <c r="E13" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="137">
+      <c r="F13" s="133">
         <v>0.13159999999999999</v>
       </c>
-      <c r="G13" s="138" t="s">
+      <c r="G13" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="139"/>
+      <c r="H13" s="135"/>
       <c r="I13" s="54"/>
       <c r="J13" s="54"/>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
-      <c r="B14" s="124"/>
-      <c r="C14" s="134" t="s">
+      <c r="B14" s="120"/>
+      <c r="C14" s="130" t="s">
         <v>312</v>
       </c>
-      <c r="D14" s="135" t="s">
+      <c r="D14" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="136" t="s">
+      <c r="E14" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="137">
+      <c r="F14" s="133">
         <v>5.57E-2</v>
       </c>
-      <c r="G14" s="138" t="s">
+      <c r="G14" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="139"/>
+      <c r="H14" s="135"/>
       <c r="I14" s="54"/>
       <c r="J14" s="54"/>
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
-      <c r="B15" s="124"/>
-      <c r="C15" s="134" t="s">
+      <c r="B15" s="120"/>
+      <c r="C15" s="130" t="s">
         <v>313</v>
       </c>
-      <c r="D15" s="135" t="s">
+      <c r="D15" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="136" t="s">
+      <c r="E15" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="137">
+      <c r="F15" s="133">
         <v>3.6200000000000003E-2</v>
       </c>
-      <c r="G15" s="138" t="s">
+      <c r="G15" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="139"/>
+      <c r="H15" s="135"/>
       <c r="I15" s="54"/>
       <c r="J15" s="54"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
-      <c r="B16" s="124"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="66"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="63"/>
       <c r="I16" s="54"/>
       <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
-      <c r="B17" s="124"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="66"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="63"/>
       <c r="I17" s="54"/>
       <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
-      <c r="B18" s="124"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="66"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="63"/>
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
-      <c r="B19" s="124"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="66"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="63"/>
       <c r="I19" s="54"/>
       <c r="J19" s="54"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
-      <c r="B20" s="124"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="66"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="63"/>
       <c r="I20" s="54"/>
       <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
-      <c r="B21" s="124"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="66"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="63"/>
       <c r="I21" s="54"/>
       <c r="J21" s="54"/>
     </row>
     <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="54"/>
-      <c r="B22" s="125"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="73"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="69"/>
       <c r="I22" s="54"/>
       <c r="J22" s="54"/>
     </row>
     <row r="23" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="127" t="s">
+      <c r="B23" s="123" t="s">
         <v>235</v>
       </c>
       <c r="C23" s="50" t="s">
@@ -5940,7 +5978,7 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="128"/>
+      <c r="B24" s="124"/>
       <c r="C24" s="51" t="s">
         <v>238</v>
       </c>
@@ -5955,7 +5993,7 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="128"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="51" t="s">
         <v>239</v>
       </c>
@@ -5970,8 +6008,8 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="129"/>
-      <c r="C26" s="87" t="s">
+      <c r="B26" s="125"/>
+      <c r="C26" s="83" t="s">
         <v>240</v>
       </c>
       <c r="D26" s="4"/>
@@ -5985,72 +6023,72 @@
       <c r="H26" s="53"/>
     </row>
     <row r="27" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="123" t="s">
+      <c r="B27" s="119" t="s">
         <v>132</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="D27" s="95" t="s">
+      <c r="D27" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="95" t="s">
+      <c r="E27" s="91" t="s">
         <v>247</v>
       </c>
-      <c r="F27" s="96">
+      <c r="F27" s="92">
         <v>0.27600000000000002</v>
       </c>
-      <c r="G27" s="95">
+      <c r="G27" s="91">
         <v>50</v>
       </c>
-      <c r="H27" s="95" t="s">
+      <c r="H27" s="91" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="124"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="102" t="s">
+      <c r="D28" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="102" t="s">
+      <c r="E28" s="98" t="s">
         <v>271</v>
       </c>
-      <c r="F28" s="103">
+      <c r="F28" s="99">
         <v>0.52239999999999998</v>
       </c>
-      <c r="G28" s="102" t="s">
+      <c r="G28" s="98" t="s">
         <v>285</v>
       </c>
-      <c r="H28" s="102" t="s">
+      <c r="H28" s="98" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B29" s="124"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="D29" s="102" t="s">
+      <c r="D29" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="102" t="s">
+      <c r="E29" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="F29" s="103">
+      <c r="F29" s="99">
         <v>0.69030000000000002</v>
       </c>
-      <c r="G29" s="102" t="s">
+      <c r="G29" s="98" t="s">
         <v>286</v>
       </c>
-      <c r="H29" s="102" t="s">
+      <c r="H29" s="98" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B30" s="124"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="13"/>
       <c r="D30" s="1" t="s">
         <v>30</v>
@@ -6063,365 +6101,434 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B31" s="124"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="D31" s="146" t="s">
+      <c r="D31" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="146" t="s">
+      <c r="E31" s="142" t="s">
         <v>280</v>
       </c>
-      <c r="F31" s="147">
+      <c r="F31" s="143">
         <v>0.67720000000000002</v>
       </c>
-      <c r="G31" s="146" t="s">
+      <c r="G31" s="142" t="s">
         <v>328</v>
       </c>
-      <c r="H31" s="146" t="s">
+      <c r="H31" s="142" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="124"/>
+      <c r="B32" s="120"/>
       <c r="C32" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="D32" s="105" t="s">
+      <c r="D32" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="106" t="s">
+      <c r="E32" s="102" t="s">
         <v>305</v>
       </c>
-      <c r="F32" s="109">
+      <c r="F32" s="105">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="G32" s="110" t="s">
+      <c r="G32" s="106" t="s">
         <v>327</v>
       </c>
-      <c r="H32" s="108" t="s">
+      <c r="H32" s="104" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B33" s="124"/>
+      <c r="B33" s="120"/>
       <c r="C33" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="D33" s="105" t="s">
+      <c r="D33" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="106" t="s">
+      <c r="E33" s="102" t="s">
         <v>306</v>
       </c>
-      <c r="F33" s="109">
+      <c r="F33" s="105">
         <v>0.1991</v>
       </c>
-      <c r="G33" s="110" t="s">
+      <c r="G33" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="108" t="s">
+      <c r="H33" s="104" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="124"/>
+      <c r="B34" s="120"/>
       <c r="C34" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="D34" s="105" t="s">
+      <c r="D34" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="106" t="s">
+      <c r="E34" s="102" t="s">
         <v>307</v>
       </c>
-      <c r="F34" s="109">
+      <c r="F34" s="105">
         <v>0.56259999999999999</v>
       </c>
-      <c r="G34" s="110" t="s">
+      <c r="G34" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="H34" s="108" t="s">
+      <c r="H34" s="104" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="124"/>
+      <c r="B35" s="120"/>
       <c r="C35" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="D35" s="135" t="s">
+      <c r="D35" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="136" t="s">
+      <c r="E35" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="140">
+      <c r="F35" s="136">
         <v>0.1024</v>
       </c>
-      <c r="G35" s="136" t="s">
+      <c r="G35" s="132" t="s">
         <v>286</v>
       </c>
-      <c r="H35" s="136"/>
+      <c r="H35" s="132"/>
     </row>
     <row r="36" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="124"/>
+      <c r="B36" s="120"/>
       <c r="C36" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="D36" s="135" t="s">
+      <c r="D36" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="136" t="s">
+      <c r="E36" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="140">
+      <c r="F36" s="136">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G36" s="136" t="s">
+      <c r="G36" s="132" t="s">
         <v>286</v>
       </c>
-      <c r="H36" s="136"/>
+      <c r="H36" s="132"/>
     </row>
     <row r="37" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B37" s="124"/>
+      <c r="B37" s="120"/>
       <c r="C37" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="D37" s="135" t="s">
+      <c r="D37" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="136" t="s">
+      <c r="E37" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="140">
+      <c r="F37" s="136">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="G37" s="136"/>
-      <c r="H37" s="136"/>
-    </row>
-    <row r="38" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="125"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="G37" s="132"/>
+      <c r="H37" s="132"/>
+    </row>
+    <row r="38" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B38" s="120"/>
+      <c r="C38" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="D38" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="147" t="s">
+        <v>338</v>
+      </c>
+      <c r="F38" s="148"/>
+      <c r="G38" s="147"/>
+      <c r="H38" s="147"/>
     </row>
     <row r="39" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="123" t="s">
+      <c r="B39" s="120"/>
+      <c r="C39" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="D39" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="147" t="s">
+        <v>339</v>
+      </c>
+      <c r="F39" s="148"/>
+      <c r="G39" s="147"/>
+      <c r="H39" s="147"/>
+    </row>
+    <row r="40" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B40" s="120"/>
+      <c r="C40" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="D40" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="147" t="s">
+        <v>340</v>
+      </c>
+      <c r="F40" s="148"/>
+      <c r="G40" s="147"/>
+      <c r="H40" s="147"/>
+    </row>
+    <row r="41" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B41" s="120"/>
+      <c r="C41" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="D41" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="147" t="s">
+        <v>341</v>
+      </c>
+      <c r="F41" s="148"/>
+      <c r="G41" s="147"/>
+      <c r="H41" s="147"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="120"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="121"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="119" t="s">
         <v>248</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C44" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="D39" s="102" t="s">
+      <c r="D44" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="102" t="s">
+      <c r="E44" s="98" t="s">
         <v>281</v>
       </c>
-      <c r="F39" s="103">
+      <c r="F44" s="99">
         <v>0.4929</v>
       </c>
-      <c r="G39" s="102" t="s">
+      <c r="G44" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="102" t="s">
+      <c r="H44" s="98" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B40" s="124"/>
-      <c r="C40" s="22" t="s">
+    <row r="45" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B45" s="120"/>
+      <c r="C45" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="D40" s="102" t="s">
+      <c r="D45" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="102" t="s">
+      <c r="E45" s="98" t="s">
         <v>283</v>
       </c>
-      <c r="F40" s="103">
+      <c r="F45" s="99">
         <v>0.66930000000000001</v>
       </c>
-      <c r="G40" s="102" t="s">
+      <c r="G45" s="98" t="s">
         <v>287</v>
       </c>
-      <c r="H40" s="102" t="s">
+      <c r="H45" s="98" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B41" s="124"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="1" t="s">
+    <row r="46" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B46" s="120"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B42" s="124"/>
-      <c r="C42" s="25" t="s">
+      <c r="F46" s="2"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B47" s="120"/>
+      <c r="C47" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="D42" s="146" t="s">
+      <c r="D47" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="146" t="s">
+      <c r="E47" s="142" t="s">
         <v>284</v>
       </c>
-      <c r="F42" s="147">
+      <c r="F47" s="143">
         <v>0.67969999999999997</v>
       </c>
-      <c r="G42" s="146" t="s">
+      <c r="G47" s="142" t="s">
         <v>333</v>
       </c>
-      <c r="H42" s="146"/>
-    </row>
-    <row r="43" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B43" s="124"/>
-      <c r="C43" s="23" t="s">
+      <c r="H47" s="142"/>
+    </row>
+    <row r="48" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="120"/>
+      <c r="C48" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="D43" s="105" t="s">
+      <c r="D48" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="106" t="s">
+      <c r="E48" s="102" t="s">
         <v>308</v>
       </c>
-      <c r="F43" s="109">
+      <c r="F48" s="105">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G43" s="149" t="s">
+      <c r="G48" s="145" t="s">
         <v>329</v>
       </c>
-      <c r="H43" s="108" t="s">
+      <c r="H48" s="104" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B44" s="124"/>
-      <c r="C44" s="23" t="s">
+    <row r="49" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B49" s="120"/>
+      <c r="C49" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="D44" s="105" t="s">
+      <c r="D49" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="106" t="s">
+      <c r="E49" s="102" t="s">
         <v>309</v>
       </c>
-      <c r="F44" s="109">
+      <c r="F49" s="105">
         <v>0.16900000000000001</v>
       </c>
-      <c r="G44" s="110">
+      <c r="G49" s="106">
         <v>50</v>
       </c>
-      <c r="H44" s="108" t="s">
+      <c r="H49" s="104" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B45" s="124"/>
-      <c r="C45" s="23" t="s">
+    <row r="50" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B50" s="120"/>
+      <c r="C50" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="D45" s="105" t="s">
+      <c r="D50" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="106" t="s">
+      <c r="E50" s="102" t="s">
         <v>310</v>
       </c>
-      <c r="F45" s="109">
+      <c r="F50" s="105">
         <v>0.54239999999999999</v>
       </c>
-      <c r="G45" s="110" t="s">
+      <c r="G50" s="106" t="s">
         <v>327</v>
       </c>
-      <c r="H45" s="108" t="s">
+      <c r="H50" s="104" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B46" s="124"/>
-      <c r="C46" s="24" t="s">
+    <row r="51" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B51" s="120"/>
+      <c r="C51" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="D46" s="135" t="s">
+      <c r="D51" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E46" s="136" t="s">
+      <c r="E51" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="F46" s="140">
+      <c r="F51" s="136">
         <v>7.7899999999999997E-2</v>
       </c>
-      <c r="G46" s="136" t="s">
+      <c r="G51" s="132" t="s">
         <v>287</v>
       </c>
-      <c r="H46" s="136"/>
-    </row>
-    <row r="47" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B47" s="124"/>
-      <c r="C47" s="24" t="s">
+      <c r="H51" s="132"/>
+    </row>
+    <row r="52" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B52" s="120"/>
+      <c r="C52" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="D47" s="135" t="s">
+      <c r="D52" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E47" s="136" t="s">
+      <c r="E52" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="140">
+      <c r="F52" s="136">
         <v>3.2099999999999997E-2</v>
       </c>
-      <c r="G47" s="136" t="s">
+      <c r="G52" s="132" t="s">
         <v>287</v>
       </c>
-      <c r="H47" s="136"/>
-    </row>
-    <row r="48" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B48" s="124"/>
-      <c r="C48" s="24" t="s">
+      <c r="H52" s="132"/>
+    </row>
+    <row r="53" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B53" s="120"/>
+      <c r="C53" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="D48" s="135" t="s">
+      <c r="D53" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E48" s="136" t="s">
+      <c r="E53" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F48" s="140">
+      <c r="F53" s="136">
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="G48" s="136" t="s">
+      <c r="G53" s="132" t="s">
         <v>287</v>
       </c>
-      <c r="H48" s="136"/>
-    </row>
-    <row r="49" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="125"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="H53" s="132"/>
+    </row>
+    <row r="54" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="121"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B39:B49"/>
+    <mergeCell ref="B44:B54"/>
     <mergeCell ref="B4:B22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="B27:B43"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6444,36 +6551,36 @@
   <sheetData>
     <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="132" t="s">
+      <c r="B4" s="128" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="126" t="s">
         <v>263</v>
       </c>
-      <c r="D4" s="131"/>
+      <c r="D4" s="127"/>
     </row>
     <row r="5" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="133"/>
-      <c r="C5" s="78" t="s">
+      <c r="B5" s="129"/>
+      <c r="C5" s="74" t="s">
         <v>258</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="75" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="76" t="s">
         <v>259</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="72" t="s">
         <v>264</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="73" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="71" t="s">
         <v>260</v>
       </c>
       <c r="C7" s="52" t="s">
@@ -6485,35 +6592,35 @@
     </row>
     <row r="9" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="79" t="s">
         <v>267</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="74" t="s">
         <v>258</v>
       </c>
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="75" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="73" t="s">
         <v>268</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="D11" s="73" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="80" t="s">
         <v>269</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="80" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMP] Sending batch 8
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBD5978-1581-9B44-B44B-7583A4DB4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070DAEF0-08CE-9C46-ABFA-4D9412DD66DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="1080" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="386">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>BAD - slower convergence than default scheduler</t>
-  </si>
-  <si>
-    <t>pos embed + dropout</t>
   </si>
   <si>
     <t>this reached 90.42 fast!!</t>
@@ -730,9 +727,6 @@
     <t>21/31</t>
   </si>
   <si>
-    <t>Resnet simple transforms (scratch). ReduceLROnPlateau</t>
-  </si>
-  <si>
     <t>p2</t>
   </si>
   <si>
@@ -773,9 +767,6 @@
   </si>
   <si>
     <t>p4</t>
-  </si>
-  <si>
-    <t>ZoomVit (scratch) + color_jitter (0.1s)</t>
   </si>
   <si>
     <t>BrainiT</t>
@@ -882,9 +873,6 @@
     <t>Resnet pretrained, correct (config tables)</t>
   </si>
   <si>
-    <t>ZoomVit scratch, correct (config tables)</t>
-  </si>
-  <si>
     <t>Resnet scratch, correct (config tables)</t>
   </si>
   <si>
@@ -900,18 +888,12 @@
     <t>p8</t>
   </si>
   <si>
-    <t>ZoomViT (pretrained), correct (config tables)</t>
-  </si>
-  <si>
     <t>p9</t>
   </si>
   <si>
     <t>p10</t>
   </si>
   <si>
-    <t>ZoomViT (pretrained), correct (config tables) but no color jitter</t>
-  </si>
-  <si>
     <t>Brainit (scratch) +  correct (config tables</t>
   </si>
   <si>
@@ -1093,6 +1075,156 @@
   </si>
   <si>
     <t>p6 with entropy loss 0.01</t>
+  </si>
+  <si>
+    <t>50/50</t>
+  </si>
+  <si>
+    <t>DIDN’T CLAMP LOSS</t>
+  </si>
+  <si>
+    <t>45/50</t>
+  </si>
+  <si>
+    <t>p36</t>
+  </si>
+  <si>
+    <t>p37</t>
+  </si>
+  <si>
+    <t>p38</t>
+  </si>
+  <si>
+    <t>p7/p34 with entropy loss 0.1</t>
+  </si>
+  <si>
+    <t>p6/p35 with entropy loss 0.1</t>
+  </si>
+  <si>
+    <t>p7/p32 with variance loss 0.001</t>
+  </si>
+  <si>
+    <t>p39</t>
+  </si>
+  <si>
+    <t>NoZoom on pretrained (p7)</t>
+  </si>
+  <si>
+    <t>NoZoom on scratch (p6)</t>
+  </si>
+  <si>
+    <t>p40</t>
+  </si>
+  <si>
+    <t>pos embed + dropout (0.1)</t>
+  </si>
+  <si>
+    <t>p7/p34 with entropy loss 0.5</t>
+  </si>
+  <si>
+    <t>p6/p35 with entropy loss 0.5</t>
+  </si>
+  <si>
+    <t>Dropout (0.2, 0.1, 0.1) and Mixup Function on p37</t>
+  </si>
+  <si>
+    <t>Pretrained or Scratch</t>
+  </si>
+  <si>
+    <t>Resnet simple transforms. ReduceLROnPlateau</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>ZoomVit + color_jitter (0.1s)</t>
+  </si>
+  <si>
+    <t>ZoomVit correct (config tables)</t>
+  </si>
+  <si>
+    <t>ZoomViT  correct (config tables)</t>
+  </si>
+  <si>
+    <t>ZoomVit correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>ZoomViT correct (config tables) but no color jitter</t>
+  </si>
+  <si>
+    <t>Dropout (0.2, 0.1, 0.1) and Mixup Function on p38</t>
+  </si>
+  <si>
+    <t>p41</t>
+  </si>
+  <si>
+    <t>p42</t>
+  </si>
+  <si>
+    <t>CLAMPED LOSS</t>
+  </si>
+  <si>
+    <t>MODEL NO LONGER OVERFITTING</t>
+  </si>
+  <si>
+    <t>p43</t>
+  </si>
+  <si>
+    <t>p44</t>
+  </si>
+  <si>
+    <t>dropout+mixup but for 70 epochs entropy 0.1 (p39)</t>
+  </si>
+  <si>
+    <t>dropout+mixup but for 70 epochs entropy 0.1 (p40)</t>
+  </si>
+  <si>
+    <t>p45</t>
+  </si>
+  <si>
+    <t>p46</t>
+  </si>
+  <si>
+    <t>p7/p34 with entropy loss 0.8</t>
+  </si>
+  <si>
+    <t>p7/34 with entropy loss 0.8</t>
+  </si>
+  <si>
+    <t>p47</t>
+  </si>
+  <si>
+    <t>p48</t>
+  </si>
+  <si>
+    <t>p7/p32 with variance loss 0.01</t>
+  </si>
+  <si>
+    <t>p7/p32 with variance loss 0.05</t>
+  </si>
+  <si>
+    <t>p49</t>
+  </si>
+  <si>
+    <t>p50</t>
+  </si>
+  <si>
+    <t>p51</t>
+  </si>
+  <si>
+    <t>p52</t>
+  </si>
+  <si>
+    <t>p6/p33 with variance loss 0.01</t>
+  </si>
+  <si>
+    <t>p6/p33 with variance loss 0.05</t>
+  </si>
+  <si>
+    <t>dropout+mixup but for 70 epochs entropy 0.5 (p49)</t>
+  </si>
+  <si>
+    <t>dropout+mixup but for 70 epochs entropy 0.5 (p50)</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1404,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="55">
+  <fills count="57">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1584,6 +1716,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="55">
     <border>
@@ -2326,7 +2470,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2775,6 +2919,32 @@
     <xf numFmtId="0" fontId="23" fillId="53" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="55" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="56" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="56" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2820,7 +2990,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2846,6 +3026,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF75489E"/>
       <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
@@ -3179,8 +3360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N102"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3201,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N1" s="38"/>
     </row>
@@ -3253,12 +3434,12 @@
       </c>
       <c r="N4" s="41"/>
     </row>
-    <row r="5" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="116" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>30</v>
@@ -3286,7 +3467,7 @@
       </c>
       <c r="N5" s="42"/>
     </row>
-    <row r="6" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="117"/>
       <c r="C6" s="115"/>
       <c r="D6" s="1" t="s">
@@ -3313,10 +3494,10 @@
       </c>
       <c r="N6" s="43"/>
     </row>
-    <row r="7" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="118"/>
       <c r="C7" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>30</v>
@@ -3344,12 +3525,12 @@
       </c>
       <c r="N7" s="44"/>
     </row>
-    <row r="8" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="111" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>30</v>
@@ -3377,10 +3558,10 @@
       </c>
       <c r="N8" s="45"/>
     </row>
-    <row r="9" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="113"/>
       <c r="C9" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>30</v>
@@ -3408,12 +3589,12 @@
       </c>
       <c r="N9" s="46"/>
     </row>
-    <row r="10" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="111" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>30</v>
@@ -3439,10 +3620,10 @@
       </c>
       <c r="N10" s="47"/>
     </row>
-    <row r="11" spans="2:14" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="112"/>
       <c r="C11" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
@@ -3464,10 +3645,10 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="2:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="112"/>
       <c r="C12" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
@@ -3492,7 +3673,7 @@
     <row r="13" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="112"/>
       <c r="C13" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>30</v>
@@ -3517,7 +3698,7 @@
     <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="112"/>
       <c r="C14" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>36</v>
@@ -3538,13 +3719,13 @@
         <v>35</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="112"/>
       <c r="C15" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
@@ -3565,13 +3746,13 @@
         <v>35</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="112"/>
       <c r="C16" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>36</v>
@@ -3592,13 +3773,13 @@
         <v>35</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="112"/>
       <c r="C17" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>36</v>
@@ -3619,13 +3800,13 @@
         <v>35</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="112"/>
       <c r="C18" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>36</v>
@@ -3646,13 +3827,13 @@
         <v>35</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="112"/>
       <c r="C19" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>46</v>
@@ -3677,7 +3858,7 @@
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="112"/>
       <c r="C20" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>46</v>
@@ -3702,7 +3883,7 @@
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="112"/>
       <c r="C21" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
@@ -3727,7 +3908,7 @@
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="112"/>
       <c r="C22" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>46</v>
@@ -3752,7 +3933,7 @@
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="112"/>
       <c r="C23" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>46</v>
@@ -3777,7 +3958,7 @@
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="112"/>
       <c r="C24" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>46</v>
@@ -3802,7 +3983,7 @@
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="112"/>
       <c r="C25" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>46</v>
@@ -3827,7 +4008,7 @@
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="112"/>
       <c r="C26" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>46</v>
@@ -3852,7 +4033,7 @@
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="112"/>
       <c r="C27" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>46</v>
@@ -3877,7 +4058,7 @@
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="112"/>
       <c r="C28" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>46</v>
@@ -3902,7 +4083,7 @@
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="112"/>
       <c r="C29" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>46</v>
@@ -3927,19 +4108,19 @@
     <row r="30" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="113"/>
       <c r="C30" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F30" s="10">
         <v>0.85589999999999999</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>34</v>
@@ -3949,12 +4130,12 @@
       </c>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="2:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="111" t="s">
         <v>68</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>30</v>
@@ -3978,10 +4159,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="112"/>
       <c r="C32" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>30</v>
@@ -4003,10 +4184,10 @@
       </c>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="112"/>
       <c r="C33" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>30</v>
@@ -4028,10 +4209,10 @@
       </c>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="112"/>
       <c r="C34" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>30</v>
@@ -4053,10 +4234,10 @@
       </c>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="112"/>
       <c r="C35" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>30</v>
@@ -4078,10 +4259,10 @@
       </c>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="112"/>
       <c r="C36" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>30</v>
@@ -4103,10 +4284,10 @@
       </c>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B37" s="112"/>
       <c r="C37" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>30</v>
@@ -4130,16 +4311,16 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" s="112"/>
       <c r="C38" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>79</v>
+        <v>349</v>
       </c>
       <c r="F38" s="2">
         <v>0.9042</v>
@@ -4154,25 +4335,25 @@
         <v>73</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="112"/>
       <c r="C39" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F39" s="2">
         <v>0.91830000000000001</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>34</v>
@@ -4182,22 +4363,22 @@
       </c>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" s="112"/>
       <c r="C40" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F40" s="2">
         <v>0.9204</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>34</v>
@@ -4206,25 +4387,25 @@
         <v>35</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="112"/>
       <c r="C41" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" s="2">
         <v>0.91979999999999995</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>34</v>
@@ -4234,22 +4415,22 @@
       </c>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="112"/>
       <c r="C42" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F42" s="2">
         <v>0.91820000000000002</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>34</v>
@@ -4259,22 +4440,22 @@
       </c>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" s="112"/>
       <c r="C43" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F43" s="2">
         <v>0.90639999999999998</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>34</v>
@@ -4284,22 +4465,22 @@
       </c>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="2:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B44" s="112"/>
       <c r="C44" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F44" s="2">
         <v>0.91010000000000002</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>34</v>
@@ -4309,22 +4490,22 @@
       </c>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B45" s="112"/>
       <c r="C45" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F45" s="2">
         <v>0.92069999999999996</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>34</v>
@@ -4334,22 +4515,22 @@
       </c>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="2:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="112"/>
       <c r="C46" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46" s="2">
         <v>0.88849999999999996</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>34</v>
@@ -4362,19 +4543,19 @@
     <row r="47" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B47" s="112"/>
       <c r="C47" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F47" s="2">
         <v>0.92730000000000001</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>34</v>
@@ -4383,25 +4564,25 @@
         <v>35</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B48" s="112"/>
       <c r="C48" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F48" s="2">
         <v>0.92849999999999999</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>34</v>
@@ -4411,22 +4592,22 @@
       </c>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="2:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B49" s="112"/>
       <c r="C49" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F49" s="2">
         <v>0.91579999999999995</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>34</v>
@@ -4437,30 +4618,30 @@
     <row r="50" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" s="112"/>
       <c r="C50" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F50" s="2">
         <v>0.91810000000000003</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" s="112"/>
       <c r="C51" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>36</v>
@@ -4472,7 +4653,7 @@
         <v>0.69769999999999999</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>34</v>
@@ -4481,13 +4662,13 @@
         <v>35</v>
       </c>
       <c r="J51" s="70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" s="112"/>
       <c r="C52" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>36</v>
@@ -4499,7 +4680,7 @@
         <v>0.84519999999999995</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>34</v>
@@ -4508,13 +4689,13 @@
         <v>35</v>
       </c>
       <c r="J52" s="70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" s="112"/>
       <c r="C53" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>36</v>
@@ -4526,7 +4707,7 @@
         <v>0.88180000000000003</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>34</v>
@@ -4535,13 +4716,13 @@
         <v>35</v>
       </c>
       <c r="J53" s="70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B54" s="112"/>
       <c r="C54" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>36</v>
@@ -4553,7 +4734,7 @@
         <v>0.19670000000000001</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>34</v>
@@ -4562,13 +4743,13 @@
         <v>35</v>
       </c>
       <c r="J54" s="70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" s="112"/>
       <c r="C55" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>36</v>
@@ -4589,13 +4770,13 @@
         <v>35</v>
       </c>
       <c r="J55" s="70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B56" s="112"/>
       <c r="C56" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>46</v>
@@ -4607,22 +4788,22 @@
         <v>0.50349999999999995</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J56" s="107" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" s="112"/>
       <c r="C57" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>46</v>
@@ -4634,20 +4815,20 @@
         <v>0.45710000000000001</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J57" s="107"/>
     </row>
     <row r="58" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B58" s="112"/>
       <c r="C58" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>46</v>
@@ -4659,20 +4840,20 @@
         <v>0.41149999999999998</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J58" s="107"/>
     </row>
     <row r="59" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B59" s="112"/>
       <c r="C59" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>46</v>
@@ -4684,20 +4865,20 @@
         <v>0.34549999999999997</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J59" s="107"/>
     </row>
     <row r="60" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="112"/>
       <c r="C60" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>46</v>
@@ -4706,23 +4887,23 @@
         <v>52</v>
       </c>
       <c r="F60" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J60" s="107"/>
     </row>
     <row r="61" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" s="112"/>
       <c r="C61" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>46</v>
@@ -4731,23 +4912,23 @@
         <v>53</v>
       </c>
       <c r="F61" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J61" s="107"/>
     </row>
     <row r="62" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="112"/>
       <c r="C62" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>46</v>
@@ -4756,23 +4937,23 @@
         <v>55</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J62" s="107"/>
     </row>
     <row r="63" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B63" s="112"/>
       <c r="C63" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>46</v>
@@ -4781,23 +4962,23 @@
         <v>57</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J63" s="107"/>
     </row>
     <row r="64" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B64" s="112"/>
       <c r="C64" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>46</v>
@@ -4806,23 +4987,23 @@
         <v>59</v>
       </c>
       <c r="F64" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J64" s="107"/>
     </row>
     <row r="65" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B65" s="112"/>
       <c r="C65" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>46</v>
@@ -4831,23 +5012,23 @@
         <v>62</v>
       </c>
       <c r="F65" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J65" s="107"/>
     </row>
-    <row r="66" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="112"/>
       <c r="C66" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>46</v>
@@ -4856,35 +5037,35 @@
         <v>65</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J66" s="107"/>
     </row>
-    <row r="67" spans="2:10" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="112"/>
       <c r="C67" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F67" s="2">
         <v>0.92459999999999998</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>34</v>
@@ -4894,22 +5075,22 @@
       </c>
       <c r="J67" s="107"/>
     </row>
-    <row r="68" spans="2:10" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="112"/>
       <c r="C68" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F68" s="2">
         <v>0.91800000000000004</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>34</v>
@@ -4919,47 +5100,47 @@
       </c>
       <c r="J68" s="107"/>
     </row>
-    <row r="69" spans="2:10" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="112"/>
       <c r="C69" s="29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F69" s="2">
         <v>0.92310000000000003</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J69" s="107"/>
     </row>
-    <row r="70" spans="2:10" ht="64" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B70" s="113"/>
       <c r="C70" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F70" s="16">
         <v>0.90859999999999996</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>34</v>
@@ -4969,54 +5150,54 @@
       </c>
       <c r="J70" s="107"/>
     </row>
-    <row r="71" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="108" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C71" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F71" s="6">
         <v>0.92759999999999998</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="107"/>
     </row>
-    <row r="72" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="109"/>
       <c r="C72" s="51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F72" s="2">
         <v>0.92759999999999998</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="107"/>
     </row>
-    <row r="73" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="109"/>
       <c r="C73" s="51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="1"/>
@@ -5024,14 +5205,14 @@
       <c r="I73" s="1"/>
       <c r="J73" s="107"/>
     </row>
-    <row r="74" spans="2:10" ht="18" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B74" s="110"/>
       <c r="C74" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F74" s="10"/>
       <c r="G74" s="9"/>
@@ -5041,16 +5222,16 @@
     </row>
     <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B75" s="111" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C75" s="48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F75" s="31">
         <v>0.84760000000000002</v>
@@ -5062,20 +5243,20 @@
         <v>34</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J75" s="107"/>
     </row>
     <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B76" s="112"/>
       <c r="C76" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F76" s="2">
         <v>0.80649999999999999</v>
@@ -5087,20 +5268,20 @@
         <v>34</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B77" s="112"/>
       <c r="C77" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F77" s="2">
         <v>0.84240000000000004</v>
@@ -5112,28 +5293,28 @@
         <v>34</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B78" s="112"/>
       <c r="C78" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F78" s="2">
         <v>0.84250000000000003</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>34</v>
@@ -5146,19 +5327,19 @@
     <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B79" s="112"/>
       <c r="C79" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F79" s="2">
         <v>0.85909999999999997</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>34</v>
@@ -5167,19 +5348,19 @@
         <v>35</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B80" s="112"/>
       <c r="C80" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F80" s="2">
         <v>0.84889999999999999</v>
@@ -5189,20 +5370,20 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B81" s="112"/>
       <c r="C81" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>220</v>
       </c>
       <c r="F81" s="16">
         <v>0.91720000000000002</v>
@@ -5212,20 +5393,20 @@
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B82" s="112"/>
       <c r="C82" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F82" s="2">
         <v>0.87190000000000001</v>
@@ -5236,13 +5417,13 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B83" s="112"/>
       <c r="C83" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>46</v>
@@ -5259,19 +5440,19 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B84" s="112"/>
       <c r="C84" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F84" s="2">
         <v>0.6804</v>
@@ -5282,7 +5463,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
@@ -5497,13 +5678,13 @@
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D5:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5513,49 +5694,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E30"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="84"/>
-    <col min="8" max="8" width="59.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="45.5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="84"/>
+    <col min="9" max="9" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="54"/>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
       <c r="D1" s="54"/>
       <c r="E1" s="54"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="54"/>
       <c r="I1" s="54"/>
       <c r="J1" s="54"/>
-    </row>
-    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="54"/>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54"/>
       <c r="B2" s="122" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C2" s="122"/>
       <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="81"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="81"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="36" t="s">
+      <c r="I2" s="81"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="38"/>
-    </row>
-    <row r="3" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="38"/>
+    </row>
+    <row r="3" spans="1:12" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54"/>
       <c r="B3" s="56" t="s">
         <v>4</v>
@@ -5567,970 +5753,1611 @@
         <v>6</v>
       </c>
       <c r="E3" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="G3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="H3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="I3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="54"/>
+      <c r="K3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="39"/>
-    </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L3" s="39"/>
+    </row>
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="54"/>
       <c r="B4" s="119" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="85" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D4" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="87" t="s">
-        <v>232</v>
-      </c>
-      <c r="F4" s="88">
+      <c r="E4" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>354</v>
+      </c>
+      <c r="G4" s="88">
         <v>0.36480000000000001</v>
       </c>
-      <c r="G4" s="87" t="s">
-        <v>231</v>
-      </c>
-      <c r="H4" s="89" t="s">
-        <v>253</v>
-      </c>
-      <c r="I4" s="54"/>
-      <c r="J4" s="36" t="s">
+      <c r="H4" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="I4" s="89" t="s">
+        <v>250</v>
+      </c>
+      <c r="J4" s="54"/>
+      <c r="K4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="40"/>
-    </row>
-    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L4" s="40"/>
+    </row>
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="54"/>
       <c r="B5" s="120"/>
       <c r="C5" s="137" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="151" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="139" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" s="140" t="s">
+        <v>319</v>
+      </c>
+      <c r="H5" s="139" t="s">
         <v>320</v>
       </c>
-      <c r="D5" s="151" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="139" t="s">
-        <v>272</v>
-      </c>
-      <c r="F5" s="140" t="s">
-        <v>325</v>
-      </c>
-      <c r="G5" s="139" t="s">
-        <v>326</v>
-      </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54" t="s">
+      <c r="I5" s="141"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="41"/>
-    </row>
-    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L5" s="41"/>
+    </row>
+    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="54"/>
       <c r="B6" s="120"/>
       <c r="C6" s="85" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D6" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="85" t="s">
+        <v>355</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>248</v>
+      </c>
+      <c r="G6" s="88">
+        <v>0.65839999999999999</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>242</v>
+      </c>
+      <c r="I6" s="89" t="s">
         <v>251</v>
       </c>
-      <c r="F6" s="88">
-        <v>0.65839999999999999</v>
-      </c>
-      <c r="G6" s="87" t="s">
-        <v>244</v>
-      </c>
-      <c r="H6" s="89" t="s">
-        <v>254</v>
-      </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="54"/>
+      <c r="K6" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="149"/>
-    </row>
-    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L6" s="149"/>
+    </row>
+    <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="54"/>
       <c r="B7" s="120"/>
       <c r="C7" s="85" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D7" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="87" t="s">
-        <v>252</v>
-      </c>
-      <c r="F7" s="88">
+      <c r="E7" s="85" t="s">
+        <v>355</v>
+      </c>
+      <c r="F7" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="88">
         <v>0.65269999999999995</v>
       </c>
-      <c r="G7" s="87" t="s">
-        <v>245</v>
-      </c>
-      <c r="H7" s="89" t="s">
-        <v>254</v>
-      </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="36" t="s">
+      <c r="H7" s="87" t="s">
+        <v>243</v>
+      </c>
+      <c r="I7" s="89" t="s">
+        <v>251</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="150"/>
-    </row>
-    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L7" s="150"/>
+    </row>
+    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
       <c r="B8" s="120"/>
       <c r="C8" s="93" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D8" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="95" t="s">
-        <v>270</v>
-      </c>
-      <c r="F8" s="96">
+      <c r="E8" s="93" t="s">
+        <v>355</v>
+      </c>
+      <c r="F8" s="95" t="s">
+        <v>267</v>
+      </c>
+      <c r="G8" s="96">
         <v>0.73540000000000005</v>
       </c>
-      <c r="G8" s="95" t="s">
+      <c r="H8" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="97" t="s">
-        <v>288</v>
-      </c>
-      <c r="I8" s="54"/>
+      <c r="I8" s="97" t="s">
+        <v>282</v>
+      </c>
       <c r="J8" s="54"/>
-    </row>
-    <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="K8" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="155"/>
+    </row>
+    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
       <c r="B9" s="120"/>
       <c r="C9" s="137" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D9" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="139" t="s">
-        <v>273</v>
-      </c>
-      <c r="F9" s="140">
+      <c r="E9" s="137" t="s">
+        <v>355</v>
+      </c>
+      <c r="F9" s="139" t="s">
+        <v>269</v>
+      </c>
+      <c r="G9" s="140">
         <v>0.74019999999999997</v>
       </c>
-      <c r="G9" s="139" t="s">
-        <v>332</v>
-      </c>
-      <c r="H9" s="141"/>
-      <c r="I9" s="54"/>
+      <c r="H9" s="139" t="s">
+        <v>326</v>
+      </c>
+      <c r="I9" s="141"/>
       <c r="J9" s="54"/>
-    </row>
-    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K9" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="161"/>
+    </row>
+    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
       <c r="B10" s="120"/>
       <c r="C10" s="100" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D10" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="102" t="s">
-        <v>302</v>
-      </c>
-      <c r="F10" s="103">
+      <c r="E10" s="100" t="s">
+        <v>355</v>
+      </c>
+      <c r="F10" s="102" t="s">
+        <v>296</v>
+      </c>
+      <c r="G10" s="103">
         <v>0.46329999999999999</v>
       </c>
-      <c r="G10" s="144" t="s">
-        <v>324</v>
-      </c>
-      <c r="H10" s="104" t="s">
-        <v>293</v>
-      </c>
-      <c r="I10" s="54"/>
+      <c r="H10" s="144" t="s">
+        <v>318</v>
+      </c>
+      <c r="I10" s="104" t="s">
+        <v>287</v>
+      </c>
       <c r="J10" s="54"/>
-    </row>
-    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
       <c r="B11" s="120"/>
       <c r="C11" s="100" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D11" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="102" t="s">
-        <v>303</v>
-      </c>
-      <c r="F11" s="103">
+      <c r="E11" s="100" t="s">
+        <v>355</v>
+      </c>
+      <c r="F11" s="102" t="s">
+        <v>297</v>
+      </c>
+      <c r="G11" s="103">
         <v>0.62519999999999998</v>
       </c>
-      <c r="G11" s="102" t="s">
-        <v>330</v>
-      </c>
-      <c r="H11" s="104" t="s">
-        <v>293</v>
-      </c>
-      <c r="I11" s="54"/>
+      <c r="H11" s="102" t="s">
+        <v>324</v>
+      </c>
+      <c r="I11" s="104" t="s">
+        <v>287</v>
+      </c>
       <c r="J11" s="54"/>
-    </row>
-    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K11" s="54"/>
+    </row>
+    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="54"/>
       <c r="B12" s="120"/>
       <c r="C12" s="100" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D12" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="F12" s="103">
+      <c r="E12" s="100" t="s">
+        <v>355</v>
+      </c>
+      <c r="F12" s="102" t="s">
+        <v>298</v>
+      </c>
+      <c r="G12" s="103">
         <v>0.69059999999999999</v>
       </c>
-      <c r="G12" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="H12" s="104" t="s">
-        <v>293</v>
-      </c>
-      <c r="I12" s="54"/>
+      <c r="H12" s="102" t="s">
+        <v>325</v>
+      </c>
+      <c r="I12" s="104" t="s">
+        <v>287</v>
+      </c>
       <c r="J12" s="54"/>
-    </row>
-    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K12" s="54"/>
+    </row>
+    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
       <c r="B13" s="120"/>
       <c r="C13" s="130" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D13" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="132" t="s">
+      <c r="E13" s="130" t="s">
+        <v>355</v>
+      </c>
+      <c r="F13" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="133">
+      <c r="G13" s="133">
         <v>0.13159999999999999</v>
       </c>
-      <c r="G13" s="134" t="s">
+      <c r="H13" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="135"/>
-      <c r="I13" s="54"/>
+      <c r="I13" s="135"/>
       <c r="J13" s="54"/>
-    </row>
-    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K13" s="54"/>
+    </row>
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
       <c r="B14" s="120"/>
       <c r="C14" s="130" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D14" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="132" t="s">
+      <c r="E14" s="130" t="s">
+        <v>355</v>
+      </c>
+      <c r="F14" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="133">
+      <c r="G14" s="133">
         <v>5.57E-2</v>
       </c>
-      <c r="G14" s="134" t="s">
+      <c r="H14" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="135"/>
-      <c r="I14" s="54"/>
+      <c r="I14" s="135"/>
       <c r="J14" s="54"/>
-    </row>
-    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K14" s="54"/>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
       <c r="B15" s="120"/>
       <c r="C15" s="130" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D15" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="132" t="s">
+      <c r="E15" s="130" t="s">
+        <v>355</v>
+      </c>
+      <c r="F15" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="133">
+      <c r="G15" s="133">
         <v>3.6200000000000003E-2</v>
       </c>
-      <c r="G15" s="134" t="s">
+      <c r="H15" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="135"/>
-      <c r="I15" s="54"/>
+      <c r="I15" s="135"/>
       <c r="J15" s="54"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K15" s="54"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
       <c r="B16" s="120"/>
       <c r="C16" s="64"/>
       <c r="D16" s="61"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="54"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="63"/>
       <c r="J16" s="54"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="54"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
       <c r="B17" s="120"/>
       <c r="C17" s="64"/>
       <c r="D17" s="61"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="54"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="63"/>
       <c r="J17" s="54"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="54"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
       <c r="B18" s="120"/>
       <c r="C18" s="64"/>
       <c r="D18" s="61"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="54"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="63"/>
       <c r="J18" s="54"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="54"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
       <c r="B19" s="120"/>
       <c r="C19" s="64"/>
       <c r="D19" s="61"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="54"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="63"/>
       <c r="J19" s="54"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="54"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="B20" s="120"/>
       <c r="C20" s="64"/>
       <c r="D20" s="61"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="54"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="63"/>
       <c r="J20" s="54"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="54"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="B21" s="120"/>
       <c r="C21" s="64"/>
       <c r="D21" s="61"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="54"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="63"/>
       <c r="J21" s="54"/>
-    </row>
-    <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="54"/>
+    </row>
+    <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="54"/>
       <c r="B22" s="121"/>
       <c r="C22" s="65"/>
       <c r="D22" s="66"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="54"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="69"/>
       <c r="J22" s="54"/>
-    </row>
-    <row r="23" spans="1:10" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="54"/>
+    </row>
+    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="123" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" s="50" t="s">
         <v>235</v>
       </c>
-      <c r="C23" s="50" t="s">
-        <v>237</v>
-      </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="E23" s="12"/>
+      <c r="F23" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G23" s="6">
         <v>47.49</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="5"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="124"/>
       <c r="C24" s="51" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="E24" s="13"/>
+      <c r="F24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G24" s="2">
         <v>47.49</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="1"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="124"/>
       <c r="C25" s="51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="E25" s="13"/>
+      <c r="F25" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G25" s="2">
         <v>6.7</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="125"/>
       <c r="C26" s="83" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F26" s="16">
+      <c r="E26" s="15"/>
+      <c r="F26" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G26" s="16">
         <v>6.7</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="53"/>
-    </row>
-    <row r="27" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="4"/>
+      <c r="I26" s="53"/>
+    </row>
+    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="119" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D27" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="91" t="s">
-        <v>247</v>
-      </c>
-      <c r="F27" s="92">
+      <c r="E27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="91" t="s">
+        <v>356</v>
+      </c>
+      <c r="G27" s="92">
         <v>0.27600000000000002</v>
       </c>
-      <c r="G27" s="91">
+      <c r="H27" s="91">
         <v>50</v>
       </c>
-      <c r="H27" s="91" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="I27" s="91" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="120"/>
       <c r="C28" s="22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D28" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="98" t="s">
-        <v>271</v>
-      </c>
-      <c r="F28" s="99">
+      <c r="E28" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="98" t="s">
+        <v>357</v>
+      </c>
+      <c r="G28" s="99">
         <v>0.52239999999999998</v>
       </c>
-      <c r="G28" s="98" t="s">
-        <v>285</v>
-      </c>
       <c r="H28" s="98" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+      <c r="I28" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="120"/>
       <c r="C29" s="22" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D29" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="98" t="s">
-        <v>277</v>
-      </c>
-      <c r="F29" s="99">
+      <c r="E29" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="F29" s="98" t="s">
+        <v>358</v>
+      </c>
+      <c r="G29" s="99">
         <v>0.69030000000000002</v>
       </c>
-      <c r="G29" s="98" t="s">
-        <v>286</v>
-      </c>
       <c r="H29" s="98" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+      <c r="I29" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="120"/>
       <c r="C30" s="13"/>
       <c r="D30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="1"/>
+      <c r="E30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G30" s="2"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="120"/>
       <c r="C31" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="D31" s="142" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="F31" s="142" t="s">
+        <v>360</v>
+      </c>
+      <c r="G31" s="143">
+        <v>0.67720000000000002</v>
+      </c>
+      <c r="H31" s="142" t="s">
         <v>322</v>
       </c>
-      <c r="D31" s="142" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="142" t="s">
-        <v>280</v>
-      </c>
-      <c r="F31" s="143">
-        <v>0.67720000000000002</v>
-      </c>
-      <c r="G31" s="142" t="s">
-        <v>328</v>
-      </c>
-      <c r="H31" s="142" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="I31" s="142" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="120"/>
       <c r="C32" s="23" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D32" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="102" t="s">
-        <v>305</v>
-      </c>
-      <c r="F32" s="105">
+      <c r="E32" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="F32" s="102" t="s">
+        <v>299</v>
+      </c>
+      <c r="G32" s="105">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="G32" s="106" t="s">
-        <v>327</v>
-      </c>
-      <c r="H32" s="104" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H32" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="I32" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="120"/>
       <c r="C33" s="23" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D33" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="102" t="s">
-        <v>306</v>
-      </c>
-      <c r="F33" s="105">
+      <c r="E33" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="F33" s="102" t="s">
+        <v>300</v>
+      </c>
+      <c r="G33" s="105">
         <v>0.1991</v>
       </c>
-      <c r="G33" s="106" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="104" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H33" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="120"/>
       <c r="C34" s="23" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D34" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="102" t="s">
-        <v>307</v>
-      </c>
-      <c r="F34" s="105">
+      <c r="E34" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="F34" s="102" t="s">
+        <v>301</v>
+      </c>
+      <c r="G34" s="105">
         <v>0.56259999999999999</v>
       </c>
-      <c r="G34" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H34" s="104" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H34" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="120"/>
       <c r="C35" s="24" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D35" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="132" t="s">
+      <c r="E35" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="F35" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="136">
+      <c r="G35" s="136">
         <v>0.1024</v>
       </c>
-      <c r="G35" s="132" t="s">
-        <v>286</v>
-      </c>
-      <c r="H35" s="132"/>
-    </row>
-    <row r="36" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H35" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="I35" s="132"/>
+    </row>
+    <row r="36" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="120"/>
       <c r="C36" s="24" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D36" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="132" t="s">
+      <c r="E36" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="F36" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="136">
+      <c r="G36" s="136">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G36" s="132" t="s">
-        <v>286</v>
-      </c>
-      <c r="H36" s="132"/>
-    </row>
-    <row r="37" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H36" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="I36" s="132"/>
+    </row>
+    <row r="37" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" s="120"/>
       <c r="C37" s="24" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D37" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="132" t="s">
+      <c r="E37" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="F37" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="136">
+      <c r="G37" s="136">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="G37" s="132"/>
-      <c r="H37" s="132"/>
-    </row>
-    <row r="38" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H37" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="I37" s="132"/>
+    </row>
+    <row r="38" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" s="120"/>
       <c r="C38" s="26" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D38" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="147" t="s">
-        <v>338</v>
-      </c>
-      <c r="F38" s="148"/>
-      <c r="G38" s="147"/>
+      <c r="E38" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="F38" s="147" t="s">
+        <v>332</v>
+      </c>
+      <c r="G38" s="148">
+        <v>1.9699999999999999E-2</v>
+      </c>
       <c r="H38" s="147"/>
-    </row>
-    <row r="39" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I38" s="147" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="120"/>
       <c r="C39" s="26" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D39" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="147" t="s">
-        <v>339</v>
-      </c>
-      <c r="F39" s="148"/>
-      <c r="G39" s="147"/>
+      <c r="E39" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="147" t="s">
+        <v>333</v>
+      </c>
+      <c r="G39" s="148">
+        <v>2.0199999999999999E-2</v>
+      </c>
       <c r="H39" s="147"/>
-    </row>
-    <row r="40" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I39" s="147" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" s="120"/>
       <c r="C40" s="26" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D40" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="147" t="s">
-        <v>340</v>
-      </c>
-      <c r="F40" s="148"/>
-      <c r="G40" s="147"/>
-      <c r="H40" s="147"/>
-    </row>
-    <row r="41" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="E40" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="F40" s="147" t="s">
+        <v>334</v>
+      </c>
+      <c r="G40" s="148">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="H40" s="147" t="s">
+        <v>338</v>
+      </c>
+      <c r="I40" s="147"/>
+    </row>
+    <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="120"/>
       <c r="C41" s="26" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D41" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E41" s="147" t="s">
+      <c r="E41" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="147" t="s">
+        <v>335</v>
+      </c>
+      <c r="G41" s="148">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="H41" s="147" t="s">
+        <v>336</v>
+      </c>
+      <c r="I41" s="147"/>
+    </row>
+    <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B42" s="120"/>
+      <c r="C42" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="D42" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F42" s="153" t="s">
+        <v>344</v>
+      </c>
+      <c r="G42" s="154">
+        <v>0.69550000000000001</v>
+      </c>
+      <c r="H42" s="153" t="s">
+        <v>280</v>
+      </c>
+      <c r="I42" s="153" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B43" s="120"/>
+      <c r="C43" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="D43" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F43" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="G43" s="154">
+        <v>0.69850000000000001</v>
+      </c>
+      <c r="H43" s="153" t="s">
+        <v>336</v>
+      </c>
+      <c r="I43" s="153"/>
+    </row>
+    <row r="44" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="120"/>
+      <c r="C44" s="27" t="s">
         <v>341</v>
       </c>
-      <c r="F41" s="148"/>
-      <c r="G41" s="147"/>
-      <c r="H41" s="147"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="120"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="121"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B44" s="119" t="s">
-        <v>248</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>276</v>
-      </c>
-      <c r="D44" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="E44" s="98" t="s">
-        <v>281</v>
-      </c>
-      <c r="F44" s="99">
-        <v>0.4929</v>
-      </c>
-      <c r="G44" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="H44" s="98" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="D44" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="153" t="s">
+        <v>343</v>
+      </c>
+      <c r="G44" s="154">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="H44" s="153" t="s">
+        <v>97</v>
+      </c>
+      <c r="I44" s="153"/>
+    </row>
+    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B45" s="120"/>
-      <c r="C45" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="D45" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" s="98" t="s">
-        <v>283</v>
-      </c>
-      <c r="F45" s="99">
-        <v>0.66930000000000001</v>
-      </c>
-      <c r="G45" s="98" t="s">
-        <v>287</v>
-      </c>
-      <c r="H45" s="98" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="C45" s="13"/>
+      <c r="D45" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="120"/>
       <c r="C46" s="13"/>
-      <c r="D46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="D46" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B47" s="120"/>
+      <c r="C47" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D47" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F47" s="153" t="s">
+        <v>352</v>
+      </c>
+      <c r="G47" s="154">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="H47" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="I47" s="153" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="120"/>
+      <c r="C48" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D48" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="153" t="s">
+        <v>361</v>
+      </c>
+      <c r="G48" s="154">
+        <v>0.55220000000000002</v>
+      </c>
+      <c r="H48" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="I48" s="153" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B49" s="120"/>
+      <c r="C49" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="D49" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F49" s="153" t="s">
+        <v>350</v>
+      </c>
+      <c r="G49" s="154">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="H49" s="153" t="s">
+        <v>97</v>
+      </c>
+      <c r="I49" s="153" t="s">
         <v>282</v>
       </c>
-      <c r="F46" s="2"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B47" s="120"/>
-      <c r="C47" s="25" t="s">
+    </row>
+    <row r="50" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B50" s="120"/>
+      <c r="C50" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="D50" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="153" t="s">
+        <v>351</v>
+      </c>
+      <c r="G50" s="154">
+        <v>0.51180000000000003</v>
+      </c>
+      <c r="H50" s="153" t="s">
+        <v>322</v>
+      </c>
+      <c r="I50" s="153" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B51" s="120"/>
+      <c r="C51" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="D51" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F51" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="G51" s="159"/>
+      <c r="H51" s="158"/>
+      <c r="I51" s="158"/>
+    </row>
+    <row r="52" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B52" s="120"/>
+      <c r="C52" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="D52" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" s="160" t="s">
+        <v>373</v>
+      </c>
+      <c r="G52" s="159"/>
+      <c r="H52" s="158"/>
+      <c r="I52" s="158"/>
+    </row>
+    <row r="53" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B53" s="120"/>
+      <c r="C53" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="D53" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F53" s="160" t="s">
+        <v>376</v>
+      </c>
+      <c r="G53" s="159"/>
+      <c r="H53" s="158"/>
+      <c r="I53" s="158"/>
+    </row>
+    <row r="54" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B54" s="120"/>
+      <c r="C54" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="D54" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" s="160" t="s">
+        <v>382</v>
+      </c>
+      <c r="G54" s="159"/>
+      <c r="H54" s="158"/>
+      <c r="I54" s="158"/>
+    </row>
+    <row r="55" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B55" s="120"/>
+      <c r="C55" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="D55" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F55" s="160" t="s">
+        <v>377</v>
+      </c>
+      <c r="G55" s="159"/>
+      <c r="H55" s="158"/>
+      <c r="I55" s="158"/>
+    </row>
+    <row r="56" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B56" s="120"/>
+      <c r="C56" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="D56" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="160" t="s">
+        <v>383</v>
+      </c>
+      <c r="G56" s="159"/>
+      <c r="H56" s="158"/>
+      <c r="I56" s="158"/>
+    </row>
+    <row r="57" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B57" s="120"/>
+      <c r="C57" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="D57" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F57" s="158" t="s">
+        <v>368</v>
+      </c>
+      <c r="G57" s="159"/>
+      <c r="H57" s="158"/>
+      <c r="I57" s="158"/>
+    </row>
+    <row r="58" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B58" s="120"/>
+      <c r="C58" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="D58" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="158" t="s">
+        <v>369</v>
+      </c>
+      <c r="G58" s="159"/>
+      <c r="H58" s="158"/>
+      <c r="I58" s="158"/>
+    </row>
+    <row r="59" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B59" s="120"/>
+      <c r="C59" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="D59" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F59" s="158" t="s">
+        <v>384</v>
+      </c>
+      <c r="G59" s="159"/>
+      <c r="H59" s="158"/>
+      <c r="I59" s="158"/>
+    </row>
+    <row r="60" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" s="120"/>
+      <c r="C60" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="D60" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="158" t="s">
+        <v>385</v>
+      </c>
+      <c r="G60" s="159"/>
+      <c r="H60" s="158"/>
+      <c r="I60" s="158"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61" s="120"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="120"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="120"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B64" s="120"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="120"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="120"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="120"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="120"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="60"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B69" s="120"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="60"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="120"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="61"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="120"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="61"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="120"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="120"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="120"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="121"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B76" s="119" t="s">
+        <v>245</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D76" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="22"/>
+      <c r="F76" s="98" t="s">
+        <v>275</v>
+      </c>
+      <c r="G76" s="99">
+        <v>0.4929</v>
+      </c>
+      <c r="H76" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="I76" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B77" s="120"/>
+      <c r="C77" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="D77" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="22"/>
+      <c r="F77" s="98" t="s">
+        <v>277</v>
+      </c>
+      <c r="G77" s="99">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="H77" s="98" t="s">
+        <v>281</v>
+      </c>
+      <c r="I77" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B78" s="120"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="13"/>
+      <c r="F78" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G78" s="2"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B79" s="120"/>
+      <c r="C79" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="D79" s="142" t="s">
+        <v>30</v>
+      </c>
+      <c r="E79" s="25"/>
+      <c r="F79" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G79" s="143">
+        <v>0.67969999999999997</v>
+      </c>
+      <c r="H79" s="142" t="s">
+        <v>327</v>
+      </c>
+      <c r="I79" s="142"/>
+    </row>
+    <row r="80" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B80" s="120"/>
+      <c r="C80" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="D80" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="23"/>
+      <c r="F80" s="102" t="s">
+        <v>302</v>
+      </c>
+      <c r="G80" s="105">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H80" s="145" t="s">
         <v>323</v>
       </c>
-      <c r="D47" s="142" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="142" t="s">
-        <v>284</v>
-      </c>
-      <c r="F47" s="143">
-        <v>0.67969999999999997</v>
-      </c>
-      <c r="G47" s="142" t="s">
-        <v>333</v>
-      </c>
-      <c r="H47" s="142"/>
-    </row>
-    <row r="48" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B48" s="120"/>
-      <c r="C48" s="23" t="s">
-        <v>299</v>
-      </c>
-      <c r="D48" s="101" t="s">
+      <c r="I80" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B81" s="120"/>
+      <c r="C81" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="D81" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="102" t="s">
-        <v>308</v>
-      </c>
-      <c r="F48" s="105">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="G48" s="145" t="s">
-        <v>329</v>
-      </c>
-      <c r="H48" s="104" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B49" s="120"/>
-      <c r="C49" s="23" t="s">
-        <v>300</v>
-      </c>
-      <c r="D49" s="101" t="s">
+      <c r="E81" s="23"/>
+      <c r="F81" s="102" t="s">
+        <v>303</v>
+      </c>
+      <c r="G81" s="105">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="H81" s="106">
+        <v>50</v>
+      </c>
+      <c r="I81" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B82" s="120"/>
+      <c r="C82" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="D82" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="102" t="s">
-        <v>309</v>
-      </c>
-      <c r="F49" s="105">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="G49" s="106">
+      <c r="E82" s="23"/>
+      <c r="F82" s="102" t="s">
+        <v>304</v>
+      </c>
+      <c r="G82" s="105">
+        <v>0.54239999999999999</v>
+      </c>
+      <c r="H82" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="I82" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B83" s="120"/>
+      <c r="C83" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D83" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="24"/>
+      <c r="F83" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" s="136">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="H83" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I83" s="132"/>
+    </row>
+    <row r="84" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B84" s="120"/>
+      <c r="C84" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="D84" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E84" s="24"/>
+      <c r="F84" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="G84" s="136">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="H84" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I84" s="132"/>
+    </row>
+    <row r="85" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B85" s="120"/>
+      <c r="C85" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D85" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" s="24"/>
+      <c r="F85" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="H49" s="104" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="120"/>
-      <c r="C50" s="23" t="s">
-        <v>301</v>
-      </c>
-      <c r="D50" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="102" t="s">
-        <v>310</v>
-      </c>
-      <c r="F50" s="105">
-        <v>0.54239999999999999</v>
-      </c>
-      <c r="G50" s="106" t="s">
-        <v>327</v>
-      </c>
-      <c r="H50" s="104" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="120"/>
-      <c r="C51" s="24" t="s">
-        <v>317</v>
-      </c>
-      <c r="D51" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="132" t="s">
-        <v>47</v>
-      </c>
-      <c r="F51" s="136">
-        <v>7.7899999999999997E-2</v>
-      </c>
-      <c r="G51" s="132" t="s">
-        <v>287</v>
-      </c>
-      <c r="H51" s="132"/>
-    </row>
-    <row r="52" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="120"/>
-      <c r="C52" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="D52" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E52" s="132" t="s">
-        <v>49</v>
-      </c>
-      <c r="F52" s="136">
-        <v>3.2099999999999997E-2</v>
-      </c>
-      <c r="G52" s="132" t="s">
-        <v>287</v>
-      </c>
-      <c r="H52" s="132"/>
-    </row>
-    <row r="53" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="120"/>
-      <c r="C53" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="D53" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" s="132" t="s">
-        <v>50</v>
-      </c>
-      <c r="F53" s="136">
+      <c r="G85" s="136">
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="G53" s="132" t="s">
-        <v>287</v>
-      </c>
-      <c r="H53" s="132"/>
-    </row>
-    <row r="54" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="121"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="H85" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I85" s="132"/>
+    </row>
+    <row r="86" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="121"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="B76:B86"/>
     <mergeCell ref="B4:B22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B43"/>
+    <mergeCell ref="B27:B75"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
+  <conditionalFormatting sqref="G27:G75">
+    <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6552,76 +7379,76 @@
     <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="128" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C4" s="126" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D4" s="127"/>
     </row>
     <row r="5" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="129"/>
       <c r="C5" s="74" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D5" s="75" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="76" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="71" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="79" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="85" x14ac:dyDescent="0.2">
       <c r="B11" s="78" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="80" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D12" s="80" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] Sending batch 9
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070DAEF0-08CE-9C46-ABFA-4D9412DD66DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1771153-4FC5-4143-875E-A83689E0CA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="15240" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="417">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -1225,6 +1225,99 @@
   </si>
   <si>
     <t>dropout+mixup but for 70 epochs entropy 0.5 (p50)</t>
+  </si>
+  <si>
+    <t>34/50</t>
+  </si>
+  <si>
+    <t>Testing only</t>
+  </si>
+  <si>
+    <t>p53</t>
+  </si>
+  <si>
+    <t>p54</t>
+  </si>
+  <si>
+    <t>p55</t>
+  </si>
+  <si>
+    <t>p56</t>
+  </si>
+  <si>
+    <t>p57</t>
+  </si>
+  <si>
+    <t>p58</t>
+  </si>
+  <si>
+    <t>FGSM 0.01 on p51</t>
+  </si>
+  <si>
+    <t>FGSM 0.05 on p51</t>
+  </si>
+  <si>
+    <t>FGSM 0.1 on p51</t>
+  </si>
+  <si>
+    <t>p59</t>
+  </si>
+  <si>
+    <t>p60</t>
+  </si>
+  <si>
+    <t>p61</t>
+  </si>
+  <si>
+    <t>Without Zoom FGSM 0.1 (r1.58)</t>
+  </si>
+  <si>
+    <t>Without Zoom FGSM 0.01 (r1.58)</t>
+  </si>
+  <si>
+    <t>Without Zoom FGSM 0.05 (r1.58)</t>
+  </si>
+  <si>
+    <t>Without Zoom FGSM 0.2 (r1.58)</t>
+  </si>
+  <si>
+    <t>Train accuracy going to 85%. Can train for longer</t>
+  </si>
+  <si>
+    <t>Train accuracy going to 80%. Can train for longer</t>
+  </si>
+  <si>
+    <t>Train accuracy going to 86%. Can train for longer</t>
+  </si>
+  <si>
+    <t>10% per class - p49</t>
+  </si>
+  <si>
+    <t>25% per class - p49</t>
+  </si>
+  <si>
+    <t>50% per class - p49</t>
+  </si>
+  <si>
+    <t>10% per class - p50</t>
+  </si>
+  <si>
+    <t>25% per class - p50</t>
+  </si>
+  <si>
+    <t>50% per class - p50</t>
+  </si>
+  <si>
+    <t>dropout+mixup but for 100 epochs entropy 0.1 (p39)</t>
+  </si>
+  <si>
+    <t>dropout+mixup but for 100 epochs entropy 0.1 (p40)</t>
+  </si>
+  <si>
+    <t>p62</t>
+  </si>
+  <si>
+    <t>p63</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1497,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="57">
+  <fills count="58">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1728,6 +1821,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="55">
     <border>
@@ -2470,7 +2569,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2945,6 +3044,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2990,7 +3105,42 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB2A5FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -2998,6 +3148,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3022,10 +3182,196 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB2A5FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9766FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9766FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB530"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB530"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB2A5FD"/>
+      <color rgb="FF9766FF"/>
+      <color rgb="FFFFB530"/>
       <color rgb="FF75489E"/>
       <color rgb="FFFF0000"/>
     </mruColors>
@@ -3358,10 +3704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
-  <dimension ref="B1:N102"/>
+  <dimension ref="B1:N118"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A48" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5125,8 +5471,8 @@
       </c>
       <c r="J69" s="107"/>
     </row>
-    <row r="70" spans="2:10" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+    <row r="70" spans="2:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="112"/>
       <c r="C70" s="49" t="s">
         <v>198</v>
       </c>
@@ -5151,496 +5497,550 @@
       <c r="J70" s="107"/>
     </row>
     <row r="71" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="108" t="s">
-        <v>130</v>
-      </c>
-      <c r="C71" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F71" s="6">
-        <v>0.92759999999999998</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="B71" s="112"/>
+      <c r="C71" s="49"/>
+      <c r="D71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F71" s="16">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="J71" s="107"/>
     </row>
-    <row r="72" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="109"/>
-      <c r="C72" s="51" t="s">
-        <v>200</v>
-      </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F72" s="2">
-        <v>0.92759999999999998</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
+    <row r="72" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="112"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F72" s="16">
+        <v>0.4204</v>
+      </c>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
       <c r="J72" s="107"/>
     </row>
-    <row r="73" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="109"/>
-      <c r="C73" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F73" s="2"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
+    <row r="73" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="112"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F73" s="16">
+        <v>0.36730000000000002</v>
+      </c>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
       <c r="J73" s="107"/>
     </row>
-    <row r="74" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="110"/>
-      <c r="C74" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F74" s="10"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
+    <row r="74" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="112"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F74" s="16">
+        <v>0.3034</v>
+      </c>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
       <c r="J74" s="107"/>
     </row>
-    <row r="75" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B75" s="111" t="s">
-        <v>128</v>
-      </c>
-      <c r="C75" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F75" s="31">
-        <v>0.84760000000000002</v>
-      </c>
-      <c r="G75" s="3">
-        <v>50</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>110</v>
-      </c>
+    <row r="75" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="112"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F75" s="16">
+        <v>0.3543</v>
+      </c>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
       <c r="J75" s="107"/>
     </row>
-    <row r="76" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="112"/>
-      <c r="C76" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F76" s="2">
-        <v>0.80649999999999999</v>
-      </c>
-      <c r="G76" s="1">
-        <v>50</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C76" s="49"/>
+      <c r="D76" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F76" s="16"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="107"/>
+    </row>
+    <row r="77" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="112"/>
-      <c r="C77" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F77" s="2">
-        <v>0.84240000000000004</v>
-      </c>
-      <c r="G77" s="1">
-        <v>50</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="C77" s="49"/>
+      <c r="D77" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F77" s="16"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="107"/>
+    </row>
+    <row r="78" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="112"/>
-      <c r="C78" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F78" s="2">
-        <v>0.84250000000000003</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J78" s="1"/>
-    </row>
-    <row r="79" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="C78" s="49"/>
+      <c r="D78" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F78" s="16"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="107"/>
+    </row>
+    <row r="79" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="112"/>
-      <c r="C79" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F79" s="2">
-        <v>0.85909999999999997</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="C79" s="49"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F79" s="16"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="107"/>
+    </row>
+    <row r="80" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="112"/>
-      <c r="C80" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F80" s="2">
-        <v>0.84889999999999999</v>
-      </c>
-      <c r="G80" s="1">
-        <v>50</v>
-      </c>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C80" s="49"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="16"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="107"/>
+    </row>
+    <row r="81" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="112"/>
-      <c r="C81" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="C81" s="49"/>
+      <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="F81" s="16">
-        <v>0.91720000000000002</v>
-      </c>
-      <c r="G81" s="1">
-        <v>50</v>
-      </c>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J81" s="4"/>
-    </row>
-    <row r="82" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="F81" s="16"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="107"/>
+    </row>
+    <row r="82" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="112"/>
-      <c r="C82" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F82" s="2">
-        <v>0.87190000000000001</v>
-      </c>
-      <c r="G82" s="1">
-        <v>50</v>
-      </c>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C82" s="49"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="107"/>
+    </row>
+    <row r="83" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="112"/>
-      <c r="C83" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F83" s="2">
-        <v>0.52159999999999995</v>
-      </c>
-      <c r="G83" s="1">
-        <v>50</v>
-      </c>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C83" s="49"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="107"/>
+    </row>
+    <row r="84" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="112"/>
-      <c r="C84" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F84" s="2">
-        <v>0.6804</v>
-      </c>
-      <c r="G84" s="1">
-        <v>50</v>
-      </c>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C84" s="49"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="107"/>
+    </row>
+    <row r="85" spans="2:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="112"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="112"/>
-      <c r="C86" s="13"/>
+      <c r="C85" s="49"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="107"/>
+    </row>
+    <row r="86" spans="2:10" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="113"/>
+      <c r="C86" s="29"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="2"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B87" s="112"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B88" s="112"/>
-      <c r="C88" s="13"/>
+      <c r="J86" s="107"/>
+    </row>
+    <row r="87" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" s="72" t="s">
+        <v>199</v>
+      </c>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F87" s="31">
+        <v>0.92759999999999998</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="107"/>
+    </row>
+    <row r="88" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="109"/>
+      <c r="C88" s="51" t="s">
+        <v>200</v>
+      </c>
       <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="1"/>
+      <c r="E88" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F88" s="2">
+        <v>0.92759999999999998</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="112"/>
-      <c r="C89" s="13"/>
+      <c r="J88" s="107"/>
+    </row>
+    <row r="89" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="109"/>
+      <c r="C89" s="51" t="s">
+        <v>201</v>
+      </c>
       <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="F89" s="2"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="112"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B91" s="112"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J89" s="107"/>
+    </row>
+    <row r="90" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="110"/>
+      <c r="C90" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F90" s="10"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="107"/>
+    </row>
+    <row r="91" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B91" s="111" t="s">
+        <v>128</v>
+      </c>
+      <c r="C91" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F91" s="31">
+        <v>0.84760000000000002</v>
+      </c>
+      <c r="G91" s="3">
+        <v>50</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J91" s="107"/>
+    </row>
+    <row r="92" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B92" s="112"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
+      <c r="C92" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F92" s="2">
+        <v>0.80649999999999999</v>
+      </c>
+      <c r="G92" s="1">
+        <v>50</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B93" s="112"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C93" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F93" s="2">
+        <v>0.84240000000000004</v>
+      </c>
+      <c r="G93" s="1">
+        <v>50</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B94" s="112"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
+      <c r="C94" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F94" s="2">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B95" s="112"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C95" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0.85909999999999997</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B96" s="112"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="1"/>
+      <c r="C96" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0.84889999999999999</v>
+      </c>
+      <c r="G96" s="1">
+        <v>50</v>
+      </c>
       <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
+      <c r="I96" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B97" s="112"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="1"/>
+      <c r="C97" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F97" s="16">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="G97" s="1">
+        <v>50</v>
+      </c>
       <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I97" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J97" s="4"/>
+    </row>
+    <row r="98" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B98" s="112"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="1"/>
+      <c r="C98" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.87190000000000001</v>
+      </c>
+      <c r="G98" s="1">
+        <v>50</v>
+      </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J98" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B99" s="112"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="1"/>
+      <c r="C99" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="G99" s="1">
+        <v>50</v>
+      </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J99" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B100" s="112"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="1"/>
+      <c r="C100" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0.6804</v>
+      </c>
+      <c r="G100" s="1">
+        <v>50</v>
+      </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
+      <c r="J100" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B101" s="112"/>
@@ -5653,8 +6053,8 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="113"/>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B102" s="112"/>
       <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -5664,27 +6064,203 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B103" s="112"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B104" s="112"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B105" s="112"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B106" s="112"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B107" s="112"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B108" s="112"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B109" s="112"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B110" s="112"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B111" s="112"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B112" s="112"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B113" s="112"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B114" s="112"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B115" s="112"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B116" s="112"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B117" s="112"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="113"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="J56:J75"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B102"/>
+    <mergeCell ref="J56:J91"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B118"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B30"/>
-    <mergeCell ref="B31:B70"/>
+    <mergeCell ref="B31:B86"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D5:D1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5694,10 +6270,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5741,7 +6317,7 @@
       </c>
       <c r="L2" s="38"/>
     </row>
-    <row r="3" spans="1:12" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54"/>
       <c r="B3" s="56" t="s">
         <v>4</v>
@@ -5977,6 +6553,7 @@
       </c>
       <c r="J10" s="54"/>
       <c r="K10" s="54"/>
+      <c r="L10" s="167"/>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
@@ -6198,7 +6775,7 @@
       <c r="J22" s="54"/>
       <c r="K22" s="54"/>
     </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="123" t="s">
         <v>233</v>
       </c>
@@ -6814,7 +7391,9 @@
       <c r="F51" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="G51" s="159"/>
+      <c r="G51" s="159">
+        <v>0.69520000000000004</v>
+      </c>
       <c r="H51" s="158"/>
       <c r="I51" s="158"/>
     </row>
@@ -6832,7 +7411,9 @@
       <c r="F52" s="160" t="s">
         <v>373</v>
       </c>
-      <c r="G52" s="159"/>
+      <c r="G52" s="159">
+        <v>0.52629999999999999</v>
+      </c>
       <c r="H52" s="158"/>
       <c r="I52" s="158"/>
     </row>
@@ -6850,8 +7431,12 @@
       <c r="F53" s="160" t="s">
         <v>376</v>
       </c>
-      <c r="G53" s="159"/>
-      <c r="H53" s="158"/>
+      <c r="G53" s="159">
+        <v>0.68289999999999995</v>
+      </c>
+      <c r="H53" s="158" t="s">
+        <v>386</v>
+      </c>
       <c r="I53" s="158"/>
     </row>
     <row r="54" spans="2:9" ht="17" x14ac:dyDescent="0.2">
@@ -6868,13 +7453,15 @@
       <c r="F54" s="160" t="s">
         <v>382</v>
       </c>
-      <c r="G54" s="159"/>
+      <c r="G54" s="159">
+        <v>0.51270000000000004</v>
+      </c>
       <c r="H54" s="158"/>
       <c r="I54" s="158"/>
     </row>
     <row r="55" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" s="120"/>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="166" t="s">
         <v>374</v>
       </c>
       <c r="D55" s="157" t="s">
@@ -6886,8 +7473,12 @@
       <c r="F55" s="160" t="s">
         <v>377</v>
       </c>
-      <c r="G55" s="159"/>
-      <c r="H55" s="158"/>
+      <c r="G55" s="159">
+        <v>0.6875</v>
+      </c>
+      <c r="H55" s="158" t="s">
+        <v>386</v>
+      </c>
       <c r="I55" s="158"/>
     </row>
     <row r="56" spans="2:9" ht="17" x14ac:dyDescent="0.2">
@@ -6904,13 +7495,15 @@
       <c r="F56" s="160" t="s">
         <v>383</v>
       </c>
-      <c r="G56" s="159"/>
+      <c r="G56" s="159">
+        <v>0.52739999999999998</v>
+      </c>
       <c r="H56" s="158"/>
       <c r="I56" s="158"/>
     </row>
     <row r="57" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" s="120"/>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="166" t="s">
         <v>378</v>
       </c>
       <c r="D57" s="157" t="s">
@@ -6922,9 +7515,13 @@
       <c r="F57" s="158" t="s">
         <v>368</v>
       </c>
-      <c r="G57" s="159"/>
+      <c r="G57" s="159">
+        <v>0.71379999999999999</v>
+      </c>
       <c r="H57" s="158"/>
-      <c r="I57" s="158"/>
+      <c r="I57" s="158" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="58" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B58" s="120"/>
@@ -6940,9 +7537,13 @@
       <c r="F58" s="158" t="s">
         <v>369</v>
       </c>
-      <c r="G58" s="159"/>
+      <c r="G58" s="159">
+        <v>0.59970000000000001</v>
+      </c>
       <c r="H58" s="158"/>
-      <c r="I58" s="158"/>
+      <c r="I58" s="158" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="59" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B59" s="120"/>
@@ -6958,13 +7559,17 @@
       <c r="F59" s="158" t="s">
         <v>384</v>
       </c>
-      <c r="G59" s="159"/>
+      <c r="G59" s="159">
+        <v>0.71199999999999997</v>
+      </c>
       <c r="H59" s="158"/>
-      <c r="I59" s="158"/>
+      <c r="I59" s="158" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="60" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="120"/>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="166" t="s">
         <v>381</v>
       </c>
       <c r="D60" s="157" t="s">
@@ -6976,116 +7581,208 @@
       <c r="F60" s="158" t="s">
         <v>385</v>
       </c>
-      <c r="G60" s="159"/>
+      <c r="G60" s="159">
+        <v>0.58930000000000005</v>
+      </c>
       <c r="H60" s="158"/>
-      <c r="I60" s="158"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I60" s="158" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" s="120"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C61" s="166" t="s">
+        <v>388</v>
+      </c>
+      <c r="D61" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="F61" s="158" t="s">
+        <v>413</v>
+      </c>
+      <c r="G61" s="159"/>
+      <c r="H61" s="158"/>
+      <c r="I61" s="158"/>
+    </row>
+    <row r="62" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="120"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C62" s="166" t="s">
+        <v>389</v>
+      </c>
+      <c r="D62" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F62" s="158" t="s">
+        <v>414</v>
+      </c>
+      <c r="G62" s="159"/>
+      <c r="H62" s="158"/>
+      <c r="I62" s="158"/>
+    </row>
+    <row r="63" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B63" s="120"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="61"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C63" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="D63" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="F63" s="164" t="s">
+        <v>407</v>
+      </c>
+      <c r="G63" s="165"/>
+      <c r="H63" s="162"/>
+      <c r="I63" s="162"/>
+    </row>
+    <row r="64" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B64" s="120"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="61"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C64" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="D64" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="F64" s="164" t="s">
+        <v>408</v>
+      </c>
+      <c r="G64" s="165"/>
+      <c r="H64" s="162"/>
+      <c r="I64" s="162"/>
+    </row>
+    <row r="65" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B65" s="120"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C65" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="D65" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="F65" s="164" t="s">
+        <v>409</v>
+      </c>
+      <c r="G65" s="165"/>
+      <c r="H65" s="162"/>
+      <c r="I65" s="162"/>
+    </row>
+    <row r="66" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="120"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C66" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="D66" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" s="164" t="s">
+        <v>410</v>
+      </c>
+      <c r="G66" s="165"/>
+      <c r="H66" s="162"/>
+      <c r="I66" s="162"/>
+    </row>
+    <row r="67" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" s="120"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C67" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="D67" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="164" t="s">
+        <v>411</v>
+      </c>
+      <c r="G67" s="165"/>
+      <c r="H67" s="162"/>
+      <c r="I67" s="162"/>
+    </row>
+    <row r="68" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B68" s="120"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="60"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C68" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="D68" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F68" s="164" t="s">
+        <v>412</v>
+      </c>
+      <c r="G68" s="165"/>
+      <c r="H68" s="162"/>
+      <c r="I68" s="162"/>
+    </row>
+    <row r="69" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B69" s="120"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="60"/>
+      <c r="C69" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="D69" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="G69" s="2"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B70" s="120"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="1"/>
+      <c r="C70" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D70" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="G70" s="2"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B71" s="120"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="61"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="1"/>
+      <c r="C71" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="D71" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="G71" s="2"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -7120,157 +7817,133 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="121"/>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B75" s="120"/>
       <c r="C75" s="13"/>
-      <c r="D75" s="1"/>
+      <c r="D75" s="61"/>
       <c r="E75" s="13"/>
       <c r="F75" s="1"/>
       <c r="G75" s="2"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B76" s="119" t="s">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="120"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="121"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B78" s="119" t="s">
         <v>245</v>
       </c>
-      <c r="C76" s="22" t="s">
+      <c r="C78" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="D76" s="98" t="s">
+      <c r="D78" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E76" s="22"/>
-      <c r="F76" s="98" t="s">
+      <c r="E78" s="22"/>
+      <c r="F78" s="98" t="s">
         <v>275</v>
       </c>
-      <c r="G76" s="99">
+      <c r="G78" s="99">
         <v>0.4929</v>
       </c>
-      <c r="H76" s="98" t="s">
+      <c r="H78" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="I76" s="98" t="s">
+      <c r="I78" s="98" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B77" s="120"/>
-      <c r="C77" s="22" t="s">
+    <row r="79" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B79" s="120"/>
+      <c r="C79" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="D77" s="98" t="s">
+      <c r="D79" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="E77" s="22"/>
-      <c r="F77" s="98" t="s">
+      <c r="E79" s="22"/>
+      <c r="F79" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="G77" s="99">
+      <c r="G79" s="99">
         <v>0.66930000000000001</v>
       </c>
-      <c r="H77" s="98" t="s">
+      <c r="H79" s="98" t="s">
         <v>281</v>
       </c>
-      <c r="I77" s="98" t="s">
+      <c r="I79" s="98" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="78" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B78" s="120"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="1" t="s">
+    <row r="80" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B80" s="120"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="13"/>
-      <c r="F78" s="1" t="s">
+      <c r="E80" s="13"/>
+      <c r="F80" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="G78" s="2"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-    </row>
-    <row r="79" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B79" s="120"/>
-      <c r="C79" s="25" t="s">
+      <c r="G80" s="2"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B81" s="120"/>
+      <c r="C81" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="D79" s="142" t="s">
+      <c r="D81" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="E79" s="25"/>
-      <c r="F79" s="142" t="s">
+      <c r="E81" s="25"/>
+      <c r="F81" s="142" t="s">
         <v>278</v>
       </c>
-      <c r="G79" s="143">
+      <c r="G81" s="143">
         <v>0.67969999999999997</v>
       </c>
-      <c r="H79" s="142" t="s">
+      <c r="H81" s="142" t="s">
         <v>327</v>
       </c>
-      <c r="I79" s="142"/>
-    </row>
-    <row r="80" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B80" s="120"/>
-      <c r="C80" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="D80" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E80" s="23"/>
-      <c r="F80" s="102" t="s">
-        <v>302</v>
-      </c>
-      <c r="G80" s="105">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="H80" s="145" t="s">
-        <v>323</v>
-      </c>
-      <c r="I80" s="104" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B81" s="120"/>
-      <c r="C81" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="D81" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E81" s="23"/>
-      <c r="F81" s="102" t="s">
-        <v>303</v>
-      </c>
-      <c r="G81" s="105">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="H81" s="106">
-        <v>50</v>
-      </c>
-      <c r="I81" s="104" t="s">
-        <v>287</v>
-      </c>
+      <c r="I81" s="142"/>
     </row>
     <row r="82" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B82" s="120"/>
       <c r="C82" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D82" s="101" t="s">
         <v>36</v>
       </c>
       <c r="E82" s="23"/>
       <c r="F82" s="102" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G82" s="105">
-        <v>0.54239999999999999</v>
-      </c>
-      <c r="H82" s="106" t="s">
-        <v>321</v>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H82" s="145" t="s">
+        <v>323</v>
       </c>
       <c r="I82" s="104" t="s">
         <v>287</v>
@@ -7278,85 +7951,151 @@
     </row>
     <row r="83" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B83" s="120"/>
-      <c r="C83" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="D83" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E83" s="24"/>
-      <c r="F83" s="132" t="s">
-        <v>47</v>
-      </c>
-      <c r="G83" s="136">
-        <v>7.7899999999999997E-2</v>
-      </c>
-      <c r="H83" s="132" t="s">
-        <v>281</v>
-      </c>
-      <c r="I83" s="132"/>
+      <c r="C83" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="D83" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" s="23"/>
+      <c r="F83" s="102" t="s">
+        <v>303</v>
+      </c>
+      <c r="G83" s="105">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="H83" s="106">
+        <v>50</v>
+      </c>
+      <c r="I83" s="104" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="84" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B84" s="120"/>
-      <c r="C84" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="D84" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E84" s="24"/>
-      <c r="F84" s="132" t="s">
-        <v>49</v>
-      </c>
-      <c r="G84" s="136">
-        <v>3.2099999999999997E-2</v>
-      </c>
-      <c r="H84" s="132" t="s">
-        <v>281</v>
-      </c>
-      <c r="I84" s="132"/>
+      <c r="C84" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="D84" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E84" s="23"/>
+      <c r="F84" s="102" t="s">
+        <v>304</v>
+      </c>
+      <c r="G84" s="105">
+        <v>0.54239999999999999</v>
+      </c>
+      <c r="H84" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="I84" s="104" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="85" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B85" s="120"/>
       <c r="C85" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D85" s="131" t="s">
         <v>46</v>
       </c>
       <c r="E85" s="24"/>
       <c r="F85" s="132" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G85" s="136">
-        <v>2.2100000000000002E-2</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="H85" s="132" t="s">
         <v>281</v>
       </c>
       <c r="I85" s="132"/>
     </row>
-    <row r="86" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="121"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
+    <row r="86" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B86" s="120"/>
+      <c r="C86" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="D86" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E86" s="24"/>
+      <c r="F86" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="G86" s="136">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="H86" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I86" s="132"/>
+    </row>
+    <row r="87" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B87" s="120"/>
+      <c r="C87" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D87" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E87" s="24"/>
+      <c r="F87" s="132" t="s">
+        <v>50</v>
+      </c>
+      <c r="G87" s="136">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="H87" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I87" s="132"/>
+    </row>
+    <row r="88" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="121"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B76:B86"/>
+    <mergeCell ref="B78:B88"/>
     <mergeCell ref="B4:B22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B75"/>
+    <mergeCell ref="B27:B77"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="G27:G75">
-    <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
+  <conditionalFormatting sqref="G27:G77">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>AND(E27="S", G27&gt;=LARGE(_xlfn._xlws.FILTER(G$27:G$77, E$27:E$77="S"), 3))</formula>
+    </cfRule>
+    <cfRule type="top10" dxfId="5" priority="7" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D1048576">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E1048576">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",E4)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[IMP] Sending batch 9v2
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1771153-4FC5-4143-875E-A83689E0CA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D78818-D1C2-3147-83FD-5565512A5402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="760" windowWidth="14160" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="15220" yWindow="780" windowWidth="14180" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
     <sheet name="StanfordDogs" sheetId="2" r:id="rId2"/>
     <sheet name="Config Tables" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="500">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -1107,12 +1120,6 @@
     <t>p39</t>
   </si>
   <si>
-    <t>NoZoom on pretrained (p7)</t>
-  </si>
-  <si>
-    <t>NoZoom on scratch (p6)</t>
-  </si>
-  <si>
     <t>p40</t>
   </si>
   <si>
@@ -1251,15 +1258,6 @@
     <t>p58</t>
   </si>
   <si>
-    <t>FGSM 0.01 on p51</t>
-  </si>
-  <si>
-    <t>FGSM 0.05 on p51</t>
-  </si>
-  <si>
-    <t>FGSM 0.1 on p51</t>
-  </si>
-  <si>
     <t>p59</t>
   </si>
   <si>
@@ -1290,24 +1288,6 @@
     <t>Train accuracy going to 86%. Can train for longer</t>
   </si>
   <si>
-    <t>10% per class - p49</t>
-  </si>
-  <si>
-    <t>25% per class - p49</t>
-  </si>
-  <si>
-    <t>50% per class - p49</t>
-  </si>
-  <si>
-    <t>10% per class - p50</t>
-  </si>
-  <si>
-    <t>25% per class - p50</t>
-  </si>
-  <si>
-    <t>50% per class - p50</t>
-  </si>
-  <si>
     <t>dropout+mixup but for 100 epochs entropy 0.1 (p39)</t>
   </si>
   <si>
@@ -1318,13 +1298,295 @@
   </si>
   <si>
     <t>p63</t>
+  </si>
+  <si>
+    <t>88/100</t>
+  </si>
+  <si>
+    <t>10% per class - p53 with early stopping</t>
+  </si>
+  <si>
+    <t>25% per class - p53 with early stopping</t>
+  </si>
+  <si>
+    <t>50% per class - p53 with early stopping</t>
+  </si>
+  <si>
+    <t>10% per class - p54 with early stopping</t>
+  </si>
+  <si>
+    <t>50% per class  - p54 with early stopping</t>
+  </si>
+  <si>
+    <t>25% per class  - p54 with early stopping</t>
+  </si>
+  <si>
+    <t>FGSM 0.01 on p53</t>
+  </si>
+  <si>
+    <t>FGSM 0.05 on p53</t>
+  </si>
+  <si>
+    <t>FGSM 0.1 on p53</t>
+  </si>
+  <si>
+    <t>p64</t>
+  </si>
+  <si>
+    <t>p65</t>
+  </si>
+  <si>
+    <t>batch 9</t>
+  </si>
+  <si>
+    <t>FGSM 0.05 on p50</t>
+  </si>
+  <si>
+    <t>FGSM 0.01 on p50</t>
+  </si>
+  <si>
+    <t>FGSM 0.1 on p50</t>
+  </si>
+  <si>
+    <t>82/92</t>
+  </si>
+  <si>
+    <t>49/59</t>
+  </si>
+  <si>
+    <t>10% per class - p28</t>
+  </si>
+  <si>
+    <t>25% per class - p28</t>
+  </si>
+  <si>
+    <t>50% per class - p28</t>
+  </si>
+  <si>
+    <t>p55v2</t>
+  </si>
+  <si>
+    <t>6--16</t>
+  </si>
+  <si>
+    <t>16/26</t>
+  </si>
+  <si>
+    <t>p58v2</t>
+  </si>
+  <si>
+    <t>FGSM 0.2 on p50</t>
+  </si>
+  <si>
+    <t>PGD 0.01 on p50</t>
+  </si>
+  <si>
+    <t>PGD 0.05 on p50</t>
+  </si>
+  <si>
+    <t>PGD 0.1 on p50</t>
+  </si>
+  <si>
+    <t>PGD 0.2 on p50</t>
+  </si>
+  <si>
+    <t>Gaussian 0.01 on p50</t>
+  </si>
+  <si>
+    <t>Gaussian 0.05 on p50</t>
+  </si>
+  <si>
+    <t>Gaussian 0.1 on p50</t>
+  </si>
+  <si>
+    <t>Gaussian 0.2 on p50</t>
+  </si>
+  <si>
+    <t>FGSM 0.2 on p53</t>
+  </si>
+  <si>
+    <t>PGD 0.01 on p53</t>
+  </si>
+  <si>
+    <t>PGD 0.05 on p53</t>
+  </si>
+  <si>
+    <t>PGD 0.1 on p53</t>
+  </si>
+  <si>
+    <t>PGD 0.2 on p53</t>
+  </si>
+  <si>
+    <t>Gaussian 0.01 on p53</t>
+  </si>
+  <si>
+    <t>Gaussian 0.05 on p53</t>
+  </si>
+  <si>
+    <t>Gaussian 0.1 on p53</t>
+  </si>
+  <si>
+    <t>Gaussian 0.2 on p53</t>
+  </si>
+  <si>
+    <t>PGD 0.01 on p5</t>
+  </si>
+  <si>
+    <t>FGSM 0.01 on p5</t>
+  </si>
+  <si>
+    <t>FGSM 0.05 on p5</t>
+  </si>
+  <si>
+    <t>FGSM 0.1 on p5</t>
+  </si>
+  <si>
+    <t>FGSM 0.2 on p5</t>
+  </si>
+  <si>
+    <t>PGD 0.05 on p5</t>
+  </si>
+  <si>
+    <t>PGD 0.1 on p5</t>
+  </si>
+  <si>
+    <t>PGD 0.2 on p5</t>
+  </si>
+  <si>
+    <t>Gaussian 0.01 on p5</t>
+  </si>
+  <si>
+    <t>Gaussian 0.05 on p5</t>
+  </si>
+  <si>
+    <t>Gaussian 0.1 on p5</t>
+  </si>
+  <si>
+    <t>Gaussian 0.2 on p5</t>
+  </si>
+  <si>
+    <t>FGSM 0.01 on p28</t>
+  </si>
+  <si>
+    <t>FGSM 0.05 on p28</t>
+  </si>
+  <si>
+    <t>FGSM 0.1 on p28</t>
+  </si>
+  <si>
+    <t>FGSM 0.2 on p28</t>
+  </si>
+  <si>
+    <t>PGD 0.01 on p28</t>
+  </si>
+  <si>
+    <t>PGD 0.05 on p28</t>
+  </si>
+  <si>
+    <t>PGD 0.1 on p28</t>
+  </si>
+  <si>
+    <t>PGD 0.2 on p28</t>
+  </si>
+  <si>
+    <t>Gaussian 0.01 on p28</t>
+  </si>
+  <si>
+    <t>Gaussian 0.05 on p28</t>
+  </si>
+  <si>
+    <t>Gaussian 0.1 on p28</t>
+  </si>
+  <si>
+    <t>Gaussian 0.2 on p28</t>
+  </si>
+  <si>
+    <t>58/68</t>
+  </si>
+  <si>
+    <t>98/100</t>
+  </si>
+  <si>
+    <t>p56v2</t>
+  </si>
+  <si>
+    <t>p57v2</t>
+  </si>
+  <si>
+    <t>10% per class - p53 100 epochs ES 20 patience</t>
+  </si>
+  <si>
+    <t>25% per class - p53 100 epochs ES 20 patience</t>
+  </si>
+  <si>
+    <t>50% per class - p53 100 epochs ES 20 patience</t>
+  </si>
+  <si>
+    <t>10% per class - p54 100 epochs ES 20 patience</t>
+  </si>
+  <si>
+    <t>25% per class - p54 100 epochs ES 20 patience</t>
+  </si>
+  <si>
+    <t>50% per class - p54 100 epochs ES 20 patience</t>
+  </si>
+  <si>
+    <t>p59v2</t>
+  </si>
+  <si>
+    <t>p60v2</t>
+  </si>
+  <si>
+    <t>NoZoom on p53</t>
+  </si>
+  <si>
+    <t>NoZoom on p54</t>
+  </si>
+  <si>
+    <t>FGSM 0.01 on p54</t>
+  </si>
+  <si>
+    <t>FGSM 0.05 on p54</t>
+  </si>
+  <si>
+    <t>FGSM 0.1 on p54</t>
+  </si>
+  <si>
+    <t>FGSM 0.2 on p54</t>
+  </si>
+  <si>
+    <t>PGD 0.01 on p54</t>
+  </si>
+  <si>
+    <t>PGD 0.05 on p54</t>
+  </si>
+  <si>
+    <t>PGD 0.1 on p54</t>
+  </si>
+  <si>
+    <t>PGD 0.2 on p54</t>
+  </si>
+  <si>
+    <t>Gaussian 0.01 on p54</t>
+  </si>
+  <si>
+    <t>Gaussian 0.05 on p54</t>
+  </si>
+  <si>
+    <t>Gaussian 0.1 on p54</t>
+  </si>
+  <si>
+    <t>Gaussian 0.2 on p54</t>
+  </si>
+  <si>
+    <t>Attack on p64 and 65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1493,6 +1755,21 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -1828,7 +2105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2524,6 +2801,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2569,7 +2892,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3059,7 +3382,112 @@
     <xf numFmtId="0" fontId="19" fillId="42" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="43" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="43" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="43" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="43" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="43" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="57" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="57" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="57" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="57" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3105,7 +3533,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF75489E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3142,26 +3590,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF75489E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
@@ -3179,189 +3607,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB2A5FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF75489E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF75489E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9766FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF75489E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9766FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB530"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF75489E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB530"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3706,8 +3951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N118"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView topLeftCell="A36" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4666,7 +4911,7 @@
         <v>30</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F38" s="2">
         <v>0.9042</v>
@@ -5503,13 +5748,13 @@
         <v>46</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F71" s="16">
         <v>0.48549999999999999</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>34</v>
@@ -5526,7 +5771,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F72" s="16">
         <v>0.4204</v>
@@ -5543,7 +5788,7 @@
         <v>46</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F73" s="16">
         <v>0.36730000000000002</v>
@@ -5560,7 +5805,7 @@
         <v>46</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F74" s="16">
         <v>0.3034</v>
@@ -6270,10 +6515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6329,7 +6574,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F3" s="57" t="s">
         <v>7</v>
@@ -6364,7 +6609,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="87" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G4" s="88">
         <v>0.36480000000000001</v>
@@ -6419,7 +6664,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="85" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F6" s="87" t="s">
         <v>248</v>
@@ -6449,7 +6694,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="85" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F7" s="87" t="s">
         <v>249</v>
@@ -6479,7 +6724,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="93" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F8" s="95" t="s">
         <v>267</v>
@@ -6509,7 +6754,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F9" s="139" t="s">
         <v>269</v>
@@ -6537,7 +6782,7 @@
         <v>36</v>
       </c>
       <c r="E10" s="100" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F10" s="102" t="s">
         <v>296</v>
@@ -6552,8 +6797,10 @@
         <v>287</v>
       </c>
       <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="167"/>
+      <c r="K10" s="54" t="s">
+        <v>418</v>
+      </c>
+      <c r="L10" s="168"/>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
@@ -6565,7 +6812,7 @@
         <v>36</v>
       </c>
       <c r="E11" s="100" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F11" s="102" t="s">
         <v>297</v>
@@ -6592,7 +6839,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="100" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F12" s="102" t="s">
         <v>298</v>
@@ -6619,10 +6866,10 @@
         <v>46</v>
       </c>
       <c r="E13" s="130" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F13" s="132" t="s">
-        <v>47</v>
+        <v>450</v>
       </c>
       <c r="G13" s="133">
         <v>0.13159999999999999</v>
@@ -6644,10 +6891,10 @@
         <v>46</v>
       </c>
       <c r="E14" s="130" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F14" s="132" t="s">
-        <v>49</v>
+        <v>451</v>
       </c>
       <c r="G14" s="133">
         <v>5.57E-2</v>
@@ -6669,10 +6916,10 @@
         <v>46</v>
       </c>
       <c r="E15" s="130" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F15" s="132" t="s">
-        <v>50</v>
+        <v>452</v>
       </c>
       <c r="G15" s="133">
         <v>3.6200000000000003E-2</v>
@@ -6684,1418 +6931,2529 @@
       <c r="J15" s="54"/>
       <c r="K15" s="54"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
       <c r="B16" s="120"/>
       <c r="C16" s="64"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="63"/>
+      <c r="D16" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F16" s="132" t="s">
+        <v>453</v>
+      </c>
+      <c r="G16" s="133"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="135"/>
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
       <c r="B17" s="120"/>
       <c r="C17" s="64"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="60"/>
+      <c r="D17" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>449</v>
+      </c>
       <c r="G17" s="62"/>
       <c r="H17" s="60"/>
       <c r="I17" s="63"/>
       <c r="J17" s="54"/>
       <c r="K17" s="54"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
       <c r="B18" s="120"/>
       <c r="C18" s="64"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="60"/>
+      <c r="D18" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>454</v>
+      </c>
       <c r="G18" s="62"/>
       <c r="H18" s="60"/>
       <c r="I18" s="63"/>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
       <c r="B19" s="120"/>
       <c r="C19" s="64"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="60"/>
+      <c r="D19" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>455</v>
+      </c>
       <c r="G19" s="62"/>
       <c r="H19" s="60"/>
       <c r="I19" s="63"/>
       <c r="J19" s="54"/>
       <c r="K19" s="54"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="B20" s="120"/>
       <c r="C20" s="64"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="60"/>
+      <c r="D20" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>456</v>
+      </c>
       <c r="G20" s="62"/>
       <c r="H20" s="60"/>
       <c r="I20" s="63"/>
       <c r="J20" s="54"/>
       <c r="K20" s="54"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="B21" s="120"/>
       <c r="C21" s="64"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="60"/>
+      <c r="D21" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>457</v>
+      </c>
       <c r="G21" s="62"/>
       <c r="H21" s="60"/>
       <c r="I21" s="63"/>
       <c r="J21" s="54"/>
       <c r="K21" s="54"/>
     </row>
-    <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
-      <c r="B22" s="121"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="69"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F22" s="60" t="s">
+        <v>458</v>
+      </c>
+      <c r="G22" s="62"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="63"/>
       <c r="J22" s="54"/>
       <c r="K22" s="54"/>
     </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="123" t="s">
+    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="54"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F23" s="60" t="s">
+        <v>459</v>
+      </c>
+      <c r="G23" s="62"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+    </row>
+    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="54"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="130" t="s">
+        <v>353</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>460</v>
+      </c>
+      <c r="G24" s="62"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="54"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="199" t="s">
+        <v>394</v>
+      </c>
+      <c r="D25" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="200" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="164" t="s">
+        <v>424</v>
+      </c>
+      <c r="G25" s="201"/>
+      <c r="H25" s="164"/>
+      <c r="I25" s="202"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+    </row>
+    <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="54"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="199" t="s">
+        <v>404</v>
+      </c>
+      <c r="D26" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="200" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="164" t="s">
+        <v>425</v>
+      </c>
+      <c r="G26" s="201"/>
+      <c r="H26" s="164"/>
+      <c r="I26" s="202"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="54"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="199" t="s">
+        <v>405</v>
+      </c>
+      <c r="D27" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="200" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="164" t="s">
+        <v>426</v>
+      </c>
+      <c r="G27" s="201"/>
+      <c r="H27" s="164"/>
+      <c r="I27" s="202"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="54"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G28" s="62"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="54"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="G29" s="62"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="54"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G30" s="62"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="54"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G31" s="62"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="54"/>
+      <c r="B32" s="120"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="60" t="s">
+        <v>465</v>
+      </c>
+      <c r="G32" s="62"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+    </row>
+    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="54"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="60" t="s">
+        <v>466</v>
+      </c>
+      <c r="G33" s="62"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="54"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="G34" s="62"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
+    </row>
+    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="54"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" s="60" t="s">
+        <v>468</v>
+      </c>
+      <c r="G35" s="62"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="54"/>
+    </row>
+    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="54"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="G36" s="62"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54"/>
+    </row>
+    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="54"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="G37" s="62"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+    </row>
+    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="54"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="G38" s="62"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+    </row>
+    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="54"/>
+      <c r="B39" s="120"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="60" t="s">
+        <v>472</v>
+      </c>
+      <c r="G39" s="62"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="54"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="54"/>
+      <c r="B40" s="120"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
+    </row>
+    <row r="41" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
+      <c r="B41" s="121"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
+    </row>
+    <row r="42" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="123" t="s">
         <v>233</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C42" s="50" t="s">
         <v>235</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="5" t="s">
+      <c r="D42" s="5"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G42" s="6">
         <v>47.49</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="124"/>
-      <c r="C24" s="51" t="s">
+      <c r="H42" s="5"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="124"/>
+      <c r="C43" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="1" t="s">
+      <c r="D43" s="1"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G43" s="2">
         <v>47.49</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="124"/>
-      <c r="C25" s="51" t="s">
+      <c r="H43" s="1"/>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="124"/>
+      <c r="C44" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="1" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G44" s="2">
         <v>6.7</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="125"/>
-      <c r="C26" s="83" t="s">
+      <c r="H44" s="1"/>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="125"/>
+      <c r="C45" s="83" t="s">
         <v>238</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="4" t="s">
+      <c r="D45" s="4"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G45" s="16">
         <v>6.7</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="53"/>
-    </row>
-    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="119" t="s">
+      <c r="H45" s="4"/>
+      <c r="I45" s="53"/>
+    </row>
+    <row r="46" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="119" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C46" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="D27" s="91" t="s">
+      <c r="D46" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="91" t="s">
+      <c r="E46" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" s="91" t="s">
+        <v>354</v>
+      </c>
+      <c r="G46" s="92">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="H46" s="91">
+        <v>50</v>
+      </c>
+      <c r="I46" s="91" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B47" s="120"/>
+      <c r="C47" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D47" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="98" t="s">
+        <v>355</v>
+      </c>
+      <c r="G47" s="99">
+        <v>0.52239999999999998</v>
+      </c>
+      <c r="H47" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="I47" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="120"/>
+      <c r="C48" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="D48" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="F48" s="98" t="s">
         <v>356</v>
       </c>
-      <c r="G27" s="92">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="H27" s="91">
-        <v>50</v>
-      </c>
-      <c r="I27" s="91" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="120"/>
-      <c r="C28" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="D28" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="98" t="s">
-        <v>357</v>
-      </c>
-      <c r="G28" s="99">
-        <v>0.52239999999999998</v>
-      </c>
-      <c r="H28" s="98" t="s">
-        <v>279</v>
-      </c>
-      <c r="I28" s="98" t="s">
+      <c r="G48" s="99">
+        <v>0.69030000000000002</v>
+      </c>
+      <c r="H48" s="98" t="s">
+        <v>280</v>
+      </c>
+      <c r="I48" s="98" t="s">
         <v>282</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="120"/>
-      <c r="C29" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="D29" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>355</v>
-      </c>
-      <c r="F29" s="98" t="s">
-        <v>358</v>
-      </c>
-      <c r="G29" s="99">
-        <v>0.69030000000000002</v>
-      </c>
-      <c r="H29" s="98" t="s">
-        <v>280</v>
-      </c>
-      <c r="I29" s="98" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B30" s="120"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B31" s="120"/>
-      <c r="C31" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="D31" s="142" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="F31" s="142" t="s">
-        <v>360</v>
-      </c>
-      <c r="G31" s="143">
-        <v>0.67720000000000002</v>
-      </c>
-      <c r="H31" s="142" t="s">
-        <v>322</v>
-      </c>
-      <c r="I31" s="142" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="120"/>
-      <c r="C32" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="D32" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>355</v>
-      </c>
-      <c r="F32" s="102" t="s">
-        <v>299</v>
-      </c>
-      <c r="G32" s="105">
-        <v>3.8199999999999998E-2</v>
-      </c>
-      <c r="H32" s="106" t="s">
-        <v>321</v>
-      </c>
-      <c r="I32" s="104" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B33" s="120"/>
-      <c r="C33" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="D33" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>355</v>
-      </c>
-      <c r="F33" s="102" t="s">
-        <v>300</v>
-      </c>
-      <c r="G33" s="105">
-        <v>0.1991</v>
-      </c>
-      <c r="H33" s="106" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="104" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="120"/>
-      <c r="C34" s="23" t="s">
-        <v>292</v>
-      </c>
-      <c r="D34" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>355</v>
-      </c>
-      <c r="F34" s="102" t="s">
-        <v>301</v>
-      </c>
-      <c r="G34" s="105">
-        <v>0.56259999999999999</v>
-      </c>
-      <c r="H34" s="106" t="s">
-        <v>97</v>
-      </c>
-      <c r="I34" s="104" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="120"/>
-      <c r="C35" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="D35" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>355</v>
-      </c>
-      <c r="F35" s="132" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" s="136">
-        <v>0.1024</v>
-      </c>
-      <c r="H35" s="132" t="s">
-        <v>280</v>
-      </c>
-      <c r="I35" s="132"/>
-    </row>
-    <row r="36" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="120"/>
-      <c r="C36" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="D36" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>355</v>
-      </c>
-      <c r="F36" s="132" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="136">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="H36" s="132" t="s">
-        <v>280</v>
-      </c>
-      <c r="I36" s="132"/>
-    </row>
-    <row r="37" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B37" s="120"/>
-      <c r="C37" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="D37" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>355</v>
-      </c>
-      <c r="F37" s="132" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="136">
-        <v>2.6200000000000001E-2</v>
-      </c>
-      <c r="H37" s="132" t="s">
-        <v>280</v>
-      </c>
-      <c r="I37" s="132"/>
-    </row>
-    <row r="38" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B38" s="120"/>
-      <c r="C38" s="26" t="s">
-        <v>328</v>
-      </c>
-      <c r="D38" s="146" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="F38" s="147" t="s">
-        <v>332</v>
-      </c>
-      <c r="G38" s="148">
-        <v>1.9699999999999999E-2</v>
-      </c>
-      <c r="H38" s="147"/>
-      <c r="I38" s="147" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="120"/>
-      <c r="C39" s="26" t="s">
-        <v>329</v>
-      </c>
-      <c r="D39" s="146" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F39" s="147" t="s">
-        <v>333</v>
-      </c>
-      <c r="G39" s="148">
-        <v>2.0199999999999999E-2</v>
-      </c>
-      <c r="H39" s="147"/>
-      <c r="I39" s="147" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B40" s="120"/>
-      <c r="C40" s="26" t="s">
-        <v>330</v>
-      </c>
-      <c r="D40" s="146" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="F40" s="147" t="s">
-        <v>334</v>
-      </c>
-      <c r="G40" s="148">
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="H40" s="147" t="s">
-        <v>338</v>
-      </c>
-      <c r="I40" s="147"/>
-    </row>
-    <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B41" s="120"/>
-      <c r="C41" s="26" t="s">
-        <v>331</v>
-      </c>
-      <c r="D41" s="146" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" s="147" t="s">
-        <v>335</v>
-      </c>
-      <c r="G41" s="148">
-        <v>0.51039999999999996</v>
-      </c>
-      <c r="H41" s="147" t="s">
-        <v>336</v>
-      </c>
-      <c r="I41" s="147"/>
-    </row>
-    <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B42" s="120"/>
-      <c r="C42" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="D42" s="152" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>355</v>
-      </c>
-      <c r="F42" s="153" t="s">
-        <v>344</v>
-      </c>
-      <c r="G42" s="154">
-        <v>0.69550000000000001</v>
-      </c>
-      <c r="H42" s="153" t="s">
-        <v>280</v>
-      </c>
-      <c r="I42" s="153" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B43" s="120"/>
-      <c r="C43" s="27" t="s">
-        <v>340</v>
-      </c>
-      <c r="D43" s="152" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="27" t="s">
-        <v>355</v>
-      </c>
-      <c r="F43" s="153" t="s">
-        <v>342</v>
-      </c>
-      <c r="G43" s="154">
-        <v>0.69850000000000001</v>
-      </c>
-      <c r="H43" s="153" t="s">
-        <v>336</v>
-      </c>
-      <c r="I43" s="153"/>
-    </row>
-    <row r="44" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B44" s="120"/>
-      <c r="C44" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="D44" s="152" t="s">
-        <v>30</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" s="153" t="s">
-        <v>343</v>
-      </c>
-      <c r="G44" s="154">
-        <v>0.51249999999999996</v>
-      </c>
-      <c r="H44" s="153" t="s">
-        <v>97</v>
-      </c>
-      <c r="I44" s="153"/>
-    </row>
-    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B45" s="120"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B46" s="120"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B47" s="120"/>
-      <c r="C47" s="27" t="s">
-        <v>345</v>
-      </c>
-      <c r="D47" s="152" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="27" t="s">
-        <v>355</v>
-      </c>
-      <c r="F47" s="153" t="s">
-        <v>352</v>
-      </c>
-      <c r="G47" s="154">
-        <v>0.70230000000000004</v>
-      </c>
-      <c r="H47" s="153" t="s">
-        <v>83</v>
-      </c>
-      <c r="I47" s="153" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B48" s="120"/>
-      <c r="C48" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D48" s="152" t="s">
-        <v>30</v>
-      </c>
-      <c r="E48" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="153" t="s">
-        <v>361</v>
-      </c>
-      <c r="G48" s="154">
-        <v>0.55220000000000002</v>
-      </c>
-      <c r="H48" s="153" t="s">
-        <v>83</v>
-      </c>
-      <c r="I48" s="153" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B49" s="120"/>
-      <c r="C49" s="27" t="s">
-        <v>362</v>
-      </c>
-      <c r="D49" s="152" t="s">
+      <c r="C49" s="13"/>
+      <c r="D49" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E49" s="27" t="s">
-        <v>355</v>
-      </c>
-      <c r="F49" s="153" t="s">
-        <v>350</v>
-      </c>
-      <c r="G49" s="154">
-        <v>0.70760000000000001</v>
-      </c>
-      <c r="H49" s="153" t="s">
-        <v>97</v>
-      </c>
-      <c r="I49" s="153" t="s">
-        <v>282</v>
-      </c>
+      <c r="E49" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
     </row>
     <row r="50" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" s="120"/>
-      <c r="C50" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="D50" s="152" t="s">
+      <c r="C50" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="D50" s="142" t="s">
         <v>30</v>
       </c>
-      <c r="E50" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="153" t="s">
-        <v>351</v>
-      </c>
-      <c r="G50" s="154">
-        <v>0.51180000000000003</v>
-      </c>
-      <c r="H50" s="153" t="s">
+      <c r="E50" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="F50" s="142" t="s">
+        <v>358</v>
+      </c>
+      <c r="G50" s="143">
+        <v>0.67720000000000002</v>
+      </c>
+      <c r="H50" s="142" t="s">
         <v>322</v>
       </c>
-      <c r="I50" s="153" t="s">
-        <v>282</v>
+      <c r="I50" s="142" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" s="120"/>
-      <c r="C51" s="28" t="s">
-        <v>366</v>
-      </c>
-      <c r="D51" s="157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="F51" s="160" t="s">
-        <v>372</v>
-      </c>
-      <c r="G51" s="159">
-        <v>0.69520000000000004</v>
-      </c>
-      <c r="H51" s="158"/>
-      <c r="I51" s="158"/>
+      <c r="C51" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="D51" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="F51" s="102" t="s">
+        <v>299</v>
+      </c>
+      <c r="G51" s="105">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="H51" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="I51" s="104" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="52" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" s="120"/>
-      <c r="C52" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D52" s="157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="160" t="s">
-        <v>373</v>
-      </c>
-      <c r="G52" s="159">
-        <v>0.52629999999999999</v>
-      </c>
-      <c r="H52" s="158"/>
-      <c r="I52" s="158"/>
+      <c r="C52" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="F52" s="102" t="s">
+        <v>300</v>
+      </c>
+      <c r="G52" s="105">
+        <v>0.1991</v>
+      </c>
+      <c r="H52" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="I52" s="104" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="53" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" s="120"/>
-      <c r="C53" s="28" t="s">
-        <v>370</v>
-      </c>
-      <c r="D53" s="157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="F53" s="160" t="s">
-        <v>376</v>
-      </c>
-      <c r="G53" s="159">
-        <v>0.68289999999999995</v>
-      </c>
-      <c r="H53" s="158" t="s">
-        <v>386</v>
-      </c>
-      <c r="I53" s="158"/>
+      <c r="C53" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D53" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="F53" s="102" t="s">
+        <v>301</v>
+      </c>
+      <c r="G53" s="105">
+        <v>0.56259999999999999</v>
+      </c>
+      <c r="H53" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="I53" s="104" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="54" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B54" s="120"/>
-      <c r="C54" s="28" t="s">
-        <v>371</v>
-      </c>
-      <c r="D54" s="157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" s="160" t="s">
-        <v>382</v>
-      </c>
-      <c r="G54" s="159">
-        <v>0.51270000000000004</v>
-      </c>
-      <c r="H54" s="158"/>
-      <c r="I54" s="158"/>
+      <c r="C54" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="D54" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="F54" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="136">
+        <v>0.1024</v>
+      </c>
+      <c r="H54" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="I54" s="132"/>
     </row>
     <row r="55" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" s="120"/>
-      <c r="C55" s="166" t="s">
-        <v>374</v>
-      </c>
-      <c r="D55" s="157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="F55" s="160" t="s">
-        <v>377</v>
-      </c>
-      <c r="G55" s="159">
-        <v>0.6875</v>
-      </c>
-      <c r="H55" s="158" t="s">
-        <v>386</v>
-      </c>
-      <c r="I55" s="158"/>
+      <c r="C55" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="D55" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="F55" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55" s="136">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H55" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="I55" s="132"/>
     </row>
     <row r="56" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B56" s="120"/>
-      <c r="C56" s="28" t="s">
-        <v>375</v>
-      </c>
-      <c r="D56" s="157" t="s">
-        <v>30</v>
-      </c>
-      <c r="E56" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" s="160" t="s">
-        <v>383</v>
-      </c>
-      <c r="G56" s="159">
-        <v>0.52739999999999998</v>
-      </c>
-      <c r="H56" s="158"/>
-      <c r="I56" s="158"/>
+      <c r="C56" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="D56" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="F56" s="132" t="s">
+        <v>50</v>
+      </c>
+      <c r="G56" s="136">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="H56" s="132" t="s">
+        <v>280</v>
+      </c>
+      <c r="I56" s="132"/>
     </row>
     <row r="57" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" s="120"/>
-      <c r="C57" s="166" t="s">
-        <v>378</v>
-      </c>
-      <c r="D57" s="157" t="s">
+      <c r="C57" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="D57" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E57" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="F57" s="158" t="s">
-        <v>368</v>
-      </c>
-      <c r="G57" s="159">
-        <v>0.71379999999999999</v>
-      </c>
-      <c r="H57" s="158"/>
-      <c r="I57" s="158" t="s">
-        <v>404</v>
+      <c r="E57" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="F57" s="147" t="s">
+        <v>332</v>
+      </c>
+      <c r="G57" s="148">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="H57" s="147"/>
+      <c r="I57" s="147" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B58" s="120"/>
-      <c r="C58" s="28" t="s">
-        <v>379</v>
-      </c>
-      <c r="D58" s="157" t="s">
+      <c r="C58" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D58" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E58" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F58" s="158" t="s">
-        <v>369</v>
-      </c>
-      <c r="G58" s="159">
-        <v>0.59970000000000001</v>
-      </c>
-      <c r="H58" s="158"/>
-      <c r="I58" s="158" t="s">
-        <v>405</v>
+      <c r="E58" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="147" t="s">
+        <v>333</v>
+      </c>
+      <c r="G58" s="148">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="H58" s="147"/>
+      <c r="I58" s="147" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B59" s="120"/>
-      <c r="C59" s="28" t="s">
-        <v>380</v>
-      </c>
-      <c r="D59" s="157" t="s">
+      <c r="C59" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D59" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E59" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="F59" s="158" t="s">
-        <v>384</v>
-      </c>
-      <c r="G59" s="159">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="H59" s="158"/>
-      <c r="I59" s="158" t="s">
-        <v>406</v>
-      </c>
+      <c r="E59" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="F59" s="147" t="s">
+        <v>334</v>
+      </c>
+      <c r="G59" s="148">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="H59" s="147" t="s">
+        <v>338</v>
+      </c>
+      <c r="I59" s="147"/>
     </row>
     <row r="60" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="120"/>
-      <c r="C60" s="166" t="s">
-        <v>381</v>
-      </c>
-      <c r="D60" s="157" t="s">
+      <c r="C60" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="D60" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="E60" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F60" s="158" t="s">
-        <v>385</v>
-      </c>
-      <c r="G60" s="159">
-        <v>0.58930000000000005</v>
-      </c>
-      <c r="H60" s="158"/>
-      <c r="I60" s="158" t="s">
-        <v>405</v>
-      </c>
+      <c r="E60" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="147" t="s">
+        <v>335</v>
+      </c>
+      <c r="G60" s="148">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="H60" s="147" t="s">
+        <v>336</v>
+      </c>
+      <c r="I60" s="147"/>
     </row>
     <row r="61" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" s="120"/>
-      <c r="C61" s="166" t="s">
-        <v>388</v>
-      </c>
-      <c r="D61" s="157" t="s">
+      <c r="C61" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="D61" s="152" t="s">
         <v>30</v>
       </c>
-      <c r="E61" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="F61" s="158" t="s">
-        <v>413</v>
-      </c>
-      <c r="G61" s="159"/>
-      <c r="H61" s="158"/>
-      <c r="I61" s="158"/>
+      <c r="E61" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="F61" s="153" t="s">
+        <v>344</v>
+      </c>
+      <c r="G61" s="154">
+        <v>0.69550000000000001</v>
+      </c>
+      <c r="H61" s="153" t="s">
+        <v>280</v>
+      </c>
+      <c r="I61" s="153" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="62" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="120"/>
-      <c r="C62" s="166" t="s">
-        <v>389</v>
-      </c>
-      <c r="D62" s="157" t="s">
+      <c r="C62" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="D62" s="152" t="s">
         <v>30</v>
       </c>
-      <c r="E62" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F62" s="158" t="s">
-        <v>414</v>
-      </c>
-      <c r="G62" s="159"/>
-      <c r="H62" s="158"/>
-      <c r="I62" s="158"/>
+      <c r="E62" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="F62" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="G62" s="154">
+        <v>0.69850000000000001</v>
+      </c>
+      <c r="H62" s="153" t="s">
+        <v>336</v>
+      </c>
+      <c r="I62" s="153"/>
     </row>
     <row r="63" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B63" s="120"/>
-      <c r="C63" s="29" t="s">
-        <v>390</v>
-      </c>
-      <c r="D63" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="29" t="s">
-        <v>355</v>
-      </c>
-      <c r="F63" s="164" t="s">
-        <v>407</v>
-      </c>
-      <c r="G63" s="165"/>
-      <c r="H63" s="162"/>
-      <c r="I63" s="162"/>
+      <c r="C63" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="D63" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" s="153" t="s">
+        <v>343</v>
+      </c>
+      <c r="G63" s="154">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="H63" s="153" t="s">
+        <v>97</v>
+      </c>
+      <c r="I63" s="153"/>
     </row>
     <row r="64" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B64" s="120"/>
-      <c r="C64" s="29" t="s">
-        <v>391</v>
-      </c>
-      <c r="D64" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="29" t="s">
-        <v>355</v>
-      </c>
-      <c r="F64" s="164" t="s">
-        <v>408</v>
-      </c>
-      <c r="G64" s="165"/>
-      <c r="H64" s="162"/>
-      <c r="I64" s="162"/>
+      <c r="C64" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D64" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="F64" s="153" t="s">
+        <v>350</v>
+      </c>
+      <c r="G64" s="154">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="H64" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="I64" s="153" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="65" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B65" s="120"/>
-      <c r="C65" s="29" t="s">
-        <v>392</v>
-      </c>
-      <c r="D65" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="E65" s="29" t="s">
-        <v>355</v>
-      </c>
-      <c r="F65" s="164" t="s">
-        <v>409</v>
-      </c>
-      <c r="G65" s="165"/>
-      <c r="H65" s="162"/>
-      <c r="I65" s="162"/>
+      <c r="C65" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="D65" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F65" s="153" t="s">
+        <v>359</v>
+      </c>
+      <c r="G65" s="154">
+        <v>0.55220000000000002</v>
+      </c>
+      <c r="H65" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="I65" s="153" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="66" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="120"/>
-      <c r="C66" s="29" t="s">
-        <v>393</v>
-      </c>
-      <c r="D66" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F66" s="164" t="s">
-        <v>410</v>
-      </c>
-      <c r="G66" s="165"/>
-      <c r="H66" s="162"/>
-      <c r="I66" s="162"/>
+      <c r="C66" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="D66" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="F66" s="153" t="s">
+        <v>348</v>
+      </c>
+      <c r="G66" s="154">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="H66" s="153" t="s">
+        <v>97</v>
+      </c>
+      <c r="I66" s="153" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="67" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" s="120"/>
-      <c r="C67" s="29" t="s">
-        <v>397</v>
-      </c>
-      <c r="D67" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F67" s="164" t="s">
-        <v>411</v>
-      </c>
-      <c r="G67" s="165"/>
-      <c r="H67" s="162"/>
-      <c r="I67" s="162"/>
+      <c r="C67" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="D67" s="152" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="153" t="s">
+        <v>349</v>
+      </c>
+      <c r="G67" s="154">
+        <v>0.51180000000000003</v>
+      </c>
+      <c r="H67" s="153" t="s">
+        <v>322</v>
+      </c>
+      <c r="I67" s="153" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="68" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B68" s="120"/>
-      <c r="C68" s="29" t="s">
-        <v>398</v>
-      </c>
-      <c r="D68" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="E68" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F68" s="164" t="s">
-        <v>412</v>
-      </c>
-      <c r="G68" s="165"/>
-      <c r="H68" s="162"/>
-      <c r="I68" s="162"/>
+      <c r="C68" s="28" t="s">
+        <v>364</v>
+      </c>
+      <c r="D68" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E68" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F68" s="160" t="s">
+        <v>370</v>
+      </c>
+      <c r="G68" s="159">
+        <v>0.69520000000000004</v>
+      </c>
+      <c r="H68" s="158"/>
+      <c r="I68" s="158"/>
     </row>
     <row r="69" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B69" s="120"/>
-      <c r="C69" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="D69" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="G69" s="2"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
+      <c r="C69" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="D69" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E69" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F69" s="160" t="s">
+        <v>371</v>
+      </c>
+      <c r="G69" s="159">
+        <v>0.52629999999999999</v>
+      </c>
+      <c r="H69" s="158"/>
+      <c r="I69" s="158"/>
     </row>
     <row r="70" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B70" s="120"/>
-      <c r="C70" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="D70" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
+      <c r="C70" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="D70" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F70" s="160" t="s">
+        <v>374</v>
+      </c>
+      <c r="G70" s="159">
+        <v>0.68289999999999995</v>
+      </c>
+      <c r="H70" s="158" t="s">
+        <v>384</v>
+      </c>
+      <c r="I70" s="158"/>
     </row>
     <row r="71" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B71" s="120"/>
-      <c r="C71" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="D71" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="G71" s="2"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C71" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="D71" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" s="160" t="s">
+        <v>380</v>
+      </c>
+      <c r="G71" s="159">
+        <v>0.51270000000000004</v>
+      </c>
+      <c r="H71" s="158"/>
+      <c r="I71" s="158"/>
+    </row>
+    <row r="72" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B72" s="120"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C72" s="166" t="s">
+        <v>372</v>
+      </c>
+      <c r="D72" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F72" s="160" t="s">
+        <v>375</v>
+      </c>
+      <c r="G72" s="159">
+        <v>0.6875</v>
+      </c>
+      <c r="H72" s="158" t="s">
+        <v>384</v>
+      </c>
+      <c r="I72" s="158"/>
+    </row>
+    <row r="73" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B73" s="120"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="61"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C73" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="D73" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F73" s="160" t="s">
+        <v>381</v>
+      </c>
+      <c r="G73" s="159">
+        <v>0.52739999999999998</v>
+      </c>
+      <c r="H73" s="158"/>
+      <c r="I73" s="158"/>
+    </row>
+    <row r="74" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B74" s="120"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="61"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C74" s="166" t="s">
+        <v>376</v>
+      </c>
+      <c r="D74" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F74" s="158" t="s">
+        <v>366</v>
+      </c>
+      <c r="G74" s="159">
+        <v>0.71379999999999999</v>
+      </c>
+      <c r="H74" s="158"/>
+      <c r="I74" s="158" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B75" s="120"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C75" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="D75" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="158" t="s">
+        <v>367</v>
+      </c>
+      <c r="G75" s="159">
+        <v>0.59970000000000001</v>
+      </c>
+      <c r="H75" s="158"/>
+      <c r="I75" s="158" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B76" s="120"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="61"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-    </row>
-    <row r="77" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="121"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
+      <c r="C76" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="D76" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F76" s="158" t="s">
+        <v>382</v>
+      </c>
+      <c r="G76" s="159">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="H76" s="158"/>
+      <c r="I76" s="158" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B77" s="120"/>
+      <c r="C77" s="166" t="s">
+        <v>379</v>
+      </c>
+      <c r="D77" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F77" s="158" t="s">
+        <v>383</v>
+      </c>
+      <c r="G77" s="159">
+        <v>0.58930000000000005</v>
+      </c>
+      <c r="H77" s="158"/>
+      <c r="I77" s="158" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="78" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="B78" s="119" t="s">
-        <v>245</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="D78" s="98" t="s">
+      <c r="B78" s="120"/>
+      <c r="C78" s="166" t="s">
+        <v>386</v>
+      </c>
+      <c r="D78" s="157" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="22"/>
-      <c r="F78" s="98" t="s">
-        <v>275</v>
-      </c>
-      <c r="G78" s="99">
-        <v>0.4929</v>
-      </c>
-      <c r="H78" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="I78" s="98" t="s">
-        <v>282</v>
-      </c>
+      <c r="E78" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="F78" s="172" t="s">
+        <v>402</v>
+      </c>
+      <c r="G78" s="159">
+        <v>0.71630000000000005</v>
+      </c>
+      <c r="H78" s="158" t="s">
+        <v>406</v>
+      </c>
+      <c r="I78" s="158"/>
     </row>
     <row r="79" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B79" s="120"/>
-      <c r="C79" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="D79" s="98" t="s">
+      <c r="C79" s="167" t="s">
+        <v>387</v>
+      </c>
+      <c r="D79" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="E79" s="22"/>
-      <c r="F79" s="98" t="s">
-        <v>277</v>
-      </c>
-      <c r="G79" s="99">
-        <v>0.66930000000000001</v>
-      </c>
-      <c r="H79" s="98" t="s">
-        <v>281</v>
-      </c>
-      <c r="I79" s="98" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="E79" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F79" s="173" t="s">
+        <v>403</v>
+      </c>
+      <c r="G79" s="165">
+        <v>0.63239999999999996</v>
+      </c>
+      <c r="H79" s="162"/>
+      <c r="I79" s="162"/>
+    </row>
+    <row r="80" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B80" s="120"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="13"/>
-      <c r="F80" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-    </row>
-    <row r="81" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="C80" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D80" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F80" s="164" t="s">
+        <v>407</v>
+      </c>
+      <c r="G80" s="165">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H80" s="169" t="s">
+        <v>428</v>
+      </c>
+      <c r="I80" s="162"/>
+    </row>
+    <row r="81" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B81" s="120"/>
-      <c r="C81" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="D81" s="142" t="s">
-        <v>30</v>
-      </c>
-      <c r="E81" s="25"/>
-      <c r="F81" s="142" t="s">
-        <v>278</v>
-      </c>
-      <c r="G81" s="143">
-        <v>0.67969999999999997</v>
-      </c>
-      <c r="H81" s="142" t="s">
-        <v>327</v>
-      </c>
-      <c r="I81" s="142"/>
+      <c r="C81" s="170" t="s">
+        <v>427</v>
+      </c>
+      <c r="D81" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F81" s="164" t="s">
+        <v>477</v>
+      </c>
+      <c r="G81" s="165"/>
+      <c r="H81" s="162"/>
+      <c r="I81" s="162"/>
     </row>
     <row r="82" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B82" s="120"/>
-      <c r="C82" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="D82" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" s="23"/>
-      <c r="F82" s="102" t="s">
-        <v>302</v>
-      </c>
-      <c r="G82" s="105">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="H82" s="145" t="s">
-        <v>323</v>
-      </c>
-      <c r="I82" s="104" t="s">
-        <v>287</v>
-      </c>
+      <c r="C82" s="171" t="s">
+        <v>389</v>
+      </c>
+      <c r="D82" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E82" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F82" s="164" t="s">
+        <v>408</v>
+      </c>
+      <c r="G82" s="165">
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="H82" s="162" t="s">
+        <v>473</v>
+      </c>
+      <c r="I82" s="162"/>
     </row>
     <row r="83" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B83" s="120"/>
-      <c r="C83" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="D83" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E83" s="23"/>
-      <c r="F83" s="102" t="s">
-        <v>303</v>
-      </c>
-      <c r="G83" s="105">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="H83" s="106">
-        <v>50</v>
-      </c>
-      <c r="I83" s="104" t="s">
-        <v>287</v>
-      </c>
+      <c r="C83" s="170" t="s">
+        <v>475</v>
+      </c>
+      <c r="D83" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F83" s="164" t="s">
+        <v>478</v>
+      </c>
+      <c r="G83" s="165"/>
+      <c r="H83" s="162"/>
+      <c r="I83" s="162"/>
     </row>
     <row r="84" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B84" s="120"/>
-      <c r="C84" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="D84" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E84" s="23"/>
-      <c r="F84" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="G84" s="105">
-        <v>0.54239999999999999</v>
-      </c>
-      <c r="H84" s="106" t="s">
-        <v>321</v>
-      </c>
-      <c r="I84" s="104" t="s">
-        <v>287</v>
-      </c>
+      <c r="C84" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="D84" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E84" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F84" s="164" t="s">
+        <v>409</v>
+      </c>
+      <c r="G84" s="165">
+        <v>0.62609999999999999</v>
+      </c>
+      <c r="H84" s="162" t="s">
+        <v>422</v>
+      </c>
+      <c r="I84" s="162"/>
     </row>
     <row r="85" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B85" s="120"/>
-      <c r="C85" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="D85" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E85" s="24"/>
-      <c r="F85" s="132" t="s">
-        <v>47</v>
-      </c>
-      <c r="G85" s="136">
-        <v>7.7899999999999997E-2</v>
-      </c>
-      <c r="H85" s="132" t="s">
-        <v>281</v>
-      </c>
-      <c r="I85" s="132"/>
+      <c r="C85" s="170" t="s">
+        <v>476</v>
+      </c>
+      <c r="D85" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E85" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F85" s="164" t="s">
+        <v>479</v>
+      </c>
+      <c r="G85" s="165"/>
+      <c r="H85" s="162"/>
+      <c r="I85" s="162"/>
     </row>
     <row r="86" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B86" s="120"/>
-      <c r="C86" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="D86" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="E86" s="24"/>
-      <c r="F86" s="132" t="s">
-        <v>49</v>
-      </c>
-      <c r="G86" s="136">
-        <v>3.2099999999999997E-2</v>
-      </c>
-      <c r="H86" s="132" t="s">
-        <v>281</v>
-      </c>
-      <c r="I86" s="132"/>
+      <c r="C86" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="D86" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F86" s="164" t="s">
+        <v>410</v>
+      </c>
+      <c r="G86" s="165">
+        <v>2.81E-2</v>
+      </c>
+      <c r="H86" s="162" t="s">
+        <v>429</v>
+      </c>
+      <c r="I86" s="162"/>
     </row>
     <row r="87" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B87" s="120"/>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="170" t="s">
+        <v>430</v>
+      </c>
+      <c r="D87" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F87" s="164" t="s">
+        <v>480</v>
+      </c>
+      <c r="G87" s="165"/>
+      <c r="H87" s="162"/>
+      <c r="I87" s="162"/>
+    </row>
+    <row r="88" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B88" s="120"/>
+      <c r="C88" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="D88" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F88" s="164" t="s">
+        <v>412</v>
+      </c>
+      <c r="G88" s="165">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="H88" s="162" t="s">
+        <v>423</v>
+      </c>
+      <c r="I88" s="162"/>
+    </row>
+    <row r="89" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B89" s="120"/>
+      <c r="C89" s="170" t="s">
+        <v>483</v>
+      </c>
+      <c r="D89" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E89" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F89" s="164" t="s">
+        <v>481</v>
+      </c>
+      <c r="G89" s="165"/>
+      <c r="H89" s="162"/>
+      <c r="I89" s="162"/>
+    </row>
+    <row r="90" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B90" s="120"/>
+      <c r="C90" s="171" t="s">
+        <v>393</v>
+      </c>
+      <c r="D90" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F90" s="164" t="s">
+        <v>411</v>
+      </c>
+      <c r="G90" s="165">
+        <v>0.40510000000000002</v>
+      </c>
+      <c r="H90" s="162" t="s">
+        <v>474</v>
+      </c>
+      <c r="I90" s="162" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="120"/>
+      <c r="C91" s="170" t="s">
+        <v>484</v>
+      </c>
+      <c r="D91" s="174" t="s">
+        <v>36</v>
+      </c>
+      <c r="E91" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="F91" s="191" t="s">
+        <v>482</v>
+      </c>
+      <c r="G91" s="176"/>
+      <c r="H91" s="175"/>
+      <c r="I91" s="175"/>
+    </row>
+    <row r="92" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B92" s="120"/>
+      <c r="C92" s="189"/>
+      <c r="D92" s="192" t="s">
+        <v>46</v>
+      </c>
+      <c r="E92" s="180" t="s">
+        <v>353</v>
+      </c>
+      <c r="F92" s="181" t="s">
+        <v>413</v>
+      </c>
+      <c r="G92" s="182">
+        <v>0.12005</v>
+      </c>
+      <c r="H92" s="181"/>
+      <c r="I92" s="183"/>
+    </row>
+    <row r="93" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B93" s="120"/>
+      <c r="C93" s="189"/>
+      <c r="D93" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E93" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F93" s="162" t="s">
+        <v>414</v>
+      </c>
+      <c r="G93" s="165">
+        <v>3.6013999999999997E-2</v>
+      </c>
+      <c r="H93" s="162"/>
+      <c r="I93" s="184"/>
+    </row>
+    <row r="94" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B94" s="120"/>
+      <c r="C94" s="189"/>
+      <c r="D94" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F94" s="162" t="s">
+        <v>415</v>
+      </c>
+      <c r="G94" s="165">
+        <v>2.6800000000000001E-2</v>
+      </c>
+      <c r="H94" s="162"/>
+      <c r="I94" s="184"/>
+    </row>
+    <row r="95" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B95" s="120"/>
+      <c r="C95" s="189"/>
+      <c r="D95" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E95" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F95" s="162" t="s">
+        <v>440</v>
+      </c>
+      <c r="G95" s="165">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="H95" s="162"/>
+      <c r="I95" s="184"/>
+    </row>
+    <row r="96" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B96" s="120"/>
+      <c r="C96" s="189"/>
+      <c r="D96" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F96" s="162" t="s">
+        <v>441</v>
+      </c>
+      <c r="G96" s="165">
+        <v>0.2064</v>
+      </c>
+      <c r="H96" s="162"/>
+      <c r="I96" s="184"/>
+    </row>
+    <row r="97" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B97" s="120"/>
+      <c r="C97" s="189"/>
+      <c r="D97" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F97" s="162" t="s">
+        <v>442</v>
+      </c>
+      <c r="G97" s="165"/>
+      <c r="H97" s="162"/>
+      <c r="I97" s="184"/>
+    </row>
+    <row r="98" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B98" s="120"/>
+      <c r="C98" s="189"/>
+      <c r="D98" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F98" s="162" t="s">
+        <v>443</v>
+      </c>
+      <c r="G98" s="165"/>
+      <c r="H98" s="162"/>
+      <c r="I98" s="184"/>
+    </row>
+    <row r="99" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B99" s="120"/>
+      <c r="C99" s="189"/>
+      <c r="D99" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F99" s="162" t="s">
+        <v>444</v>
+      </c>
+      <c r="G99" s="165"/>
+      <c r="H99" s="162"/>
+      <c r="I99" s="184"/>
+    </row>
+    <row r="100" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B100" s="120"/>
+      <c r="C100" s="189"/>
+      <c r="D100" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E100" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F100" s="162" t="s">
+        <v>445</v>
+      </c>
+      <c r="G100" s="165">
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="H100" s="162"/>
+      <c r="I100" s="184"/>
+    </row>
+    <row r="101" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B101" s="120"/>
+      <c r="C101" s="189"/>
+      <c r="D101" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E101" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F101" s="162" t="s">
+        <v>446</v>
+      </c>
+      <c r="G101" s="165">
+        <v>0.1958</v>
+      </c>
+      <c r="H101" s="162"/>
+      <c r="I101" s="184"/>
+    </row>
+    <row r="102" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B102" s="120"/>
+      <c r="C102" s="189"/>
+      <c r="D102" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E102" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F102" s="162" t="s">
+        <v>447</v>
+      </c>
+      <c r="G102" s="165">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="H102" s="162"/>
+      <c r="I102" s="184"/>
+    </row>
+    <row r="103" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="120"/>
+      <c r="C103" s="190"/>
+      <c r="D103" s="194" t="s">
+        <v>46</v>
+      </c>
+      <c r="E103" s="185" t="s">
+        <v>353</v>
+      </c>
+      <c r="F103" s="186" t="s">
+        <v>448</v>
+      </c>
+      <c r="G103" s="187">
+        <v>0.1017</v>
+      </c>
+      <c r="H103" s="186"/>
+      <c r="I103" s="188"/>
+    </row>
+    <row r="104" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B104" s="120"/>
+      <c r="C104" s="195"/>
+      <c r="D104" s="192" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104" s="180" t="s">
+        <v>36</v>
+      </c>
+      <c r="F104" s="181" t="s">
+        <v>420</v>
+      </c>
+      <c r="G104" s="182">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="H104" s="181"/>
+      <c r="I104" s="183"/>
+    </row>
+    <row r="105" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B105" s="120"/>
+      <c r="C105" s="196"/>
+      <c r="D105" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E105" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F105" s="162" t="s">
+        <v>419</v>
+      </c>
+      <c r="G105" s="165">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="H105" s="162"/>
+      <c r="I105" s="184"/>
+    </row>
+    <row r="106" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B106" s="120"/>
+      <c r="C106" s="196"/>
+      <c r="D106" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" s="162" t="s">
+        <v>421</v>
+      </c>
+      <c r="G106" s="165">
+        <v>1.52E-2</v>
+      </c>
+      <c r="H106" s="162"/>
+      <c r="I106" s="184"/>
+    </row>
+    <row r="107" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B107" s="120"/>
+      <c r="C107" s="196"/>
+      <c r="D107" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E107" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F107" s="162" t="s">
+        <v>431</v>
+      </c>
+      <c r="G107" s="165">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="H107" s="162"/>
+      <c r="I107" s="184"/>
+    </row>
+    <row r="108" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B108" s="120"/>
+      <c r="C108" s="196"/>
+      <c r="D108" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E108" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F108" s="162" t="s">
+        <v>432</v>
+      </c>
+      <c r="G108" s="165">
+        <v>0.1211</v>
+      </c>
+      <c r="H108" s="162"/>
+      <c r="I108" s="184"/>
+    </row>
+    <row r="109" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B109" s="120"/>
+      <c r="C109" s="196"/>
+      <c r="D109" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E109" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F109" s="162" t="s">
+        <v>433</v>
+      </c>
+      <c r="G109" s="165"/>
+      <c r="H109" s="162"/>
+      <c r="I109" s="184"/>
+    </row>
+    <row r="110" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B110" s="120"/>
+      <c r="C110" s="196"/>
+      <c r="D110" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E110" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F110" s="162" t="s">
+        <v>434</v>
+      </c>
+      <c r="G110" s="165"/>
+      <c r="H110" s="162"/>
+      <c r="I110" s="184"/>
+    </row>
+    <row r="111" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B111" s="120"/>
+      <c r="C111" s="196"/>
+      <c r="D111" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E111" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F111" s="162" t="s">
+        <v>435</v>
+      </c>
+      <c r="G111" s="165"/>
+      <c r="H111" s="162"/>
+      <c r="I111" s="184"/>
+    </row>
+    <row r="112" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B112" s="120"/>
+      <c r="C112" s="196"/>
+      <c r="D112" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E112" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F112" s="162" t="s">
+        <v>436</v>
+      </c>
+      <c r="G112" s="165">
+        <v>0.121</v>
+      </c>
+      <c r="H112" s="162"/>
+      <c r="I112" s="184"/>
+    </row>
+    <row r="113" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B113" s="120"/>
+      <c r="C113" s="196"/>
+      <c r="D113" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E113" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F113" s="162" t="s">
+        <v>437</v>
+      </c>
+      <c r="G113" s="165">
+        <v>0.1196</v>
+      </c>
+      <c r="H113" s="162"/>
+      <c r="I113" s="184"/>
+    </row>
+    <row r="114" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B114" s="120"/>
+      <c r="C114" s="196"/>
+      <c r="D114" s="193" t="s">
+        <v>46</v>
+      </c>
+      <c r="E114" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F114" s="162" t="s">
+        <v>438</v>
+      </c>
+      <c r="G114" s="165">
+        <v>0.1023</v>
+      </c>
+      <c r="H114" s="162"/>
+      <c r="I114" s="184"/>
+    </row>
+    <row r="115" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="120"/>
+      <c r="C115" s="197"/>
+      <c r="D115" s="194" t="s">
+        <v>46</v>
+      </c>
+      <c r="E115" s="185" t="s">
+        <v>36</v>
+      </c>
+      <c r="F115" s="186" t="s">
+        <v>439</v>
+      </c>
+      <c r="G115" s="187">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="H115" s="186"/>
+      <c r="I115" s="188"/>
+    </row>
+    <row r="116" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B116" s="120"/>
+      <c r="C116" s="178"/>
+      <c r="D116" s="177" t="s">
+        <v>46</v>
+      </c>
+      <c r="E116" s="178" t="s">
+        <v>36</v>
+      </c>
+      <c r="F116" s="179" t="s">
+        <v>487</v>
+      </c>
+      <c r="G116" s="198"/>
+      <c r="H116" s="179"/>
+      <c r="I116" s="179"/>
+    </row>
+    <row r="117" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B117" s="120"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E117" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F117" s="162" t="s">
+        <v>488</v>
+      </c>
+      <c r="G117" s="165"/>
+      <c r="H117" s="162"/>
+      <c r="I117" s="162"/>
+    </row>
+    <row r="118" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B118" s="120"/>
+      <c r="C118" s="29"/>
+      <c r="D118" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E118" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F118" s="162" t="s">
+        <v>489</v>
+      </c>
+      <c r="G118" s="165"/>
+      <c r="H118" s="162"/>
+      <c r="I118" s="162"/>
+    </row>
+    <row r="119" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B119" s="120"/>
+      <c r="C119" s="29"/>
+      <c r="D119" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E119" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F119" s="162" t="s">
+        <v>490</v>
+      </c>
+      <c r="G119" s="165"/>
+      <c r="H119" s="162"/>
+      <c r="I119" s="162"/>
+    </row>
+    <row r="120" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B120" s="120"/>
+      <c r="C120" s="29"/>
+      <c r="D120" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E120" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F120" s="162" t="s">
+        <v>491</v>
+      </c>
+      <c r="G120" s="165"/>
+      <c r="H120" s="162"/>
+      <c r="I120" s="162"/>
+    </row>
+    <row r="121" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B121" s="120"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E121" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F121" s="162" t="s">
+        <v>492</v>
+      </c>
+      <c r="G121" s="165"/>
+      <c r="H121" s="162"/>
+      <c r="I121" s="162"/>
+    </row>
+    <row r="122" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B122" s="120"/>
+      <c r="C122" s="29"/>
+      <c r="D122" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E122" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F122" s="162" t="s">
+        <v>493</v>
+      </c>
+      <c r="G122" s="165"/>
+      <c r="H122" s="162"/>
+      <c r="I122" s="162"/>
+    </row>
+    <row r="123" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B123" s="120"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E123" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F123" s="162" t="s">
+        <v>494</v>
+      </c>
+      <c r="G123" s="165"/>
+      <c r="H123" s="162"/>
+      <c r="I123" s="162"/>
+    </row>
+    <row r="124" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B124" s="120"/>
+      <c r="C124" s="29"/>
+      <c r="D124" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E124" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F124" s="162" t="s">
+        <v>495</v>
+      </c>
+      <c r="G124" s="165"/>
+      <c r="H124" s="162"/>
+      <c r="I124" s="162"/>
+    </row>
+    <row r="125" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B125" s="120"/>
+      <c r="C125" s="29"/>
+      <c r="D125" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E125" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F125" s="162" t="s">
+        <v>496</v>
+      </c>
+      <c r="G125" s="165"/>
+      <c r="H125" s="162"/>
+      <c r="I125" s="162"/>
+    </row>
+    <row r="126" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B126" s="120"/>
+      <c r="C126" s="29"/>
+      <c r="D126" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E126" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F126" s="162" t="s">
+        <v>497</v>
+      </c>
+      <c r="G126" s="165"/>
+      <c r="H126" s="162"/>
+      <c r="I126" s="162"/>
+    </row>
+    <row r="127" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B127" s="120"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E127" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F127" s="162" t="s">
+        <v>498</v>
+      </c>
+      <c r="G127" s="165"/>
+      <c r="H127" s="162"/>
+      <c r="I127" s="162"/>
+    </row>
+    <row r="128" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B128" s="120"/>
+      <c r="C128" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="D128" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E128" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F128" s="162" t="s">
+        <v>485</v>
+      </c>
+      <c r="G128" s="165"/>
+      <c r="H128" s="162"/>
+      <c r="I128" s="162"/>
+    </row>
+    <row r="129" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B129" s="120"/>
+      <c r="C129" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="D129" s="163" t="s">
+        <v>46</v>
+      </c>
+      <c r="E129" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" s="162" t="s">
+        <v>486</v>
+      </c>
+      <c r="G129" s="165"/>
+      <c r="H129" s="162"/>
+      <c r="I129" s="162"/>
+    </row>
+    <row r="130" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B130" s="120"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="61"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G130" s="2"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B131" s="120"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="61"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B132" s="120"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="61"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B133" s="120"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="61"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B134" s="120"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="61"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B135" s="120"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="61"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+    </row>
+    <row r="136" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="121"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+    </row>
+    <row r="137" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B137" s="119" t="s">
+        <v>245</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D137" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E137" s="22"/>
+      <c r="F137" s="98" t="s">
+        <v>275</v>
+      </c>
+      <c r="G137" s="99">
+        <v>0.4929</v>
+      </c>
+      <c r="H137" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="I137" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B138" s="120"/>
+      <c r="C138" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="D138" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E138" s="22"/>
+      <c r="F138" s="98" t="s">
+        <v>277</v>
+      </c>
+      <c r="G138" s="99">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="H138" s="98" t="s">
+        <v>281</v>
+      </c>
+      <c r="I138" s="98" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B139" s="120"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E139" s="13"/>
+      <c r="F139" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G139" s="2"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+    </row>
+    <row r="140" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B140" s="120"/>
+      <c r="C140" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="D140" s="142" t="s">
+        <v>30</v>
+      </c>
+      <c r="E140" s="25"/>
+      <c r="F140" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G140" s="143">
+        <v>0.67969999999999997</v>
+      </c>
+      <c r="H140" s="142" t="s">
+        <v>327</v>
+      </c>
+      <c r="I140" s="142"/>
+    </row>
+    <row r="141" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B141" s="120"/>
+      <c r="C141" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="D141" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E141" s="23"/>
+      <c r="F141" s="102" t="s">
+        <v>302</v>
+      </c>
+      <c r="G141" s="105">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H141" s="145" t="s">
+        <v>323</v>
+      </c>
+      <c r="I141" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="142" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B142" s="120"/>
+      <c r="C142" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="D142" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E142" s="23"/>
+      <c r="F142" s="102" t="s">
+        <v>303</v>
+      </c>
+      <c r="G142" s="105">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="H142" s="106">
+        <v>50</v>
+      </c>
+      <c r="I142" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B143" s="120"/>
+      <c r="C143" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="D143" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E143" s="23"/>
+      <c r="F143" s="102" t="s">
+        <v>304</v>
+      </c>
+      <c r="G143" s="105">
+        <v>0.54239999999999999</v>
+      </c>
+      <c r="H143" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="I143" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="144" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B144" s="120"/>
+      <c r="C144" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D144" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E144" s="24"/>
+      <c r="F144" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="G144" s="136">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="H144" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I144" s="132"/>
+    </row>
+    <row r="145" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B145" s="120"/>
+      <c r="C145" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="D145" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="E145" s="24"/>
+      <c r="F145" s="132" t="s">
+        <v>49</v>
+      </c>
+      <c r="G145" s="136">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="H145" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="I145" s="132"/>
+    </row>
+    <row r="146" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B146" s="120"/>
+      <c r="C146" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D87" s="131" t="s">
+      <c r="D146" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="E87" s="24"/>
-      <c r="F87" s="132" t="s">
+      <c r="E146" s="24"/>
+      <c r="F146" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="G87" s="136">
+      <c r="G146" s="136">
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="H87" s="132" t="s">
+      <c r="H146" s="132" t="s">
         <v>281</v>
       </c>
-      <c r="I87" s="132"/>
-    </row>
-    <row r="88" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="121"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
+      <c r="I146" s="132"/>
+    </row>
+    <row r="147" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="121"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B78:B88"/>
-    <mergeCell ref="B4:B22"/>
+    <mergeCell ref="B137:B147"/>
+    <mergeCell ref="B4:B41"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B77"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B136"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="G27:G77">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>AND(E27="S", G27&gt;=LARGE(_xlfn._xlws.FILTER(G$27:G$77, E$27:E$77="S"), 3))</formula>
-    </cfRule>
-    <cfRule type="top10" dxfId="5" priority="7" rank="3"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D4:D1048576">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",E4)))</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46:G136">
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>AND(E46="S", G46&gt;=LARGE(_xlfn._xlws.FILTER(G$46:G$136, E$46:E$136="S"), 3))</formula>
+    </cfRule>
+    <cfRule type="top10" dxfId="0" priority="9" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[IMP] Sending round 5
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranathipoojary/Imperial/FYP/Brain-Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099EECBF-B323-7A42-8017-91E337970981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FD5B81-F51F-F24A-8EDA-D7D3714D2D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="760" windowWidth="14220" windowHeight="18360" activeTab="1" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
+    <workbookView xWindow="15160" yWindow="760" windowWidth="14240" windowHeight="9180" activeTab="2" xr2:uid="{3B9ED3F3-1652-324A-9B6F-F2810DA6453C}"/>
   </bookViews>
   <sheets>
     <sheet name="CIFAR-10" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="566">
   <si>
     <t>Early stop, 256 batch size, ReduceLROnPlateau, no label smoothing unless mentioned otherwise</t>
   </si>
@@ -1770,6 +1770,18 @@
   </si>
   <si>
     <t>Stanford dogs settings with correct resnet layers =4</t>
+  </si>
+  <si>
+    <t>NeuroZoom</t>
+  </si>
+  <si>
+    <t>NeuroFocus</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>Models</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +1991,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="58">
+  <fills count="59">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2309,6 +2321,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="66">
     <border>
@@ -3182,7 +3200,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="322">
+  <cellXfs count="336">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4134,6 +4152,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="58" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="58" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="58" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="24" fillId="58" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="58" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="24" fillId="58" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="58" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="58" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="58" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -4703,8 +4763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34122BB4-1EF2-ED42-BCD3-D5825C92F864}">
   <dimension ref="B1:N151"/>
   <sheetViews>
-    <sheetView topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7754,8 +7814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC4FE0-F2D6-F045-B950-561C0B4FDED8}">
   <dimension ref="B1:O198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="81" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="D175" sqref="D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10244,7 +10304,9 @@
       <c r="D164" s="211">
         <v>0.94489999999999996</v>
       </c>
-      <c r="E164" s="134"/>
+      <c r="E164" s="134">
+        <v>0.91810000000000003</v>
+      </c>
       <c r="F164" s="134">
         <v>0.91720000000000002</v>
       </c>
@@ -10338,7 +10400,9 @@
       <c r="D170" s="211">
         <v>0.50160000000000005</v>
       </c>
-      <c r="E170" s="2"/>
+      <c r="E170" s="2">
+        <v>0.48549999999999999</v>
+      </c>
       <c r="F170" s="134">
         <v>0.52149999999999996</v>
       </c>
@@ -10355,7 +10419,9 @@
       <c r="D171" s="211">
         <v>0.4703</v>
       </c>
-      <c r="E171" s="2"/>
+      <c r="E171" s="2">
+        <v>0.4204</v>
+      </c>
       <c r="F171" s="134">
         <v>0.47370000000000001</v>
       </c>
@@ -10372,7 +10438,9 @@
       <c r="D172" s="211">
         <v>0.4274</v>
       </c>
-      <c r="E172" s="2"/>
+      <c r="E172" s="2">
+        <v>0.36730000000000002</v>
+      </c>
       <c r="F172" s="134">
         <v>0.42499999999999999</v>
       </c>
@@ -10389,7 +10457,9 @@
       <c r="D173" s="211">
         <v>0.35680000000000001</v>
       </c>
-      <c r="E173" s="2"/>
+      <c r="E173" s="2">
+        <v>0.3034</v>
+      </c>
       <c r="F173" s="134">
         <v>0.36480000000000001</v>
       </c>
@@ -10497,274 +10567,278 @@
       <c r="H180" s="314"/>
     </row>
     <row r="181" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C181" s="266" t="s">
+      <c r="B181" s="322"/>
+      <c r="C181" s="323" t="s">
         <v>535</v>
       </c>
-      <c r="D181" s="266"/>
-      <c r="E181" s="266"/>
-      <c r="F181" s="266"/>
+      <c r="D181" s="323"/>
+      <c r="E181" s="323"/>
+      <c r="F181" s="323"/>
       <c r="G181" s="316"/>
       <c r="H181" s="314"/>
     </row>
     <row r="182" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B182" s="208"/>
-      <c r="C182" s="209" t="s">
+      <c r="B182" s="324"/>
+      <c r="C182" s="325" t="s">
         <v>528</v>
       </c>
-      <c r="D182" s="209" t="s">
+      <c r="D182" s="325" t="s">
         <v>529</v>
       </c>
-      <c r="E182" s="209" t="s">
+      <c r="E182" s="325" t="s">
         <v>536</v>
       </c>
-      <c r="F182" s="214" t="s">
+      <c r="F182" s="326" t="s">
         <v>538</v>
       </c>
       <c r="G182" s="316"/>
       <c r="H182" s="314"/>
     </row>
     <row r="183" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B183" s="209" t="s">
+      <c r="B183" s="325" t="s">
         <v>8</v>
       </c>
-      <c r="C183" s="134">
+      <c r="C183" s="327">
         <v>0.92649999999999999</v>
       </c>
-      <c r="D183" s="211">
+      <c r="D183" s="328">
         <v>0.92849999999999999</v>
       </c>
-      <c r="E183" s="134">
+      <c r="E183" s="327">
         <v>0.91810000000000003</v>
       </c>
-      <c r="F183" s="134">
+      <c r="F183" s="327">
         <v>0.91720000000000002</v>
       </c>
       <c r="G183" s="316"/>
       <c r="H183" s="314"/>
     </row>
     <row r="184" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B184" s="210" t="s">
+      <c r="B184" s="329" t="s">
         <v>530</v>
       </c>
-      <c r="C184" s="212">
+      <c r="C184" s="330">
         <v>0.71350000000000002</v>
       </c>
-      <c r="D184" s="2">
+      <c r="D184" s="331">
         <v>0.69769999999999999</v>
       </c>
-      <c r="E184" s="133"/>
-      <c r="F184" s="134">
+      <c r="E184" s="324"/>
+      <c r="F184" s="327">
         <v>0.67959999999999998</v>
       </c>
       <c r="G184" s="316"/>
       <c r="H184" s="314"/>
     </row>
     <row r="185" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B185" s="210" t="s">
+      <c r="B185" s="329" t="s">
         <v>531</v>
       </c>
-      <c r="C185" s="213">
+      <c r="C185" s="332">
         <v>0.84379999999999999</v>
       </c>
-      <c r="D185" s="212">
+      <c r="D185" s="330">
         <v>0.84519999999999995</v>
       </c>
-      <c r="E185" s="133"/>
-      <c r="F185" s="134">
+      <c r="E185" s="324"/>
+      <c r="F185" s="327">
         <v>0.81100000000000005</v>
       </c>
       <c r="G185" s="316"/>
       <c r="H185" s="314"/>
     </row>
     <row r="186" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B186" s="210" t="s">
+      <c r="B186" s="329" t="s">
         <v>532</v>
       </c>
-      <c r="C186" s="212">
+      <c r="C186" s="330">
         <v>0.88500000000000001</v>
       </c>
-      <c r="D186" s="2">
+      <c r="D186" s="331">
         <v>0.88180000000000003</v>
       </c>
-      <c r="E186" s="133"/>
-      <c r="F186" s="134">
+      <c r="E186" s="324"/>
+      <c r="F186" s="327">
         <v>0.878</v>
       </c>
       <c r="G186" s="316"/>
       <c r="H186" s="314"/>
     </row>
     <row r="187" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B187" s="209" t="s">
+      <c r="B187" s="325" t="s">
         <v>533</v>
       </c>
-      <c r="C187" s="212">
+      <c r="C187" s="330">
         <v>0.26769999999999999</v>
       </c>
-      <c r="D187" s="2">
+      <c r="D187" s="331">
         <v>0.19670000000000001</v>
       </c>
-      <c r="E187" s="133"/>
-      <c r="F187" s="134"/>
+      <c r="E187" s="324"/>
+      <c r="F187" s="327"/>
     </row>
     <row r="188" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B188" s="209" t="s">
+      <c r="B188" s="325" t="s">
         <v>534</v>
       </c>
-      <c r="C188" s="212">
+      <c r="C188" s="330">
         <v>0.47689999999999999</v>
       </c>
-      <c r="D188" s="2">
+      <c r="D188" s="331">
         <v>0.31030000000000002</v>
       </c>
-      <c r="E188" s="133"/>
-      <c r="F188" s="134"/>
+      <c r="E188" s="324"/>
+      <c r="F188" s="327"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B189" s="209" t="s">
+      <c r="B189" s="325" t="s">
         <v>47</v>
       </c>
-      <c r="C189" s="213">
+      <c r="C189" s="332">
         <v>0.4521</v>
       </c>
-      <c r="D189" s="212">
+      <c r="D189" s="330">
         <v>0.50349999999999995</v>
       </c>
-      <c r="E189" s="2">
+      <c r="E189" s="331">
         <v>0.48549999999999999</v>
       </c>
-      <c r="F189" s="134">
+      <c r="F189" s="327">
         <v>0.52149999999999996</v>
       </c>
     </row>
     <row r="190" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B190" s="209" t="s">
+      <c r="B190" s="325" t="s">
         <v>49</v>
       </c>
-      <c r="C190" s="2">
+      <c r="C190" s="331">
         <v>0.42209999999999998</v>
       </c>
-      <c r="D190" s="212">
+      <c r="D190" s="330">
         <v>0.45710000000000001</v>
       </c>
-      <c r="E190" s="2">
+      <c r="E190" s="331">
         <v>0.4204</v>
       </c>
-      <c r="F190" s="134">
+      <c r="F190" s="327">
         <v>0.47370000000000001</v>
       </c>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B191" s="209" t="s">
+      <c r="B191" s="325" t="s">
         <v>50</v>
       </c>
-      <c r="C191" s="2">
+      <c r="C191" s="331">
         <v>0.39529999999999998</v>
       </c>
-      <c r="D191" s="212">
+      <c r="D191" s="330">
         <v>0.41149999999999998</v>
       </c>
-      <c r="E191" s="2">
+      <c r="E191" s="331">
         <v>0.36730000000000002</v>
       </c>
-      <c r="F191" s="134">
+      <c r="F191" s="327">
         <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="192" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B192" s="209" t="s">
+      <c r="B192" s="325" t="s">
         <v>51</v>
       </c>
-      <c r="C192" s="2">
+      <c r="C192" s="331">
         <v>0.34429999999999999</v>
       </c>
-      <c r="D192" s="212">
+      <c r="D192" s="330">
         <v>0.34549999999999997</v>
       </c>
-      <c r="E192" s="2">
+      <c r="E192" s="331">
         <v>0.3034</v>
       </c>
-      <c r="F192" s="134">
+      <c r="F192" s="327">
         <v>0.36480000000000001</v>
       </c>
     </row>
     <row r="193" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B193" s="209" t="s">
+      <c r="B193" s="325" t="s">
         <v>52</v>
       </c>
-      <c r="C193" s="2">
+      <c r="C193" s="331">
         <v>0.32550000000000001</v>
       </c>
-      <c r="D193" s="212">
+      <c r="D193" s="330">
         <v>0.3498</v>
       </c>
-      <c r="E193" s="133"/>
-      <c r="F193" s="134">
+      <c r="E193" s="324"/>
+      <c r="F193" s="327">
         <v>0.39050000000000001</v>
       </c>
     </row>
     <row r="194" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B194" s="209" t="s">
+      <c r="B194" s="325" t="s">
         <v>53</v>
       </c>
-      <c r="C194" s="212">
+      <c r="C194" s="330">
         <v>0.129</v>
       </c>
-      <c r="D194" s="2">
+      <c r="D194" s="331">
         <v>9.5500000000000002E-2</v>
       </c>
-      <c r="E194" s="133"/>
-      <c r="F194" s="134">
+      <c r="E194" s="324"/>
+      <c r="F194" s="327">
         <v>0.12479999999999999</v>
       </c>
     </row>
     <row r="195" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B195" s="209" t="s">
+      <c r="B195" s="325" t="s">
         <v>59</v>
       </c>
-      <c r="C195" s="2">
+      <c r="C195" s="331">
         <v>0.45910000000000001</v>
       </c>
-      <c r="D195" s="212">
+      <c r="D195" s="330">
         <v>0.51249999999999996</v>
       </c>
-      <c r="E195" s="133"/>
-      <c r="F195" s="134">
+      <c r="E195" s="324"/>
+      <c r="F195" s="327">
         <v>0.5292</v>
       </c>
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B196" s="209" t="s">
+      <c r="B196" s="325" t="s">
         <v>62</v>
       </c>
-      <c r="C196" s="2">
+      <c r="C196" s="331">
         <v>0.443</v>
       </c>
-      <c r="D196" s="212">
+      <c r="D196" s="330">
         <v>0.49199999999999999</v>
       </c>
-      <c r="E196" s="133"/>
-      <c r="F196" s="134">
+      <c r="E196" s="324"/>
+      <c r="F196" s="327">
         <v>0.51029999999999998</v>
       </c>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B197" s="209" t="s">
+      <c r="B197" s="325" t="s">
         <v>65</v>
       </c>
-      <c r="C197" s="2">
+      <c r="C197" s="331">
         <v>0.40279999999999999</v>
       </c>
-      <c r="D197" s="212">
+      <c r="D197" s="330">
         <v>0.4279</v>
       </c>
-      <c r="E197" s="133"/>
-      <c r="F197" s="134">
+      <c r="E197" s="324"/>
+      <c r="F197" s="327">
         <v>0.46629999999999999</v>
       </c>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E198" s="171"/>
-      <c r="F198" s="27"/>
+      <c r="B198" s="322"/>
+      <c r="C198" s="322"/>
+      <c r="D198" s="322"/>
+      <c r="E198" s="333"/>
+      <c r="F198" s="334"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -10838,10 +10912,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}">
-  <dimension ref="A1:L207"/>
+  <dimension ref="A1:P207"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="C76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14470,7 +14544,7 @@
       <c r="K176" s="43"/>
       <c r="L176" s="44"/>
     </row>
-    <row r="177" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B177" s="230" t="s">
         <v>531</v>
       </c>
@@ -14493,7 +14567,7 @@
       <c r="K177" s="43"/>
       <c r="L177" s="44"/>
     </row>
-    <row r="178" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B178" s="230" t="s">
         <v>532</v>
       </c>
@@ -14516,7 +14590,7 @@
       <c r="K178" s="43"/>
       <c r="L178" s="44"/>
     </row>
-    <row r="179" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B179" s="229" t="s">
         <v>47</v>
       </c>
@@ -14543,7 +14617,7 @@
       <c r="K179" s="43"/>
       <c r="L179" s="44"/>
     </row>
-    <row r="180" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B180" s="229" t="s">
         <v>49</v>
       </c>
@@ -14570,7 +14644,7 @@
       <c r="K180" s="70"/>
       <c r="L180" s="44"/>
     </row>
-    <row r="181" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B181" s="229" t="s">
         <v>50</v>
       </c>
@@ -14597,7 +14671,7 @@
       <c r="K181" s="70"/>
       <c r="L181" s="44"/>
     </row>
-    <row r="182" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B182" s="229" t="s">
         <v>51</v>
       </c>
@@ -14624,7 +14698,7 @@
       <c r="K182" s="70"/>
       <c r="L182" s="44"/>
     </row>
-    <row r="183" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B183" s="229" t="s">
         <v>52</v>
       </c>
@@ -14651,7 +14725,7 @@
       <c r="K183" s="70"/>
       <c r="L183" s="44"/>
     </row>
-    <row r="184" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B184" s="229" t="s">
         <v>53</v>
       </c>
@@ -14678,7 +14752,7 @@
       <c r="K184" s="43"/>
       <c r="L184" s="44"/>
     </row>
-    <row r="185" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B185" s="229" t="s">
         <v>540</v>
       </c>
@@ -14705,7 +14779,7 @@
       <c r="K185" s="43"/>
       <c r="L185" s="44"/>
     </row>
-    <row r="186" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B186" s="229" t="s">
         <v>59</v>
       </c>
@@ -14732,7 +14806,7 @@
       <c r="K186" s="43"/>
       <c r="L186" s="44"/>
     </row>
-    <row r="187" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B187" s="229" t="s">
         <v>62</v>
       </c>
@@ -14759,7 +14833,7 @@
       <c r="K187" s="43"/>
       <c r="L187" s="44"/>
     </row>
-    <row r="188" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B188" s="231" t="s">
         <v>65</v>
       </c>
@@ -14786,8 +14860,8 @@
       <c r="K188" s="43"/>
       <c r="L188" s="44"/>
     </row>
-    <row r="190" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B191" s="286"/>
       <c r="C191" s="283" t="s">
         <v>535</v>
@@ -14796,7 +14870,7 @@
       <c r="E191" s="284"/>
       <c r="F191" s="285"/>
     </row>
-    <row r="192" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="287"/>
       <c r="C192" s="232" t="s">
         <v>528</v>
@@ -14810,8 +14884,16 @@
       <c r="F192" s="264" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="M192" s="335" t="s">
+        <v>565</v>
+      </c>
+      <c r="N192" s="335"/>
+      <c r="O192" s="335" t="s">
+        <v>8</v>
+      </c>
+      <c r="P192" s="335"/>
+    </row>
+    <row r="193" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B193" s="265" t="s">
         <v>8</v>
       </c>
@@ -14827,8 +14909,16 @@
       <c r="F193" s="260">
         <v>0.91720000000000002</v>
       </c>
-    </row>
-    <row r="194" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="M193" s="335"/>
+      <c r="N193" s="335"/>
+      <c r="O193" t="s">
+        <v>535</v>
+      </c>
+      <c r="P193" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="194" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B194" s="222" t="s">
         <v>530</v>
       </c>
@@ -14842,8 +14932,20 @@
       <c r="F194" s="134">
         <v>0.67959999999999998</v>
       </c>
-    </row>
-    <row r="195" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="M194" s="335" t="s">
+        <v>253</v>
+      </c>
+      <c r="N194" t="s">
+        <v>562</v>
+      </c>
+      <c r="O194">
+        <v>94.5</v>
+      </c>
+      <c r="P194">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="195" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B195" s="222" t="s">
         <v>531</v>
       </c>
@@ -14857,8 +14959,18 @@
       <c r="F195" s="134">
         <v>0.81100000000000005</v>
       </c>
-    </row>
-    <row r="196" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="M195" s="335"/>
+      <c r="N195" t="s">
+        <v>563</v>
+      </c>
+      <c r="O195">
+        <v>91.7</v>
+      </c>
+      <c r="P195" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="196" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B196" s="222" t="s">
         <v>532</v>
       </c>
@@ -14872,8 +14984,18 @@
       <c r="F196" s="134">
         <v>0.878</v>
       </c>
-    </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="M196" s="335"/>
+      <c r="N196" t="s">
+        <v>528</v>
+      </c>
+      <c r="O196">
+        <v>92.7</v>
+      </c>
+      <c r="P196">
+        <v>45.2</v>
+      </c>
+    </row>
+    <row r="197" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B197" s="223" t="s">
         <v>533</v>
       </c>
@@ -14885,8 +15007,20 @@
       </c>
       <c r="E197" s="133"/>
       <c r="F197" s="221"/>
-    </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="M197" s="335" t="s">
+        <v>252</v>
+      </c>
+      <c r="N197" t="s">
+        <v>562</v>
+      </c>
+      <c r="O197" t="s">
+        <v>564</v>
+      </c>
+      <c r="P197">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="198" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B198" s="223" t="s">
         <v>534</v>
       </c>
@@ -14898,8 +15032,18 @@
       </c>
       <c r="E198" s="133"/>
       <c r="F198" s="221"/>
-    </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="M198" s="335"/>
+      <c r="N198" t="s">
+        <v>563</v>
+      </c>
+      <c r="O198" t="s">
+        <v>564</v>
+      </c>
+      <c r="P198" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="199" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B199" s="223" t="s">
         <v>47</v>
       </c>
@@ -14915,8 +15059,18 @@
       <c r="F199" s="134">
         <v>0.52149999999999996</v>
       </c>
-    </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="M199" s="335"/>
+      <c r="N199" t="s">
+        <v>528</v>
+      </c>
+      <c r="O199" t="s">
+        <v>564</v>
+      </c>
+      <c r="P199">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="200" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B200" s="223" t="s">
         <v>49</v>
       </c>
@@ -14933,7 +15087,7 @@
         <v>0.47370000000000001</v>
       </c>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B201" s="223" t="s">
         <v>50</v>
       </c>
@@ -14950,7 +15104,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B202" s="223" t="s">
         <v>51</v>
       </c>
@@ -14967,7 +15121,7 @@
         <v>0.36480000000000001</v>
       </c>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B203" s="223" t="s">
         <v>52</v>
       </c>
@@ -14982,7 +15136,7 @@
         <v>0.39050000000000001</v>
       </c>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B204" s="223" t="s">
         <v>53</v>
       </c>
@@ -14997,7 +15151,7 @@
         <v>0.12479999999999999</v>
       </c>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B205" s="223" t="s">
         <v>59</v>
       </c>
@@ -15012,7 +15166,7 @@
         <v>0.5292</v>
       </c>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B206" s="223" t="s">
         <v>62</v>
       </c>
@@ -15027,7 +15181,7 @@
         <v>0.51029999999999998</v>
       </c>
     </row>
-    <row r="207" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B207" s="224" t="s">
         <v>65</v>
       </c>
@@ -15044,7 +15198,11 @@
     </row>
   </sheetData>
   <autoFilter ref="B3:I168" xr:uid="{2A4850F9-D7DB-6D40-89DE-4DEBEF4CA67F}"/>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="M194:M196"/>
+    <mergeCell ref="M197:M199"/>
+    <mergeCell ref="O192:P192"/>
+    <mergeCell ref="M192:N193"/>
     <mergeCell ref="B158:B168"/>
     <mergeCell ref="B4:B41"/>
     <mergeCell ref="B42:B45"/>
@@ -15092,8 +15250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B63F8CF-F012-4149-9CDA-3AB5262AB13A}">
   <dimension ref="A3:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="111" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>